<commit_message>
update etl for finance dim table.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7050" windowWidth="24240" windowHeight="5925" firstSheet="18" activeTab="23"/>
+    <workbookView xWindow="-90" yWindow="7110" windowWidth="24240" windowHeight="5865" firstSheet="18" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -4602,7 +4602,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5812,8 +5812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update finance etl for account_dim
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="242">
   <si>
     <t>Category</t>
   </si>
@@ -753,29 +753,19 @@
     <t xml:space="preserve">Fk for ledger </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Left join GLF_chart_acct with accnbri </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Question: some acounts will miss entity, debtor and costing,etc.)</t>
-    </r>
-  </si>
-  <si>
-    <t>GLF_LDG_acct_desc1: do we need to filter based on LGD_NAME?</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
     <t>terms_days</t>
+  </si>
+  <si>
+    <t>for debtor just limit to ARCHART</t>
+  </si>
+  <si>
+    <t>For Debtor just limit LDG_NAME='R1'</t>
+  </si>
+  <si>
+    <t>For debotr, cannot get consting information from this table.</t>
   </si>
 </sst>
 </file>
@@ -4589,7 +4579,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -5153,7 +5143,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -5298,7 +5288,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -5443,7 +5433,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -5813,7 +5803,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6003,7 +5993,7 @@
       <c r="G12" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="65" t="s">
         <v>233</v>
       </c>
       <c r="I12" s="38" t="s">
@@ -6012,7 +6002,9 @@
       <c r="J12" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="K12" s="38"/>
+      <c r="K12" s="65" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="13" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
@@ -6040,7 +6032,7 @@
         <v>149</v>
       </c>
       <c r="K13" s="65" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -6068,9 +6060,7 @@
       <c r="J14" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="K14" s="65" t="s">
-        <v>238</v>
-      </c>
+      <c r="K14" s="65"/>
     </row>
     <row r="15" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
@@ -6097,7 +6087,7 @@
       <c r="J15" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="K15" s="38"/>
+      <c r="K15" s="65"/>
     </row>
     <row r="16" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
@@ -6124,7 +6114,7 @@
       <c r="J16" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="65"/>
     </row>
     <row r="17" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
@@ -6151,7 +6141,9 @@
       <c r="J17" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="K17" s="38"/>
+      <c r="K17" s="65" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
@@ -6630,7 +6622,7 @@
         <v>151</v>
       </c>
       <c r="I35" s="65" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J35" s="38" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
update elts for finance_debtor_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7110" windowWidth="24240" windowHeight="5865" firstSheet="18" activeTab="23"/>
+    <workbookView xWindow="-90" yWindow="7110" windowWidth="24240" windowHeight="5865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="244">
   <si>
     <t>Category</t>
   </si>
@@ -669,12 +669,6 @@
     <t>abn</t>
   </si>
   <si>
-    <t>glf_ldg_acct_trans</t>
-  </si>
-  <si>
-    <t>join back to account_dim using this</t>
-  </si>
-  <si>
     <t>FK for cost centre</t>
   </si>
   <si>
@@ -766,6 +760,31 @@
   </si>
   <si>
     <t>For debotr, cannot get consting information from this table.</t>
+  </si>
+  <si>
+    <t>select distinct ldg_name from extract.GLF_LDG_ACCT_DESC1</t>
+  </si>
+  <si>
+    <t>glf_ldg_acc_trans</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">join back to account_dim using this
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ldg_name='R1'</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">full_date </t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1199,6 +1218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4579,7 +4599,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -4591,16 +4611,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="23" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="23" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="23"/>
     <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
@@ -4691,7 +4711,7 @@
         <v>24</v>
       </c>
       <c r="L8" s="62" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4713,7 +4733,7 @@
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>145</v>
       </c>
@@ -4729,15 +4749,15 @@
       <c r="G10" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H10" s="38" t="s">
-        <v>209</v>
+      <c r="H10" s="65" t="s">
+        <v>241</v>
       </c>
       <c r="I10" s="38" t="s">
         <v>194</v>
       </c>
       <c r="J10" s="38"/>
       <c r="K10" s="45" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -4745,7 +4765,7 @@
         <v>183</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>30</v>
@@ -4756,7 +4776,7 @@
       <c r="G11" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H11" s="38"/>
+      <c r="H11" s="65"/>
       <c r="I11" s="36"/>
       <c r="J11" s="38"/>
       <c r="K11" s="45"/>
@@ -4777,7 +4797,7 @@
       <c r="G12" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="65"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38"/>
       <c r="K12" s="38"/>
@@ -4798,7 +4818,7 @@
       <c r="G13" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H13" s="38"/>
+      <c r="H13" s="65"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38"/>
       <c r="K13" s="38"/>
@@ -4819,17 +4839,17 @@
       <c r="G14" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H14" s="38"/>
+      <c r="H14" s="65"/>
       <c r="I14" s="38"/>
       <c r="J14" s="38"/>
       <c r="K14" s="38"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>30</v>
@@ -4840,20 +4860,20 @@
       <c r="G15" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H15" s="38" t="s">
-        <v>209</v>
+      <c r="H15" s="65" t="s">
+        <v>241</v>
       </c>
       <c r="I15" s="38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J15" s="38"/>
       <c r="K15" s="38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>25</v>
@@ -4867,18 +4887,18 @@
       <c r="G16" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H16" s="38" t="s">
-        <v>209</v>
+      <c r="H16" s="65" t="s">
+        <v>241</v>
       </c>
       <c r="I16" s="38" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>25</v>
@@ -4892,16 +4912,16 @@
       <c r="G17" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H17" s="38" t="s">
-        <v>209</v>
+      <c r="H17" s="65" t="s">
+        <v>241</v>
       </c>
       <c r="I17" s="38" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J17" s="38"/>
       <c r="K17" s="36"/>
       <c r="L17" s="61" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -4909,7 +4929,7 @@
         <v>193</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C18" s="38" t="s">
         <v>30</v>
@@ -4918,7 +4938,7 @@
       <c r="E18" s="38"/>
       <c r="F18" s="38"/>
       <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="H18" s="65"/>
       <c r="I18" s="38"/>
       <c r="J18" s="38"/>
       <c r="K18" s="38"/>
@@ -4931,7 +4951,7 @@
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="H19" s="65"/>
       <c r="I19" s="38"/>
       <c r="J19" s="38"/>
       <c r="K19" s="38"/>
@@ -4944,7 +4964,7 @@
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="H20" s="65"/>
       <c r="I20" s="38"/>
       <c r="J20" s="38"/>
       <c r="K20" s="38"/>
@@ -4952,7 +4972,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="38" t="s">
@@ -4964,11 +4984,11 @@
       <c r="G21" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H21" s="38" t="s">
-        <v>209</v>
+      <c r="H21" s="65" t="s">
+        <v>241</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J21" s="38"/>
       <c r="K21" s="38"/>
@@ -4989,11 +5009,11 @@
       <c r="G22" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="38" t="s">
-        <v>209</v>
+      <c r="H22" s="65" t="s">
+        <v>241</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J22" s="38" t="s">
         <v>206</v>
@@ -5143,7 +5163,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -5288,7 +5308,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -5433,7 +5453,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -5446,7 +5466,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5631,7 +5651,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="22" t="s">
@@ -5800,10 +5820,13 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5994,7 +6017,7 @@
         <v>150</v>
       </c>
       <c r="H12" s="65" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I12" s="38" t="s">
         <v>200</v>
@@ -6003,7 +6026,7 @@
         <v>149</v>
       </c>
       <c r="K12" s="65" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -6023,7 +6046,7 @@
         <v>150</v>
       </c>
       <c r="H13" s="64" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I13" s="38" t="s">
         <v>201</v>
@@ -6032,7 +6055,7 @@
         <v>149</v>
       </c>
       <c r="K13" s="65" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -6052,7 +6075,7 @@
         <v>150</v>
       </c>
       <c r="H14" s="64" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I14" s="38" t="s">
         <v>202</v>
@@ -6079,7 +6102,7 @@
         <v>150</v>
       </c>
       <c r="H15" s="64" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I15" s="38" t="s">
         <v>203</v>
@@ -6106,7 +6129,7 @@
         <v>150</v>
       </c>
       <c r="H16" s="64" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I16" s="38" t="s">
         <v>204</v>
@@ -6142,7 +6165,7 @@
         <v>149</v>
       </c>
       <c r="K17" s="65" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -6435,7 +6458,7 @@
         <v>151</v>
       </c>
       <c r="I28" s="38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J28" s="38" t="s">
         <v>149</v>
@@ -6606,7 +6629,7 @@
     </row>
     <row r="35" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B35" s="38"/>
       <c r="C35" s="38" t="s">
@@ -6622,10 +6645,10 @@
         <v>151</v>
       </c>
       <c r="I35" s="65" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K35" s="38"/>
     </row>
@@ -6930,10 +6953,13 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7117,7 +7143,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B10" s="38"/>
       <c r="C10" s="38" t="s">
@@ -7132,7 +7158,9 @@
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
+      <c r="K10" s="65" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -7416,10 +7444,13 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7438,7 +7469,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -7472,7 +7503,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -7489,7 +7520,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -7585,7 +7616,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B9" s="38" t="s">
         <v>29</v>
@@ -7604,7 +7635,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B10" s="38"/>
       <c r="C10" s="38" t="s">
@@ -7621,7 +7652,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38" t="s">
@@ -7656,16 +7687,18 @@
       <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>217</v>
-      </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+      <c r="A13" s="66" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="65">
+        <v>11</v>
+      </c>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="36"/>
@@ -7673,11 +7706,15 @@
       <c r="K13" s="38"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
+      <c r="A14" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
@@ -7910,6 +7947,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10099,7 +10137,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update etl for debtor_fact to get org structure.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7110" windowWidth="24240" windowHeight="5865" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" firstSheet="21" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,100 @@
     <sheet name="Employee_DIM" sheetId="5" r:id="rId25"/>
     <sheet name="Ledger_DIM" sheetId="33" r:id="rId26"/>
     <sheet name="accounting_period_dim" sheetId="34" r:id="rId27"/>
+    <sheet name="program_mapping" sheetId="35" r:id="rId28"/>
+    <sheet name="data for program_mapping" sheetId="36" r:id="rId29"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jerry Shen</author>
+  </authors>
+  <commentList>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jerry Shen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Manual checking
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jerry Shen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HRIS org structure
+need to input manually
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jerry Shen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+will automaticlly get value from database/ don't inpurt key values here.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="306">
   <si>
     <t>Category</t>
   </si>
@@ -786,12 +873,198 @@
   <si>
     <t xml:space="preserve">full_date </t>
   </si>
+  <si>
+    <t>for ARCHART, using SELN_TYPE2_CODE to map org structure.</t>
+  </si>
+  <si>
+    <t>program_mapping_key</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>table3</t>
+  </si>
+  <si>
+    <t>name3</t>
+  </si>
+  <si>
+    <t>value3</t>
+  </si>
+  <si>
+    <t>table4</t>
+  </si>
+  <si>
+    <t>name4</t>
+  </si>
+  <si>
+    <t>value4</t>
+  </si>
+  <si>
+    <t>table5</t>
+  </si>
+  <si>
+    <t>name5</t>
+  </si>
+  <si>
+    <t>value5</t>
+  </si>
+  <si>
+    <t>mapping_type</t>
+  </si>
+  <si>
+    <t>program_name</t>
+  </si>
+  <si>
+    <t>PROGRAM_MAPPING</t>
+  </si>
+  <si>
+    <t>program mapping table</t>
+  </si>
+  <si>
+    <t>to map fiannce org structure to hris org structure</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>GLF_CHART_ACCT</t>
+  </si>
+  <si>
+    <t>SELN_TYPE2_CODE</t>
+  </si>
+  <si>
+    <t>ALLIEDH</t>
+  </si>
+  <si>
+    <t>BREAKAWA</t>
+  </si>
+  <si>
+    <t>BUSHIRE</t>
+  </si>
+  <si>
+    <t>CASEMAN</t>
+  </si>
+  <si>
+    <t>CHILDREN</t>
+  </si>
+  <si>
+    <t>CHSPE</t>
+  </si>
+  <si>
+    <t>CHSPN</t>
+  </si>
+  <si>
+    <t>CHSPS</t>
+  </si>
+  <si>
+    <t>CHSPW</t>
+  </si>
+  <si>
+    <t>CHSPY</t>
+  </si>
+  <si>
+    <t>COUNSEL</t>
+  </si>
+  <si>
+    <t>DISABILI</t>
+  </si>
+  <si>
+    <t>DSCC</t>
+  </si>
+  <si>
+    <t>DSDA</t>
+  </si>
+  <si>
+    <t>DSIS</t>
+  </si>
+  <si>
+    <t>DSOATS</t>
+  </si>
+  <si>
+    <t>DSOR</t>
+  </si>
+  <si>
+    <t>ELIZABAT</t>
+  </si>
+  <si>
+    <t>ELIZABET</t>
+  </si>
+  <si>
+    <t>EXCEPTIO</t>
+  </si>
+  <si>
+    <t>FFS</t>
+  </si>
+  <si>
+    <t>GOVERNME</t>
+  </si>
+  <si>
+    <t>HCPEAST</t>
+  </si>
+  <si>
+    <t>HCPNORTH</t>
+  </si>
+  <si>
+    <t>HCPSOUTH</t>
+  </si>
+  <si>
+    <t>HCPWEST</t>
+  </si>
+  <si>
+    <t>HCPYLNB</t>
+  </si>
+  <si>
+    <t>PLATFORM</t>
+  </si>
+  <si>
+    <t>RECHARGE</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>WESTWORK</t>
+  </si>
+  <si>
+    <t>Allied Health</t>
+  </si>
+  <si>
+    <t>Home Care North &amp; East</t>
+  </si>
+  <si>
+    <t>Home Care South &amp; West</t>
+  </si>
+  <si>
+    <t>Children's Disability Services</t>
+  </si>
+  <si>
+    <t>see tab: data for program_mapping</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -855,8 +1128,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -873,6 +1166,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -1111,7 +1410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1219,6 +1518,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4611,8 +4925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4842,7 +5156,9 @@
       <c r="H14" s="65"/>
       <c r="I14" s="38"/>
       <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
+      <c r="K14" s="65" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
@@ -5324,7 +5640,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A8" sqref="A8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5466,7 +5782,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5825,8 +6141,8 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7948,6 +8264,1670 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="39.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="23" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="38">
+        <v>30</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="38">
+        <v>100</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="38">
+        <v>100</v>
+      </c>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="38">
+        <v>100</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="38">
+        <v>100</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="38">
+        <v>100</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="38">
+        <v>100</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="38">
+        <v>100</v>
+      </c>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="38">
+        <v>100</v>
+      </c>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="38">
+        <v>100</v>
+      </c>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="38">
+        <v>100</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="38">
+        <v>100</v>
+      </c>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="38">
+        <v>100</v>
+      </c>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="38">
+        <v>100</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="38">
+        <v>100</v>
+      </c>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="38">
+        <v>100</v>
+      </c>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="38">
+        <v>20</v>
+      </c>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="38">
+        <v>50</v>
+      </c>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:T32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="14"/>
+    <col min="19" max="19" width="27.42578125" style="14" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="R1" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="S1" s="68" t="s">
+        <v>263</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="67">
+        <v>317</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="67" t="s">
+        <v>270</v>
+      </c>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="71" t="s">
+        <v>301</v>
+      </c>
+      <c r="T2" s="72"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="67">
+        <v>318</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D3" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E3" s="67" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="71"/>
+      <c r="T3" s="72"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="67">
+        <v>319</v>
+      </c>
+      <c r="B4" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E4" s="67" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" s="71"/>
+      <c r="T4" s="72"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="67">
+        <v>320</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D5" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S5" s="71"/>
+      <c r="T5" s="72"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="67">
+        <v>321</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="71"/>
+      <c r="T6" s="72"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="67">
+        <v>322</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>275</v>
+      </c>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S7" s="71" t="s">
+        <v>302</v>
+      </c>
+      <c r="T7" s="72"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="67">
+        <v>323</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E8" s="67" t="s">
+        <v>276</v>
+      </c>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S8" s="71" t="s">
+        <v>302</v>
+      </c>
+      <c r="T8" s="72"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="67">
+        <v>324</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="67" t="s">
+        <v>277</v>
+      </c>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="67"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S9" s="71" t="s">
+        <v>303</v>
+      </c>
+      <c r="T9" s="72"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="67">
+        <v>325</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E10" s="67" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="67"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10" s="71" t="s">
+        <v>303</v>
+      </c>
+      <c r="T10" s="72"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="67">
+        <v>326</v>
+      </c>
+      <c r="B11" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E11" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S11" s="71" t="s">
+        <v>303</v>
+      </c>
+      <c r="T11" s="72"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="67">
+        <v>327</v>
+      </c>
+      <c r="B12" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E12" s="67" t="s">
+        <v>280</v>
+      </c>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S12" s="71"/>
+      <c r="T12" s="72"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="67">
+        <v>328</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>281</v>
+      </c>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S13" s="71" t="s">
+        <v>304</v>
+      </c>
+      <c r="T13" s="72"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="67">
+        <v>329</v>
+      </c>
+      <c r="B14" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>282</v>
+      </c>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S14" s="71" t="s">
+        <v>304</v>
+      </c>
+      <c r="T14" s="72"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="67">
+        <v>330</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E15" s="67" t="s">
+        <v>283</v>
+      </c>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="67"/>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S15" s="71" t="s">
+        <v>304</v>
+      </c>
+      <c r="T15" s="72"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="67">
+        <v>331</v>
+      </c>
+      <c r="B16" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E16" s="67" t="s">
+        <v>284</v>
+      </c>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" s="71" t="s">
+        <v>304</v>
+      </c>
+      <c r="T16" s="72"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="67">
+        <v>332</v>
+      </c>
+      <c r="B17" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D17" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E17" s="67" t="s">
+        <v>285</v>
+      </c>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="67"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" s="71" t="s">
+        <v>304</v>
+      </c>
+      <c r="T17" s="72"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="67">
+        <v>333</v>
+      </c>
+      <c r="B18" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D18" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" s="67" t="s">
+        <v>286</v>
+      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="67"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S18" s="71" t="s">
+        <v>304</v>
+      </c>
+      <c r="T18" s="72"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="67">
+        <v>334</v>
+      </c>
+      <c r="B19" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D19" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E19" s="67" t="s">
+        <v>287</v>
+      </c>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S19" s="71"/>
+      <c r="T19" s="72"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="67">
+        <v>335</v>
+      </c>
+      <c r="B20" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D20" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" s="67" t="s">
+        <v>288</v>
+      </c>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S20" s="71"/>
+      <c r="T20" s="72"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="67">
+        <v>336</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E21" s="67" t="s">
+        <v>289</v>
+      </c>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S21" s="71"/>
+      <c r="T21" s="72"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="67">
+        <v>337</v>
+      </c>
+      <c r="B22" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C22" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E22" s="67" t="s">
+        <v>290</v>
+      </c>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S22" s="71"/>
+      <c r="T22" s="72"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="67">
+        <v>338</v>
+      </c>
+      <c r="B23" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C23" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D23" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E23" s="67" t="s">
+        <v>291</v>
+      </c>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S23" s="71"/>
+      <c r="T23" s="72"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="67">
+        <v>339</v>
+      </c>
+      <c r="B24" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C24" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D24" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E24" s="67" t="s">
+        <v>292</v>
+      </c>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="67"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S24" s="71" t="s">
+        <v>302</v>
+      </c>
+      <c r="T24" s="72"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="67">
+        <v>340</v>
+      </c>
+      <c r="B25" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C25" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D25" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>293</v>
+      </c>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S25" s="71" t="s">
+        <v>302</v>
+      </c>
+      <c r="T25" s="72"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="67">
+        <v>341</v>
+      </c>
+      <c r="B26" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C26" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D26" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>294</v>
+      </c>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="67"/>
+      <c r="P26" s="67"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S26" s="71" t="s">
+        <v>303</v>
+      </c>
+      <c r="T26" s="72"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="67">
+        <v>342</v>
+      </c>
+      <c r="B27" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C27" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E27" s="67" t="s">
+        <v>295</v>
+      </c>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="67"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="67"/>
+      <c r="R27" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S27" s="71" t="s">
+        <v>303</v>
+      </c>
+      <c r="T27" s="72"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="67">
+        <v>343</v>
+      </c>
+      <c r="B28" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C28" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D28" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E28" s="67" t="s">
+        <v>296</v>
+      </c>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
+      <c r="O28" s="67"/>
+      <c r="P28" s="67"/>
+      <c r="Q28" s="67"/>
+      <c r="R28" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S28" s="71" t="s">
+        <v>302</v>
+      </c>
+      <c r="T28" s="72"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="67">
+        <v>344</v>
+      </c>
+      <c r="B29" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C29" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D29" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>297</v>
+      </c>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="67"/>
+      <c r="N29" s="67"/>
+      <c r="O29" s="67"/>
+      <c r="P29" s="67"/>
+      <c r="Q29" s="67"/>
+      <c r="R29" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S29" s="71"/>
+      <c r="T29" s="72"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="67">
+        <v>345</v>
+      </c>
+      <c r="B30" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C30" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D30" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E30" s="67" t="s">
+        <v>298</v>
+      </c>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="67"/>
+      <c r="P30" s="67"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S30" s="71"/>
+      <c r="T30" s="72"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="67">
+        <v>346</v>
+      </c>
+      <c r="B31" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C31" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D31" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E31" s="67" t="s">
+        <v>299</v>
+      </c>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S31" s="71"/>
+      <c r="T31" s="72"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="67">
+        <v>347</v>
+      </c>
+      <c r="B32" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C32" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D32" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E32" s="67" t="s">
+        <v>300</v>
+      </c>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="67"/>
+      <c r="P32" s="67"/>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="S32" s="71"/>
+      <c r="T32" s="72"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update matrxi for finance.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" firstSheet="21" activeTab="28"/>
+    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" firstSheet="21" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -8274,7 +8274,7 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -8761,12 +8761,13 @@
   </sheetPr>
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
@@ -9185,7 +9186,7 @@
         <v>3</v>
       </c>
       <c r="S11" s="71" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T11" s="72"/>
     </row>

</xml_diff>

<commit_message>
[finance].[debtor_fact] table changed as request.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -1152,7 +1152,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1175,12 +1175,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1419,7 +1413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1548,15 +1542,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4951,7 +4936,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5374,114 +5359,114 @@
       <c r="L22" s="21"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="75" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77" t="s">
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="77" t="s">
+      <c r="H23" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="I23" s="77" t="s">
+      <c r="I23" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="J23" s="77" t="s">
+      <c r="J23" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="75" t="s">
+      <c r="B24" s="19"/>
+      <c r="C24" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="76">
+      <c r="D24" s="19">
         <v>40</v>
       </c>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77" t="s">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="H24" s="77" t="s">
+      <c r="H24" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="I24" s="77" t="s">
+      <c r="I24" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="J24" s="77" t="s">
+      <c r="J24" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="75" t="s">
+      <c r="A25" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="B25" s="76"/>
-      <c r="C25" s="75" t="s">
+      <c r="B25" s="19"/>
+      <c r="C25" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="76">
+      <c r="D25" s="19">
         <v>40</v>
       </c>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77" t="s">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="H25" s="77" t="s">
+      <c r="H25" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="I25" s="77" t="s">
+      <c r="I25" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="J25" s="77" t="s">
+      <c r="J25" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="75" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="76">
+      <c r="D26" s="19">
         <v>40</v>
       </c>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77" t="s">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="H26" s="77" t="s">
+      <c r="H26" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="I26" s="77" t="s">
+      <c r="I26" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="J26" s="77" t="s">
+      <c r="J26" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update matrix_bus for finance.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" firstSheet="21" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="326">
   <si>
     <t>Category</t>
   </si>
@@ -1061,6 +1061,51 @@
   </si>
   <si>
     <t>due_datei</t>
+  </si>
+  <si>
+    <t>LDG_NAME</t>
+  </si>
+  <si>
+    <t>EDACCNBR</t>
+  </si>
+  <si>
+    <t>DESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP1</t>
+  </si>
+  <si>
+    <t>ACC_COMP2</t>
+  </si>
+  <si>
+    <t>ACC_COMP3</t>
+  </si>
+  <si>
+    <t>ACC_COMP11</t>
+  </si>
+  <si>
+    <t>ACC_COMP1_SCESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP2_SCESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP3_SCESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP11_SCESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP4</t>
+  </si>
+  <si>
+    <t>ACC_COMP4_SCESCR</t>
+  </si>
+  <si>
+    <t>ldg_name LIKE '%ACT'</t>
+  </si>
+  <si>
+    <t>GLF_LDG_ACCT_DESC1</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1542,6 +1587,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4935,7 +4983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
@@ -5911,18 +5959,19 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.5703125" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="66.5703125" customWidth="1"/>
@@ -6098,171 +6147,521 @@
       <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="22" t="s">
+      <c r="A10" s="64" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="63">
+        <v>8</v>
+      </c>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>311</v>
+      </c>
+      <c r="J10" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="75" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="63"/>
+      <c r="C11" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="63">
+        <v>32</v>
+      </c>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I11" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="75"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="64" t="s">
+        <v>312</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="63">
+        <v>32</v>
+      </c>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H12" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I12" s="64" t="s">
+        <v>312</v>
+      </c>
+      <c r="J12" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="63"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="64" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="63">
+        <v>15</v>
+      </c>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>155</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="63"/>
+    </row>
+    <row r="14" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="64" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="63">
+        <v>192</v>
+      </c>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H14" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I14" s="64" t="s">
+        <v>313</v>
+      </c>
+      <c r="J14" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="63"/>
+    </row>
+    <row r="15" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="64" t="s">
+        <v>314</v>
+      </c>
+      <c r="B15" s="63"/>
+      <c r="C15" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="63">
+        <v>32</v>
+      </c>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I15" s="64" t="s">
+        <v>314</v>
+      </c>
+      <c r="J15" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="63"/>
+    </row>
+    <row r="16" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="63">
+        <v>15</v>
+      </c>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H16" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I16" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="J16" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="63"/>
+    </row>
+    <row r="17" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="64" t="s">
+        <v>315</v>
+      </c>
+      <c r="B17" s="63"/>
+      <c r="C17" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="63">
+        <v>32</v>
+      </c>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I17" s="64" t="s">
+        <v>315</v>
+      </c>
+      <c r="J17" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="63"/>
+    </row>
+    <row r="18" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="64" t="s">
+        <v>319</v>
+      </c>
+      <c r="B18" s="63"/>
+      <c r="C18" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="63">
+        <v>15</v>
+      </c>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I18" s="64" t="s">
+        <v>319</v>
+      </c>
+      <c r="J18" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="63"/>
+    </row>
+    <row r="19" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="64" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="63">
+        <v>32</v>
+      </c>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H19" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I19" s="64" t="s">
+        <v>316</v>
+      </c>
+      <c r="J19" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="63"/>
+    </row>
+    <row r="20" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="64" t="s">
+        <v>320</v>
+      </c>
+      <c r="B20" s="63"/>
+      <c r="C20" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="63">
+        <v>15</v>
+      </c>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I20" s="64" t="s">
+        <v>320</v>
+      </c>
+      <c r="J20" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="63"/>
+    </row>
+    <row r="21" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="64" t="s">
+        <v>322</v>
+      </c>
+      <c r="B21" s="63"/>
+      <c r="C21" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="63">
+        <v>32</v>
+      </c>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H21" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>322</v>
+      </c>
+      <c r="J21" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="63"/>
+    </row>
+    <row r="22" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
+        <v>323</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="63">
+        <v>15</v>
+      </c>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H22" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I22" s="64" t="s">
+        <v>323</v>
+      </c>
+      <c r="J22" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" s="63"/>
+    </row>
+    <row r="23" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="64" t="s">
+        <v>317</v>
+      </c>
+      <c r="B23" s="63"/>
+      <c r="C23" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="63">
+        <v>32</v>
+      </c>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H23" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I23" s="64" t="s">
+        <v>317</v>
+      </c>
+      <c r="J23" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" s="63"/>
+    </row>
+    <row r="24" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="64" t="s">
+        <v>321</v>
+      </c>
+      <c r="B24" s="63"/>
+      <c r="C24" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="63">
+        <v>15</v>
+      </c>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="I24" s="64" t="s">
+        <v>321</v>
+      </c>
+      <c r="J24" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="K24" s="63"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="18">
+        <v>5</v>
+      </c>
+      <c r="E25" s="44"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="18">
         <v>50</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="34"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="34"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18" t="s">
+      <c r="E26" s="44"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="18">
-        <v>5</v>
-      </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="18">
-        <v>50</v>
-      </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="18">
+      <c r="D29" s="18">
         <v>1</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E29" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6274,7 +6673,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cost Centre Dim table updated.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" firstSheet="21" activeTab="22"/>
+    <workbookView xWindow="-90" yWindow="7230" windowWidth="24240" windowHeight="5745" firstSheet="21" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -1458,7 +1458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1587,9 +1587,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1892,6 +1889,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2802,6 +2800,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3028,6 +3027,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3254,6 +3254,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3480,6 +3481,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3706,6 +3708,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3932,6 +3935,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4158,6 +4162,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4384,6 +4389,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4610,6 +4616,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4836,7 +4843,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet19">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K13"/>
@@ -4981,6 +4988,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5524,7 +5532,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet20">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K14"/>
@@ -5669,7 +5677,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet21">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K12"/>
@@ -5814,7 +5822,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet22">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K11"/>
@@ -5959,10 +5967,11 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6147,411 +6156,411 @@
       <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="64" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="20">
         <v>8</v>
       </c>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63" t="s">
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H10" s="63" t="s">
+      <c r="H10" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I10" s="64" t="s">
+      <c r="I10" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="J10" s="64" t="s">
+      <c r="J10" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="75" t="s">
+      <c r="K10" s="33" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="64" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="20">
         <v>32</v>
       </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63" t="s">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H11" s="63" t="s">
+      <c r="H11" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="75"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="64" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="20">
         <v>32</v>
       </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H12" s="63" t="s">
+      <c r="H12" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I12" s="64" t="s">
+      <c r="I12" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="J12" s="64" t="s">
+      <c r="J12" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="63"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="63">
+      <c r="D13" s="20">
         <v>15</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H13" s="63" t="s">
+      <c r="H13" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I13" s="64" t="s">
+      <c r="I13" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="J13" s="64" t="s">
+      <c r="J13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="63"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="64" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="20">
         <v>192</v>
       </c>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63" t="s">
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H14" s="63" t="s">
+      <c r="H14" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I14" s="64" t="s">
+      <c r="I14" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="J14" s="64" t="s">
+      <c r="J14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="63"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="20">
         <v>32</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63" t="s">
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H15" s="63" t="s">
+      <c r="H15" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I15" s="64" t="s">
+      <c r="I15" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="J15" s="64" t="s">
+      <c r="J15" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K15" s="63"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="20"/>
+      <c r="C16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="63">
+      <c r="D16" s="20">
         <v>15</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63" t="s">
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H16" s="63" t="s">
+      <c r="H16" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I16" s="64" t="s">
+      <c r="I16" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="J16" s="64" t="s">
+      <c r="J16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="63"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="20">
         <v>32</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63" t="s">
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H17" s="63" t="s">
+      <c r="H17" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I17" s="64" t="s">
+      <c r="I17" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="J17" s="64" t="s">
+      <c r="J17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="63"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="20">
         <v>15</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63" t="s">
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H18" s="63" t="s">
+      <c r="H18" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I18" s="64" t="s">
+      <c r="I18" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="J18" s="64" t="s">
+      <c r="J18" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="63"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="64" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="63">
+      <c r="D19" s="20">
         <v>32</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H19" s="63" t="s">
+      <c r="H19" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I19" s="64" t="s">
+      <c r="I19" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="J19" s="64" t="s">
+      <c r="J19" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="63"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="63">
+      <c r="D20" s="20">
         <v>15</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H20" s="63" t="s">
+      <c r="H20" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I20" s="64" t="s">
+      <c r="I20" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="J20" s="64" t="s">
+      <c r="J20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="63"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="63">
+      <c r="D21" s="20">
         <v>32</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63" t="s">
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H21" s="63" t="s">
+      <c r="H21" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I21" s="64" t="s">
+      <c r="I21" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="J21" s="64" t="s">
+      <c r="J21" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="63"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="20"/>
+      <c r="C22" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="63">
+      <c r="D22" s="20">
         <v>15</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63" t="s">
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="63" t="s">
+      <c r="H22" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I22" s="64" t="s">
+      <c r="I22" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="J22" s="64" t="s">
+      <c r="J22" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="63"/>
+      <c r="K22" s="20"/>
     </row>
     <row r="23" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="64" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="63">
+      <c r="D23" s="20">
         <v>32</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63" t="s">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="63" t="s">
+      <c r="H23" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I23" s="64" t="s">
+      <c r="I23" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="J23" s="64" t="s">
+      <c r="J23" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="63"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="64" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="63">
+      <c r="D24" s="20">
         <v>15</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63" t="s">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H24" s="63" t="s">
+      <c r="H24" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="I24" s="64" t="s">
+      <c r="I24" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="J24" s="64" t="s">
+      <c r="J24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="63"/>
+      <c r="K24" s="20"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
@@ -6667,7 +6676,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet24">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K41"/>
@@ -7613,7 +7622,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet25">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K10"/>
@@ -7800,7 +7809,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet26">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K29"/>
@@ -8291,7 +8300,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet27">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K29"/>
@@ -8800,7 +8809,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet28">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:K28"/>
@@ -9287,7 +9296,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet29">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:T32"/>
@@ -10465,7 +10474,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L55"/>
@@ -11194,7 +11203,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L55"/>
@@ -11920,7 +11929,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L55"/>
@@ -12646,6 +12655,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12936,6 +12946,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13162,6 +13173,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13388,6 +13400,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
update etl for debtor_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" firstSheet="21" activeTab="22"/>
+    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" firstSheet="17" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="332">
   <si>
     <t>Category</t>
   </si>
@@ -1106,6 +1106,24 @@
   </si>
   <si>
     <t>GLF_LDG_ACCT_DESC1</t>
+  </si>
+  <si>
+    <t>ACC_COMP1_SDESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP2_SDESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP3_SDESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP4_SDESCR</t>
+  </si>
+  <si>
+    <t>ACC_COMP11_SDESCR</t>
+  </si>
+  <si>
+    <t>join back to extract.glf_ldg_acc_trans using doc_ref1. and cost_centre_dim</t>
   </si>
 </sst>
 </file>
@@ -1458,7 +1476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1590,6 +1608,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4984,7 +5005,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5134,7 +5155,7 @@
       </c>
       <c r="L10" s="21"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="70" t="s">
         <v>183</v>
       </c>
@@ -5153,7 +5174,9 @@
       <c r="H11" s="21"/>
       <c r="I11" s="70"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="74"/>
+      <c r="K11" s="76" t="s">
+        <v>331</v>
+      </c>
       <c r="L11" s="21"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -5959,10 +5982,13 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5972,7 +5998,7 @@
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="66.5703125" customWidth="1"/>
   </cols>
@@ -6330,7 +6356,7 @@
         <v>325</v>
       </c>
       <c r="I16" s="64" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="J16" s="64" t="s">
         <v>31</v>
@@ -6384,7 +6410,7 @@
         <v>325</v>
       </c>
       <c r="I18" s="64" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="J18" s="64" t="s">
         <v>31</v>
@@ -6438,7 +6464,7 @@
         <v>325</v>
       </c>
       <c r="I20" s="64" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="J20" s="64" t="s">
         <v>31</v>
@@ -6492,7 +6518,7 @@
         <v>325</v>
       </c>
       <c r="I22" s="64" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J22" s="64" t="s">
         <v>31</v>
@@ -6546,7 +6572,7 @@
         <v>325</v>
       </c>
       <c r="I24" s="64" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="J24" s="64" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
change etl for debtor_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" firstSheet="17" activeTab="22"/>
+    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="333">
   <si>
     <t>Category</t>
   </si>
@@ -1124,6 +1124,9 @@
   </si>
   <si>
     <t>join back to extract.glf_ldg_acc_trans using doc_ref1. and cost_centre_dim</t>
+  </si>
+  <si>
+    <t>doc_type</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1611,6 +1614,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5002,10 +5011,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5430,114 +5439,142 @@
       <c r="L22" s="21"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="77" t="s">
         <v>310</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="77"/>
+      <c r="C23" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19" t="s">
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="77" t="s">
         <v>241</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="77" t="s">
         <v>310</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="77" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="19"/>
       <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="77" t="s">
         <v>305</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="77"/>
+      <c r="C24" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="77">
         <v>40</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19" t="s">
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="77" t="s">
         <v>241</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="77" t="s">
         <v>305</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="77" t="s">
         <v>306</v>
       </c>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="77" t="s">
         <v>307</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19" t="s">
+      <c r="B25" s="77"/>
+      <c r="C25" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="77">
         <v>40</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19" t="s">
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="77" t="s">
         <v>241</v>
       </c>
-      <c r="I25" s="19" t="s">
+      <c r="I25" s="77" t="s">
         <v>305</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="77" t="s">
         <v>306</v>
       </c>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="77" t="s">
         <v>308</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19" t="s">
+      <c r="B26" s="77"/>
+      <c r="C26" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="77">
         <v>40</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19" t="s">
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="H26" s="19" t="s">
+      <c r="H26" s="77" t="s">
         <v>241</v>
       </c>
-      <c r="I26" s="19" t="s">
+      <c r="I26" s="77" t="s">
         <v>305</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="77" t="s">
         <v>306</v>
       </c>
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="78" t="s">
+        <v>332</v>
+      </c>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="78">
+        <v>10</v>
+      </c>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77" t="s">
+        <v>150</v>
+      </c>
+      <c r="H27" s="77" t="s">
+        <v>241</v>
+      </c>
+      <c r="I27" s="78" t="s">
+        <v>332</v>
+      </c>
+      <c r="J27" s="77">
+        <v>10</v>
+      </c>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5987,7 +6024,7 @@
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change debtor_fact etl to add overdue_days.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="334">
   <si>
     <t>Category</t>
   </si>
@@ -1127,6 +1127,9 @@
   </si>
   <si>
     <t>doc_type</t>
+  </si>
+  <si>
+    <t>overdue_days</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1475,11 +1478,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1619,6 +1633,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5011,10 +5028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:J27"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5575,6 +5592,14 @@
       </c>
       <c r="K27" s="65"/>
       <c r="L27" s="65"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="C28" s="79" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update two extra columns to debtor_fact table.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="338">
   <si>
     <t>Category</t>
   </si>
@@ -1136,6 +1136,15 @@
   when DUE_DATEI &lt;&gt; '1900-01-01 00:00:00.000'  then   Datediff(day,t1.due_datei,getdate())
   else 0
   end</t>
+  </si>
+  <si>
+    <t>alloc_amt1</t>
+  </si>
+  <si>
+    <t>outstanding_amt</t>
+  </si>
+  <si>
+    <t>alloc_amt 1- amount when doc_type ='ARINV'</t>
   </si>
 </sst>
 </file>
@@ -5020,10 +5029,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5604,6 +5613,56 @@
       <c r="L28" s="78" t="s">
         <v>334</v>
       </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="78" t="s">
+        <v>335</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="78" t="s">
+        <v>206</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="77" t="s">
+        <v>150</v>
+      </c>
+      <c r="H29" s="77" t="s">
+        <v>241</v>
+      </c>
+      <c r="I29" s="78" t="s">
+        <v>335</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="K29" s="38"/>
+      <c r="L29" s="78" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="78" t="s">
+        <v>336</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="78" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update matrix bus for finance.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7170" windowWidth="24240" windowHeight="5805" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="7230" windowWidth="24240" windowHeight="5745" firstSheet="21" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="385">
   <si>
     <t>Category</t>
   </si>
@@ -1145,6 +1145,147 @@
   </si>
   <si>
     <t>alloc_amt 1- amount when doc_type ='ARINV'</t>
+  </si>
+  <si>
+    <t>No Program</t>
+  </si>
+  <si>
+    <t>All Hallows</t>
+  </si>
+  <si>
+    <t>Autism Services</t>
+  </si>
+  <si>
+    <t>Better Places Stronger Communities</t>
+  </si>
+  <si>
+    <t>Canterbury Close</t>
+  </si>
+  <si>
+    <t>Central Foster Care Support</t>
+  </si>
+  <si>
+    <t>ComCare Project</t>
+  </si>
+  <si>
+    <t>Communities for Children</t>
+  </si>
+  <si>
+    <t>Communities for Children Plus</t>
+  </si>
+  <si>
+    <t>Community Financial Services</t>
+  </si>
+  <si>
+    <t>Daphne Street Child Care Centre</t>
+  </si>
+  <si>
+    <t>Disability Support</t>
+  </si>
+  <si>
+    <t>Dutton Court</t>
+  </si>
+  <si>
+    <t>Emergency Assistance &amp; Community Support</t>
+  </si>
+  <si>
+    <t>Enterprise Architecture</t>
+  </si>
+  <si>
+    <t>Exceptional Needs</t>
+  </si>
+  <si>
+    <t>Family Preservation &amp; Reunification Service</t>
+  </si>
+  <si>
+    <t>Family Relationships</t>
+  </si>
+  <si>
+    <t>Family Support</t>
+  </si>
+  <si>
+    <t>Finance - Active Living</t>
+  </si>
+  <si>
+    <t>Finance - Community</t>
+  </si>
+  <si>
+    <t>Finance - Corporate Services</t>
+  </si>
+  <si>
+    <t>Finance - Housing</t>
+  </si>
+  <si>
+    <t>Grandview Court</t>
+  </si>
+  <si>
+    <t>Housing Inclusion</t>
+  </si>
+  <si>
+    <t>Housing Operations</t>
+  </si>
+  <si>
+    <t>Housing Services</t>
+  </si>
+  <si>
+    <t>HRIS Project</t>
+  </si>
+  <si>
+    <t>Ian George Court</t>
+  </si>
+  <si>
+    <t>IT Projects</t>
+  </si>
+  <si>
+    <t>Loss &amp; Grief</t>
+  </si>
+  <si>
+    <t>Northern Foster Carer Support</t>
+  </si>
+  <si>
+    <t>Personal Helpers &amp; Mentors (PHaMs)</t>
+  </si>
+  <si>
+    <t>Practice Development Unit</t>
+  </si>
+  <si>
+    <t>Property &amp; Facilities</t>
+  </si>
+  <si>
+    <t>Service Delivery</t>
+  </si>
+  <si>
+    <t>Settlement Services</t>
+  </si>
+  <si>
+    <t>Southern Foster Carer Support</t>
+  </si>
+  <si>
+    <t>Specialist Care Programs</t>
+  </si>
+  <si>
+    <t>SRF Under 65 &amp; Mental Health Respite</t>
+  </si>
+  <si>
+    <t>St Laurence's Court</t>
+  </si>
+  <si>
+    <t>Tenancy Services</t>
+  </si>
+  <si>
+    <t>The Arches</t>
+  </si>
+  <si>
+    <t>Wanslea Child Care Centre</t>
+  </si>
+  <si>
+    <t>Youth Services</t>
+  </si>
+  <si>
+    <t>Multicultural Services</t>
+  </si>
+  <si>
+    <t>DWH - program_name</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1377,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1259,6 +1400,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1497,7 +1644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1637,6 +1784,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5031,7 +5183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -9441,10 +9593,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9456,9 +9608,10 @@
     <col min="18" max="18" width="9.140625" style="14"/>
     <col min="19" max="19" width="27.42578125" style="14" customWidth="1"/>
     <col min="20" max="20" width="15.42578125" style="71" customWidth="1"/>
+    <col min="22" max="22" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>244</v>
       </c>
@@ -9510,7 +9663,7 @@
       <c r="Q1" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="80" t="s">
         <v>261</v>
       </c>
       <c r="S1" s="66" t="s">
@@ -9519,8 +9672,11 @@
       <c r="T1" s="29" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V1" s="79" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="65">
         <v>317</v>
       </c>
@@ -9533,7 +9689,7 @@
       <c r="D2" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="81" t="s">
         <v>269</v>
       </c>
       <c r="F2" s="65"/>
@@ -9548,15 +9704,19 @@
       <c r="O2" s="65"/>
       <c r="P2" s="65"/>
       <c r="Q2" s="65"/>
-      <c r="R2" s="69" t="s">
+      <c r="R2" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S2" s="69" t="s">
         <v>300</v>
       </c>
       <c r="T2" s="70"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" s="23"/>
+      <c r="V2" s="36" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="65">
         <v>318</v>
       </c>
@@ -9569,7 +9729,7 @@
       <c r="D3" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="81" t="s">
         <v>270</v>
       </c>
       <c r="F3" s="65"/>
@@ -9584,13 +9744,17 @@
       <c r="O3" s="65"/>
       <c r="P3" s="65"/>
       <c r="Q3" s="65"/>
-      <c r="R3" s="69" t="s">
+      <c r="R3" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S3" s="69"/>
       <c r="T3" s="70"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" s="23"/>
+      <c r="V3" s="36" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="65">
         <v>319</v>
       </c>
@@ -9603,7 +9767,7 @@
       <c r="D4" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="E4" s="81" t="s">
         <v>271</v>
       </c>
       <c r="F4" s="65"/>
@@ -9618,13 +9782,17 @@
       <c r="O4" s="65"/>
       <c r="P4" s="65"/>
       <c r="Q4" s="65"/>
-      <c r="R4" s="69" t="s">
+      <c r="R4" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S4" s="69"/>
       <c r="T4" s="70"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="23"/>
+      <c r="V4" s="36" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="65">
         <v>320</v>
       </c>
@@ -9637,7 +9805,7 @@
       <c r="D5" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="81" t="s">
         <v>272</v>
       </c>
       <c r="F5" s="65"/>
@@ -9652,13 +9820,17 @@
       <c r="O5" s="65"/>
       <c r="P5" s="65"/>
       <c r="Q5" s="65"/>
-      <c r="R5" s="69" t="s">
+      <c r="R5" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S5" s="69"/>
       <c r="T5" s="70"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="23"/>
+      <c r="V5" s="36" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="65">
         <v>321</v>
       </c>
@@ -9671,7 +9843,7 @@
       <c r="D6" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="81" t="s">
         <v>273</v>
       </c>
       <c r="F6" s="65"/>
@@ -9686,13 +9858,17 @@
       <c r="O6" s="65"/>
       <c r="P6" s="65"/>
       <c r="Q6" s="65"/>
-      <c r="R6" s="69" t="s">
+      <c r="R6" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S6" s="69"/>
       <c r="T6" s="70"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="23"/>
+      <c r="V6" s="36" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="65">
         <v>322</v>
       </c>
@@ -9705,7 +9881,7 @@
       <c r="D7" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="81" t="s">
         <v>274</v>
       </c>
       <c r="F7" s="65"/>
@@ -9720,15 +9896,19 @@
       <c r="O7" s="65"/>
       <c r="P7" s="65"/>
       <c r="Q7" s="65"/>
-      <c r="R7" s="69" t="s">
+      <c r="R7" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S7" s="69" t="s">
         <v>301</v>
       </c>
       <c r="T7" s="70"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="23"/>
+      <c r="V7" s="36" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="65">
         <v>323</v>
       </c>
@@ -9741,7 +9921,7 @@
       <c r="D8" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="81" t="s">
         <v>275</v>
       </c>
       <c r="F8" s="65"/>
@@ -9756,15 +9936,19 @@
       <c r="O8" s="65"/>
       <c r="P8" s="65"/>
       <c r="Q8" s="65"/>
-      <c r="R8" s="69" t="s">
+      <c r="R8" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S8" s="69" t="s">
         <v>301</v>
       </c>
       <c r="T8" s="70"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="23"/>
+      <c r="V8" s="36" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="65">
         <v>324</v>
       </c>
@@ -9777,7 +9961,7 @@
       <c r="D9" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="81" t="s">
         <v>276</v>
       </c>
       <c r="F9" s="65"/>
@@ -9792,15 +9976,19 @@
       <c r="O9" s="65"/>
       <c r="P9" s="65"/>
       <c r="Q9" s="65"/>
-      <c r="R9" s="69" t="s">
+      <c r="R9" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S9" s="69" t="s">
         <v>302</v>
       </c>
       <c r="T9" s="70"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="23"/>
+      <c r="V9" s="36" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="65">
         <v>325</v>
       </c>
@@ -9813,7 +10001,7 @@
       <c r="D10" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="81" t="s">
         <v>277</v>
       </c>
       <c r="F10" s="65"/>
@@ -9828,15 +10016,19 @@
       <c r="O10" s="65"/>
       <c r="P10" s="65"/>
       <c r="Q10" s="65"/>
-      <c r="R10" s="69" t="s">
+      <c r="R10" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S10" s="69" t="s">
         <v>302</v>
       </c>
       <c r="T10" s="70"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="23"/>
+      <c r="V10" s="36" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="65">
         <v>326</v>
       </c>
@@ -9849,7 +10041,7 @@
       <c r="D11" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E11" s="65" t="s">
+      <c r="E11" s="81" t="s">
         <v>278</v>
       </c>
       <c r="F11" s="65"/>
@@ -9864,15 +10056,19 @@
       <c r="O11" s="65"/>
       <c r="P11" s="65"/>
       <c r="Q11" s="65"/>
-      <c r="R11" s="69" t="s">
+      <c r="R11" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S11" s="69" t="s">
         <v>301</v>
       </c>
       <c r="T11" s="70"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="23"/>
+      <c r="V11" s="36" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="65">
         <v>327</v>
       </c>
@@ -9885,7 +10081,7 @@
       <c r="D12" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="E12" s="81" t="s">
         <v>279</v>
       </c>
       <c r="F12" s="65"/>
@@ -9900,13 +10096,17 @@
       <c r="O12" s="65"/>
       <c r="P12" s="65"/>
       <c r="Q12" s="65"/>
-      <c r="R12" s="69" t="s">
+      <c r="R12" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S12" s="69"/>
       <c r="T12" s="70"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="23"/>
+      <c r="V12" s="36" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="65">
         <v>328</v>
       </c>
@@ -9919,7 +10119,7 @@
       <c r="D13" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E13" s="65" t="s">
+      <c r="E13" s="81" t="s">
         <v>280</v>
       </c>
       <c r="F13" s="65"/>
@@ -9934,15 +10134,19 @@
       <c r="O13" s="65"/>
       <c r="P13" s="65"/>
       <c r="Q13" s="65"/>
-      <c r="R13" s="69" t="s">
+      <c r="R13" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S13" s="69" t="s">
         <v>303</v>
       </c>
-      <c r="T13" s="70"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T13" s="78"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="36" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="65">
         <v>329</v>
       </c>
@@ -9955,7 +10159,7 @@
       <c r="D14" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="81" t="s">
         <v>281</v>
       </c>
       <c r="F14" s="65"/>
@@ -9970,15 +10174,19 @@
       <c r="O14" s="65"/>
       <c r="P14" s="65"/>
       <c r="Q14" s="65"/>
-      <c r="R14" s="69" t="s">
+      <c r="R14" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S14" s="69" t="s">
         <v>303</v>
       </c>
       <c r="T14" s="70"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="23"/>
+      <c r="V14" s="36" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="65">
         <v>330</v>
       </c>
@@ -9991,7 +10199,7 @@
       <c r="D15" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E15" s="65" t="s">
+      <c r="E15" s="81" t="s">
         <v>282</v>
       </c>
       <c r="F15" s="65"/>
@@ -10006,15 +10214,19 @@
       <c r="O15" s="65"/>
       <c r="P15" s="65"/>
       <c r="Q15" s="65"/>
-      <c r="R15" s="69" t="s">
+      <c r="R15" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S15" s="69" t="s">
         <v>303</v>
       </c>
       <c r="T15" s="70"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="23"/>
+      <c r="V15" s="36" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="65">
         <v>331</v>
       </c>
@@ -10027,7 +10239,7 @@
       <c r="D16" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="81" t="s">
         <v>283</v>
       </c>
       <c r="F16" s="65"/>
@@ -10042,15 +10254,19 @@
       <c r="O16" s="65"/>
       <c r="P16" s="65"/>
       <c r="Q16" s="65"/>
-      <c r="R16" s="69" t="s">
+      <c r="R16" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S16" s="69" t="s">
         <v>303</v>
       </c>
       <c r="T16" s="70"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16" s="23"/>
+      <c r="V16" s="36" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="65">
         <v>332</v>
       </c>
@@ -10063,7 +10279,7 @@
       <c r="D17" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="81" t="s">
         <v>284</v>
       </c>
       <c r="F17" s="65"/>
@@ -10078,15 +10294,19 @@
       <c r="O17" s="65"/>
       <c r="P17" s="65"/>
       <c r="Q17" s="65"/>
-      <c r="R17" s="69" t="s">
+      <c r="R17" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S17" s="69" t="s">
         <v>303</v>
       </c>
       <c r="T17" s="70"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="23"/>
+      <c r="V17" s="36" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="65">
         <v>333</v>
       </c>
@@ -10099,7 +10319,7 @@
       <c r="D18" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="81" t="s">
         <v>285</v>
       </c>
       <c r="F18" s="65"/>
@@ -10114,15 +10334,19 @@
       <c r="O18" s="65"/>
       <c r="P18" s="65"/>
       <c r="Q18" s="65"/>
-      <c r="R18" s="69" t="s">
+      <c r="R18" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S18" s="69" t="s">
         <v>303</v>
       </c>
       <c r="T18" s="70"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="23"/>
+      <c r="V18" s="36" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="65">
         <v>334</v>
       </c>
@@ -10135,7 +10359,7 @@
       <c r="D19" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E19" s="65" t="s">
+      <c r="E19" s="81" t="s">
         <v>286</v>
       </c>
       <c r="F19" s="65"/>
@@ -10150,13 +10374,17 @@
       <c r="O19" s="65"/>
       <c r="P19" s="65"/>
       <c r="Q19" s="65"/>
-      <c r="R19" s="69" t="s">
+      <c r="R19" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S19" s="69"/>
       <c r="T19" s="70"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="23"/>
+      <c r="V19" s="36" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="65">
         <v>335</v>
       </c>
@@ -10169,7 +10397,7 @@
       <c r="D20" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E20" s="65" t="s">
+      <c r="E20" s="81" t="s">
         <v>287</v>
       </c>
       <c r="F20" s="65"/>
@@ -10184,13 +10412,17 @@
       <c r="O20" s="65"/>
       <c r="P20" s="65"/>
       <c r="Q20" s="65"/>
-      <c r="R20" s="69" t="s">
+      <c r="R20" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S20" s="69"/>
       <c r="T20" s="70"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20" s="23"/>
+      <c r="V20" s="36" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="65">
         <v>336</v>
       </c>
@@ -10203,7 +10435,7 @@
       <c r="D21" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E21" s="65" t="s">
+      <c r="E21" s="81" t="s">
         <v>288</v>
       </c>
       <c r="F21" s="65"/>
@@ -10218,13 +10450,17 @@
       <c r="O21" s="65"/>
       <c r="P21" s="65"/>
       <c r="Q21" s="65"/>
-      <c r="R21" s="69" t="s">
+      <c r="R21" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S21" s="69"/>
       <c r="T21" s="70"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21" s="23"/>
+      <c r="V21" s="36" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="65">
         <v>337</v>
       </c>
@@ -10237,7 +10473,7 @@
       <c r="D22" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="81" t="s">
         <v>289</v>
       </c>
       <c r="F22" s="65"/>
@@ -10252,13 +10488,17 @@
       <c r="O22" s="65"/>
       <c r="P22" s="65"/>
       <c r="Q22" s="65"/>
-      <c r="R22" s="69" t="s">
+      <c r="R22" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S22" s="69"/>
       <c r="T22" s="70"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U22" s="23"/>
+      <c r="V22" s="36" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="65">
         <v>338</v>
       </c>
@@ -10271,7 +10511,7 @@
       <c r="D23" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="81" t="s">
         <v>290</v>
       </c>
       <c r="F23" s="65"/>
@@ -10286,13 +10526,17 @@
       <c r="O23" s="65"/>
       <c r="P23" s="65"/>
       <c r="Q23" s="65"/>
-      <c r="R23" s="69" t="s">
+      <c r="R23" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S23" s="69"/>
       <c r="T23" s="70"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U23" s="23"/>
+      <c r="V23" s="36" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="65">
         <v>339</v>
       </c>
@@ -10305,7 +10549,7 @@
       <c r="D24" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E24" s="65" t="s">
+      <c r="E24" s="81" t="s">
         <v>291</v>
       </c>
       <c r="F24" s="65"/>
@@ -10320,15 +10564,19 @@
       <c r="O24" s="65"/>
       <c r="P24" s="65"/>
       <c r="Q24" s="65"/>
-      <c r="R24" s="69" t="s">
+      <c r="R24" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S24" s="69" t="s">
         <v>301</v>
       </c>
       <c r="T24" s="70"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24" s="23"/>
+      <c r="V24" s="36" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="65">
         <v>340</v>
       </c>
@@ -10341,7 +10589,7 @@
       <c r="D25" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E25" s="65" t="s">
+      <c r="E25" s="81" t="s">
         <v>292</v>
       </c>
       <c r="F25" s="65"/>
@@ -10356,15 +10604,19 @@
       <c r="O25" s="65"/>
       <c r="P25" s="65"/>
       <c r="Q25" s="65"/>
-      <c r="R25" s="69" t="s">
+      <c r="R25" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S25" s="69" t="s">
         <v>301</v>
       </c>
       <c r="T25" s="70"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25" s="23"/>
+      <c r="V25" s="36" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="65">
         <v>341</v>
       </c>
@@ -10377,7 +10629,7 @@
       <c r="D26" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E26" s="65" t="s">
+      <c r="E26" s="81" t="s">
         <v>293</v>
       </c>
       <c r="F26" s="65"/>
@@ -10392,15 +10644,19 @@
       <c r="O26" s="65"/>
       <c r="P26" s="65"/>
       <c r="Q26" s="65"/>
-      <c r="R26" s="69" t="s">
+      <c r="R26" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S26" s="69" t="s">
         <v>302</v>
       </c>
       <c r="T26" s="70"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U26" s="23"/>
+      <c r="V26" s="36" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="65">
         <v>342</v>
       </c>
@@ -10413,7 +10669,7 @@
       <c r="D27" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E27" s="65" t="s">
+      <c r="E27" s="81" t="s">
         <v>294</v>
       </c>
       <c r="F27" s="65"/>
@@ -10428,15 +10684,19 @@
       <c r="O27" s="65"/>
       <c r="P27" s="65"/>
       <c r="Q27" s="65"/>
-      <c r="R27" s="69" t="s">
+      <c r="R27" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S27" s="69" t="s">
         <v>302</v>
       </c>
       <c r="T27" s="70"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U27" s="23"/>
+      <c r="V27" s="36" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="65">
         <v>343</v>
       </c>
@@ -10449,7 +10709,7 @@
       <c r="D28" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E28" s="65" t="s">
+      <c r="E28" s="81" t="s">
         <v>295</v>
       </c>
       <c r="F28" s="65"/>
@@ -10464,15 +10724,19 @@
       <c r="O28" s="65"/>
       <c r="P28" s="65"/>
       <c r="Q28" s="65"/>
-      <c r="R28" s="69" t="s">
+      <c r="R28" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S28" s="69" t="s">
         <v>301</v>
       </c>
       <c r="T28" s="70"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U28" s="23"/>
+      <c r="V28" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="65">
         <v>344</v>
       </c>
@@ -10485,7 +10749,7 @@
       <c r="D29" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E29" s="65" t="s">
+      <c r="E29" s="81" t="s">
         <v>296</v>
       </c>
       <c r="F29" s="65"/>
@@ -10500,13 +10764,17 @@
       <c r="O29" s="65"/>
       <c r="P29" s="65"/>
       <c r="Q29" s="65"/>
-      <c r="R29" s="69" t="s">
+      <c r="R29" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S29" s="69"/>
       <c r="T29" s="70"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U29" s="23"/>
+      <c r="V29" s="36" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="65">
         <v>345</v>
       </c>
@@ -10519,7 +10787,7 @@
       <c r="D30" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E30" s="65" t="s">
+      <c r="E30" s="81" t="s">
         <v>297</v>
       </c>
       <c r="F30" s="65"/>
@@ -10534,13 +10802,17 @@
       <c r="O30" s="65"/>
       <c r="P30" s="65"/>
       <c r="Q30" s="65"/>
-      <c r="R30" s="69" t="s">
+      <c r="R30" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S30" s="69"/>
       <c r="T30" s="70"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U30" s="23"/>
+      <c r="V30" s="36" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="65">
         <v>346</v>
       </c>
@@ -10553,7 +10825,7 @@
       <c r="D31" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E31" s="65" t="s">
+      <c r="E31" s="81" t="s">
         <v>298</v>
       </c>
       <c r="F31" s="65"/>
@@ -10568,13 +10840,17 @@
       <c r="O31" s="65"/>
       <c r="P31" s="65"/>
       <c r="Q31" s="65"/>
-      <c r="R31" s="69" t="s">
+      <c r="R31" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S31" s="69"/>
       <c r="T31" s="70"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U31" s="23"/>
+      <c r="V31" s="36" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="65">
         <v>347</v>
       </c>
@@ -10587,7 +10863,7 @@
       <c r="D32" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="E32" s="65" t="s">
+      <c r="E32" s="81" t="s">
         <v>299</v>
       </c>
       <c r="F32" s="65"/>
@@ -10602,15 +10878,117 @@
       <c r="O32" s="65"/>
       <c r="P32" s="65"/>
       <c r="Q32" s="65"/>
-      <c r="R32" s="69" t="s">
+      <c r="R32" s="70" t="s">
         <v>3</v>
       </c>
       <c r="S32" s="69"/>
       <c r="T32" s="70"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="36" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="33" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U33" s="23"/>
+      <c r="V33" s="36" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="34" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U34" s="23"/>
+      <c r="V34" s="36" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="35" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V35" s="36" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="36" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V36" s="36" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="37" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V37" s="36" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="38" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V38" s="36" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="39" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V39" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="40" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V40" s="36" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="41" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V41" s="36" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="42" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V42" s="36" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="43" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V43" s="36" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="44" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V44" s="36" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="45" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V45" s="36" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="46" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V46" s="36" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="47" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V47" s="36" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="48" spans="21:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V48" s="36" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="49" spans="22:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V49" s="36" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="50" spans="22:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V50" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="51" spans="22:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V51" s="36" t="s">
+        <v>383</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update etl for finance.KPI_FACT.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -1343,9 +1343,6 @@
     <t>kpi_key</t>
   </si>
   <si>
-    <t>month_key</t>
-  </si>
-  <si>
     <t>kpi_name</t>
   </si>
   <si>
@@ -1404,6 +1401,9 @@
   </si>
   <si>
     <t xml:space="preserve"> [conform_finance]</t>
+  </si>
+  <si>
+    <t>date_key</t>
   </si>
 </sst>
 </file>
@@ -13888,7 +13888,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13977,7 +13977,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -14073,51 +14073,51 @@
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="65" t="s">
+    <row r="10" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="70" t="s">
         <v>403</v>
       </c>
-      <c r="B10" s="65" t="s">
-        <v>421</v>
-      </c>
+      <c r="B10" s="38"/>
       <c r="C10" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="38"/>
+        <v>31</v>
+      </c>
+      <c r="D10" s="70">
+        <v>50</v>
+      </c>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38" t="s">
-        <v>422</v>
-      </c>
+      <c r="G10" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="45"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="70" t="s">
-        <v>404</v>
-      </c>
-      <c r="B11" s="38"/>
+      <c r="A11" s="65" t="s">
+        <v>423</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>420</v>
+      </c>
       <c r="C11" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="70">
-        <v>50</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D11" s="38"/>
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
-      <c r="G11" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="I11" s="38"/>
       <c r="J11" s="38"/>
       <c r="K11" s="45"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="65" t="s">
@@ -14138,7 +14138,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="65" t="s">
@@ -14159,7 +14159,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="65" t="s">
@@ -14180,7 +14180,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="65" t="s">
@@ -14201,7 +14201,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B16" s="38"/>
       <c r="C16" s="65" t="s">
@@ -14222,7 +14222,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B17" s="38"/>
       <c r="C17" s="65" t="s">
@@ -14243,7 +14243,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B18" s="38"/>
       <c r="C18" s="65" t="s">
@@ -14264,7 +14264,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B19" s="38"/>
       <c r="C19" s="65" t="s">
@@ -14285,7 +14285,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="73" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="65" t="s">
@@ -14306,7 +14306,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="73" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="65" t="s">
@@ -14327,7 +14327,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="73" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B22" s="38"/>
       <c r="C22" s="65" t="s">
@@ -14348,7 +14348,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="73" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B23" s="38"/>
       <c r="C23" s="65" t="s">
@@ -14369,7 +14369,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="73" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B24" s="38"/>
       <c r="C24" s="65" t="s">
@@ -14390,7 +14390,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="73" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B25" s="38"/>
       <c r="C25" s="65" t="s">
@@ -14411,7 +14411,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="73" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B26" s="38"/>
       <c r="C26" s="65" t="s">
@@ -14432,7 +14432,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="73" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B27" s="38"/>
       <c r="C27" s="65" t="s">

</xml_diff>

<commit_message>
Added source system to finance fact mapping sheet
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7290" windowWidth="24240" windowHeight="5685" activeTab="6"/>
+    <workbookView xWindow="-90" yWindow="7290" windowWidth="24240" windowHeight="5685" firstSheet="23" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="accounting_period_dim" sheetId="34" r:id="rId28"/>
     <sheet name="program_mapping" sheetId="35" r:id="rId29"/>
     <sheet name="data for program_mapping" sheetId="36" r:id="rId30"/>
+    <sheet name="Fact 2 Source Mapping" sheetId="38" r:id="rId31"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -128,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="430">
   <si>
     <t>Category</t>
   </si>
@@ -1404,13 +1405,31 @@
   </si>
   <si>
     <t xml:space="preserve"> [conform_finance]</t>
+  </si>
+  <si>
+    <t>ComCare</t>
+  </si>
+  <si>
+    <t>Kypera</t>
+  </si>
+  <si>
+    <t>ANZ Expense Manager</t>
+  </si>
+  <si>
+    <t>TechOne (Finance)</t>
+  </si>
+  <si>
+    <t>TechOne (HRP)</t>
+  </si>
+  <si>
+    <t>CIM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1494,6 +1513,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1527,7 +1553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1758,11 +1784,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1909,6 +1993,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2213,7 +2311,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="B3" sqref="B3:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12062,6 +12160,314 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="B1:O32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2" s="85" t="s">
+        <v>428</v>
+      </c>
+      <c r="E2" s="85" t="s">
+        <v>427</v>
+      </c>
+      <c r="F2" s="84" t="s">
+        <v>425</v>
+      </c>
+      <c r="G2" s="85" t="s">
+        <v>426</v>
+      </c>
+      <c r="H2" s="86" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="38"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+    </row>
+    <row r="32" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O32" s="87"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13887,7 +14293,7 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added fact 2 system mapping for finance stuff
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7290" windowWidth="24240" windowHeight="5685" activeTab="6"/>
+    <workbookView xWindow="-90" yWindow="7290" windowWidth="24240" windowHeight="5685" firstSheet="23" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="accounting_period_dim" sheetId="34" r:id="rId28"/>
     <sheet name="program_mapping" sheetId="35" r:id="rId29"/>
     <sheet name="data for program_mapping" sheetId="36" r:id="rId30"/>
+    <sheet name="Fact 2 system mapping" sheetId="38" r:id="rId31"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -128,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="430">
   <si>
     <t>Category</t>
   </si>
@@ -1404,6 +1405,24 @@
   </si>
   <si>
     <t>date_key</t>
+  </si>
+  <si>
+    <t>Comcare</t>
+  </si>
+  <si>
+    <t>Techone (HRP)</t>
+  </si>
+  <si>
+    <t>TechOne (Finance)</t>
+  </si>
+  <si>
+    <t>Kypera</t>
+  </si>
+  <si>
+    <t>ANZ Expense manager</t>
+  </si>
+  <si>
+    <t>CIM</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1546,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1758,11 +1777,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1908,6 +1985,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2213,7 +2300,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="B3" sqref="B3:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12062,6 +12149,308 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="B1:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>425</v>
+      </c>
+      <c r="E2" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="F2" s="84" t="s">
+        <v>427</v>
+      </c>
+      <c r="G2" s="84" t="s">
+        <v>428</v>
+      </c>
+      <c r="H2" s="85" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="38"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13887,7 +14276,7 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update finance bus matrix.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7290" windowWidth="24240" windowHeight="5685" firstSheet="24" activeTab="9"/>
+    <workbookView xWindow="-90" yWindow="7290" windowWidth="24240" windowHeight="5685" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="487">
   <si>
     <t>Category</t>
   </si>
@@ -1606,9 +1606,6 @@
     <t>Records all transactions for long service leave and calculation</t>
   </si>
   <si>
-    <t>Date_of_Service_Key</t>
-  </si>
-  <si>
     <t>LSL_Average_Hours</t>
   </si>
   <si>
@@ -1624,7 +1621,25 @@
     <t>c8000or9000</t>
   </si>
   <si>
-    <t>Date of Service(LSL)  --- in employee_position_fact. Date_of_Service_Key -- most of them are NULL</t>
+    <t>Date_of_Service</t>
+  </si>
+  <si>
+    <t>Date of Service(LSL)  : val_date2 in table: [extract].[HRHMN_USR_FLD]</t>
+  </si>
+  <si>
+    <t>calcualte_date_key</t>
+  </si>
+  <si>
+    <t>PK for date</t>
+  </si>
+  <si>
+    <t>Input Value.</t>
+  </si>
+  <si>
+    <t>val_num1 in table: [HRHMN_USR_FLD]</t>
+  </si>
+  <si>
+    <t>based on primary position: pay_item_rate</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1731,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1744,6 +1759,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2041,7 +2062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2200,6 +2221,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3416,10 +3440,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K25" sqref="K25:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3521,7 +3545,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="87" t="s">
         <v>432</v>
       </c>
       <c r="B9" s="65" t="s">
@@ -3541,10 +3565,10 @@
     </row>
     <row r="10" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="87" t="s">
-        <v>433</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>434</v>
+        <v>482</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>483</v>
       </c>
       <c r="C10" s="65" t="s">
         <v>30</v>
@@ -3557,36 +3581,36 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
-        <v>429</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="87" t="s">
-        <v>44</v>
+        <v>433</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="70" t="s">
+        <v>434</v>
+      </c>
+      <c r="C11" s="65" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21" t="s">
-        <v>148</v>
-      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
+      <c r="K11" s="19" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="12" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="87" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="C12" s="70" t="s">
         <v>30</v>
@@ -3604,10 +3628,10 @@
     </row>
     <row r="13" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="87" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C13" s="70" t="s">
         <v>30</v>
@@ -3625,10 +3649,10 @@
     </row>
     <row r="14" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="87" t="s">
-        <v>436</v>
+        <v>46</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>437</v>
+        <v>18</v>
       </c>
       <c r="C14" s="70" t="s">
         <v>30</v>
@@ -3636,67 +3660,67 @@
       <c r="D14" s="19"/>
       <c r="E14" s="72"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>148</v>
+      </c>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
-      <c r="K14" s="19" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="19"/>
+    </row>
+    <row r="15" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="87" t="s">
-        <v>475</v>
-      </c>
-      <c r="B15" s="73" t="s">
-        <v>25</v>
+        <v>436</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>437</v>
       </c>
       <c r="C15" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="72"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="21" t="s">
-        <v>148</v>
-      </c>
+      <c r="G15" s="21"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
-      <c r="K15" s="86" t="s">
-        <v>481</v>
+      <c r="K15" s="19" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>444</v>
-      </c>
-      <c r="B16" s="19"/>
+      <c r="A16" s="87" t="s">
+        <v>480</v>
+      </c>
+      <c r="B16" s="73"/>
       <c r="C16" s="70" t="s">
-        <v>204</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>446</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+        <v>32</v>
+      </c>
+      <c r="D16" s="65"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>148</v>
+      </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
-      <c r="K16" s="19" t="s">
-        <v>435</v>
+      <c r="K16" s="88" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>439</v>
+      <c r="A17" s="87" t="s">
+        <v>444</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="19"/>
+      <c r="C17" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>446</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
@@ -3704,20 +3728,18 @@
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
       <c r="K17" s="19" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>441</v>
+      <c r="A18" s="87" t="s">
+        <v>439</v>
       </c>
       <c r="B18" s="19"/>
-      <c r="C18" s="70" t="s">
-        <v>204</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>446</v>
-      </c>
+      <c r="C18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -3725,12 +3747,12 @@
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>443</v>
+      <c r="A19" s="87" t="s">
+        <v>441</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="70" t="s">
@@ -3745,13 +3767,13 @@
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
-      <c r="K19" s="86" t="s">
-        <v>445</v>
+      <c r="K19" s="19" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>476</v>
+      <c r="A20" s="87" t="s">
+        <v>443</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="70" t="s">
@@ -3766,13 +3788,13 @@
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
-      <c r="K20" s="86" t="s">
+      <c r="K20" s="21" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>430</v>
+      <c r="A21" s="87" t="s">
+        <v>475</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="70" t="s">
@@ -3787,20 +3809,20 @@
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
-      <c r="K21" s="19" t="s">
-        <v>447</v>
+      <c r="K21" s="21" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>450</v>
+      <c r="A22" s="87" t="s">
+        <v>430</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="70" t="s">
         <v>204</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
@@ -3808,20 +3830,20 @@
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
-      <c r="K22" s="86" t="s">
-        <v>449</v>
+      <c r="K22" s="19" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>431</v>
+      <c r="A23" s="87" t="s">
+        <v>450</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="70" t="s">
         <v>204</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -3829,13 +3851,13 @@
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
-      <c r="K23" s="19" t="s">
-        <v>451</v>
+      <c r="K23" s="21" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>452</v>
+      <c r="A24" s="87" t="s">
+        <v>431</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="70" t="s">
@@ -3850,13 +3872,13 @@
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
       <c r="J24" s="19"/>
-      <c r="K24" s="86" t="s">
-        <v>453</v>
+      <c r="K24" s="19" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>454</v>
+      <c r="A25" s="87" t="s">
+        <v>452</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="70" t="s">
@@ -3871,20 +3893,20 @@
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
-      <c r="K25" s="19" t="s">
-        <v>455</v>
+      <c r="K25" s="21" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="87" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B26" s="19"/>
-      <c r="C26" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="19">
-        <v>10</v>
+      <c r="C26" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>446</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
@@ -3892,20 +3914,20 @@
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
       <c r="J26" s="19"/>
-      <c r="K26" s="86" t="s">
-        <v>449</v>
+      <c r="K26" s="21" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="87" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="19">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -3913,20 +3935,20 @@
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
-      <c r="K27" s="86" t="s">
+      <c r="K27" s="21" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>477</v>
+      <c r="A28" s="87" t="s">
+        <v>457</v>
       </c>
       <c r="B28" s="19"/>
-      <c r="C28" s="70" t="s">
-        <v>204</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>446</v>
+      <c r="C28" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="19">
+        <v>100</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -3934,34 +3956,34 @@
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
-      <c r="K28" s="86" t="s">
+      <c r="K28" s="21" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="86" t="s">
+        <v>476</v>
+      </c>
+      <c r="B29" s="86"/>
+      <c r="C29" s="77" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>446</v>
+      </c>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="86"/>
+      <c r="K29" s="86" t="s">
         <v>458</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>478</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="70" t="s">
-        <v>204</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>446</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="86" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="70" t="s">
@@ -3982,7 +4004,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="70" t="s">
@@ -3997,13 +4019,13 @@
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
-      <c r="K31" s="19" t="s">
-        <v>461</v>
+      <c r="K31" s="86" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="70" t="s">
@@ -4019,12 +4041,12 @@
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="70" t="s">
@@ -4040,12 +4062,12 @@
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
       <c r="K33" s="19" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="70" t="s">
@@ -4061,12 +4083,12 @@
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="70" t="s">
@@ -4082,12 +4104,12 @@
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="K35" s="19" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="70" t="s">
@@ -4103,19 +4125,19 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="K36" s="19" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B37" s="19"/>
-      <c r="C37" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="19">
-        <v>20</v>
+      <c r="C37" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>446</v>
       </c>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
@@ -4124,19 +4146,19 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="K37" s="19" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>480</v>
+      <c r="A38" s="87" t="s">
+        <v>472</v>
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="19" t="s">
         <v>31</v>
       </c>
       <c r="D38" s="19">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
@@ -4145,21 +4167,42 @@
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
       <c r="K38" s="19" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="87" t="s">
+        <v>479</v>
+      </c>
       <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
+      <c r="C39" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="19">
+        <v>10</v>
+      </c>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
+      <c r="K39" s="19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update finance_bus_matrix to add finance_variable_dim table.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7290" windowWidth="24240" windowHeight="5685" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="-90" yWindow="7350" windowWidth="24240" windowHeight="5625" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -16,28 +16,30 @@
     <sheet name="KPI_fact" sheetId="17" r:id="rId7"/>
     <sheet name="bad_debt_fact" sheetId="20" r:id="rId8"/>
     <sheet name="creditor_fact" sheetId="21" r:id="rId9"/>
-    <sheet name="LSL_fact" sheetId="23" r:id="rId10"/>
-    <sheet name="PO_fact" sheetId="24" r:id="rId11"/>
-    <sheet name="invoice_fact" sheetId="25" r:id="rId12"/>
-    <sheet name="SC_fact" sheetId="26" r:id="rId13"/>
-    <sheet name="expense_fact" sheetId="27" r:id="rId14"/>
-    <sheet name="wage_fact" sheetId="28" r:id="rId15"/>
-    <sheet name="forecasting_fact" sheetId="29" r:id="rId16"/>
-    <sheet name="payments_fact" sheetId="30" r:id="rId17"/>
-    <sheet name="GL_transaction_fact" sheetId="31" r:id="rId18"/>
-    <sheet name="budget_fact" sheetId="32" r:id="rId19"/>
-    <sheet name="Date_DIM" sheetId="7" r:id="rId20"/>
-    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId21"/>
-    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId22"/>
-    <sheet name="Program_DIM" sheetId="11" r:id="rId23"/>
-    <sheet name="cost_centre_DIM" sheetId="15" r:id="rId24"/>
-    <sheet name="Account_DIM" sheetId="13" r:id="rId25"/>
-    <sheet name="Employee_DIM" sheetId="5" r:id="rId26"/>
-    <sheet name="Ledger_DIM" sheetId="33" r:id="rId27"/>
-    <sheet name="accounting_period_dim" sheetId="34" r:id="rId28"/>
-    <sheet name="program_mapping" sheetId="35" r:id="rId29"/>
-    <sheet name="data for program_mapping" sheetId="36" r:id="rId30"/>
-    <sheet name="Fact 2 system mapping" sheetId="38" r:id="rId31"/>
+    <sheet name="Finance_Variable_Dim" sheetId="40" r:id="rId10"/>
+    <sheet name="LSL_fact" sheetId="23" r:id="rId11"/>
+    <sheet name="extract.employee_workcover_rate" sheetId="39" r:id="rId12"/>
+    <sheet name="PO_fact" sheetId="24" r:id="rId13"/>
+    <sheet name="invoice_fact" sheetId="25" r:id="rId14"/>
+    <sheet name="SC_fact" sheetId="26" r:id="rId15"/>
+    <sheet name="expense_fact" sheetId="27" r:id="rId16"/>
+    <sheet name="wage_fact" sheetId="28" r:id="rId17"/>
+    <sheet name="forecasting_fact" sheetId="29" r:id="rId18"/>
+    <sheet name="payments_fact" sheetId="30" r:id="rId19"/>
+    <sheet name="GL_transaction_fact" sheetId="31" r:id="rId20"/>
+    <sheet name="budget_fact" sheetId="32" r:id="rId21"/>
+    <sheet name="Date_DIM" sheetId="7" r:id="rId22"/>
+    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId23"/>
+    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId24"/>
+    <sheet name="Program_DIM" sheetId="11" r:id="rId25"/>
+    <sheet name="cost_centre_DIM" sheetId="15" r:id="rId26"/>
+    <sheet name="Account_DIM" sheetId="13" r:id="rId27"/>
+    <sheet name="Employee_DIM" sheetId="5" r:id="rId28"/>
+    <sheet name="Ledger_DIM" sheetId="33" r:id="rId29"/>
+    <sheet name="accounting_period_dim" sheetId="34" r:id="rId30"/>
+    <sheet name="program_mapping" sheetId="35" r:id="rId31"/>
+    <sheet name="data for program_mapping" sheetId="36" r:id="rId32"/>
+    <sheet name="Fact 2 system mapping" sheetId="38" r:id="rId33"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -129,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="512">
   <si>
     <t>Category</t>
   </si>
@@ -1494,9 +1496,6 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Fixed data.</t>
-  </si>
-  <si>
     <t>Revised_Liability_based_on_probability</t>
   </si>
   <si>
@@ -1507,9 +1506,6 @@
   </si>
   <si>
     <t>Primary_Work_Location</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
   <si>
     <t>NPV_of_Liability</t>
@@ -1640,6 +1636,111 @@
   </si>
   <si>
     <t>based on primary position: pay_item_rate</t>
+  </si>
+  <si>
+    <r>
+      <t>using formula to calucate /</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if years rounded down&lt;7 update it same as  Weeks based on Completed years of Service</t>
+    </r>
+  </si>
+  <si>
+    <t>employee_workcover_rate</t>
+  </si>
+  <si>
+    <t>workcover rate for LSL_fact</t>
+  </si>
+  <si>
+    <t>export using T1 ETL into csv file and import into dwh</t>
+  </si>
+  <si>
+    <t>Id_Number</t>
+  </si>
+  <si>
+    <t>Active_Indicator</t>
+  </si>
+  <si>
+    <t>Effective_Date_Job</t>
+  </si>
+  <si>
+    <t>Position_Code</t>
+  </si>
+  <si>
+    <t>Pay_Component_Code</t>
+  </si>
+  <si>
+    <t>Pay_Component_Description</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>T1 ETL to export: from HRIS.Employee Entitlement - Primary Position: pay component details - pay compoment 2000.0 OnCosts - Workcover Levy</t>
+  </si>
+  <si>
+    <t>some cannot find value.</t>
+  </si>
+  <si>
+    <t>Fixed data. -- question: not all 1.
+ update   conform_finance.lsl_fact 
+     set Probability=
+      case Years_Rounded_Down
+      when 6 then  0.87
+      when 5 then  0.5
+         when 4 then  0.12
+         when 3 then  0.12
+         when 2 then  0.12
+      when 1 then  0.12
+      when 0 then 0.12
+          else 1
+      end;</t>
+  </si>
+  <si>
+    <t>dim</t>
+  </si>
+  <si>
+    <t>Used to store variable values for fiannct reports and easy to change</t>
+  </si>
+  <si>
+    <t>variable_key</t>
+  </si>
+  <si>
+    <t>report_name</t>
+  </si>
+  <si>
+    <t>variable_name</t>
+  </si>
+  <si>
+    <t>variable_value</t>
+  </si>
+  <si>
+    <t>validate_date</t>
+  </si>
+  <si>
+    <t>expire_date</t>
+  </si>
+  <si>
+    <t>validate_flag</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>Finance_Variable_Dim</t>
+  </si>
+  <si>
+    <t>report owner</t>
+  </si>
+  <si>
+    <t>16,4</t>
   </si>
 </sst>
 </file>
@@ -2062,7 +2163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2225,6 +2326,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3440,10 +3548,336 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>509</v>
+      </c>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="85" t="s">
+        <v>499</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="85" t="s">
+        <v>509</v>
+      </c>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>421</v>
+      </c>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="85"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="73" t="s">
+        <v>501</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="73" t="s">
+        <v>502</v>
+      </c>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="70">
+        <v>50</v>
+      </c>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="73" t="s">
+        <v>503</v>
+      </c>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="70">
+        <v>50</v>
+      </c>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="73" t="s">
+        <v>504</v>
+      </c>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="65" t="s">
+        <v>511</v>
+      </c>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+    </row>
+    <row r="13" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="73" t="s">
+        <v>508</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>510</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="70">
+        <v>50</v>
+      </c>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="73" t="s">
+        <v>505</v>
+      </c>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="73" t="s">
+        <v>506</v>
+      </c>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="73" t="s">
+        <v>507</v>
+      </c>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="65">
+        <v>2</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25:K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3490,7 +3924,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3565,10 +3999,10 @@
     </row>
     <row r="10" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="87" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C10" s="65" t="s">
         <v>30</v>
@@ -3581,7 +4015,7 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
@@ -3691,7 +4125,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="87" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B16" s="73"/>
       <c r="C16" s="70" t="s">
@@ -3707,7 +4141,7 @@
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" s="88" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3772,7 +4206,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="89" t="s">
         <v>443</v>
       </c>
       <c r="B20" s="19"/>
@@ -3789,12 +4223,12 @@
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="21" t="s">
-        <v>445</v>
+        <v>485</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="87" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="70" t="s">
@@ -3810,7 +4244,7 @@
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" s="21" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3852,7 +4286,7 @@
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
       <c r="K23" s="21" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3876,8 +4310,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="87" t="s">
+    <row r="25" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="A25" s="89" t="s">
         <v>452</v>
       </c>
       <c r="B25" s="19"/>
@@ -3893,13 +4327,13 @@
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
-      <c r="K25" s="21" t="s">
-        <v>453</v>
+      <c r="K25" s="91" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="87" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="70" t="s">
@@ -3915,12 +4349,12 @@
       <c r="I26" s="19"/>
       <c r="J26" s="19"/>
       <c r="K26" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="87" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19" t="s">
@@ -3941,7 +4375,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="87" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19" t="s">
@@ -3961,29 +4395,31 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="86" t="s">
-        <v>476</v>
-      </c>
-      <c r="B29" s="86"/>
-      <c r="C29" s="77" t="s">
+      <c r="A29" s="89" t="s">
+        <v>474</v>
+      </c>
+      <c r="B29" s="89"/>
+      <c r="C29" s="89" t="s">
         <v>204</v>
       </c>
-      <c r="D29" s="63" t="s">
-        <v>446</v>
+      <c r="D29" s="90" t="s">
+        <v>448</v>
       </c>
       <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
+      <c r="F29" s="86" t="s">
+        <v>497</v>
+      </c>
       <c r="G29" s="86"/>
       <c r="H29" s="86"/>
       <c r="I29" s="86"/>
       <c r="J29" s="86"/>
-      <c r="K29" s="86" t="s">
-        <v>458</v>
+      <c r="K29" s="21" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>477</v>
+      <c r="A30" s="87" t="s">
+        <v>475</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="70" t="s">
@@ -3998,13 +4434,13 @@
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
-      <c r="K30" s="86" t="s">
+      <c r="K30" s="21" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>459</v>
+      <c r="A31" s="87" t="s">
+        <v>457</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="70" t="s">
@@ -4019,13 +4455,13 @@
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
-      <c r="K31" s="86" t="s">
+      <c r="K31" s="19" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>460</v>
+      <c r="A32" s="87" t="s">
+        <v>458</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="70" t="s">
@@ -4041,12 +4477,12 @@
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>462</v>
+      <c r="A33" s="87" t="s">
+        <v>460</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="70" t="s">
@@ -4062,12 +4498,12 @@
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
       <c r="K33" s="19" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>478</v>
+      <c r="A34" s="87" t="s">
+        <v>476</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="70" t="s">
@@ -4083,12 +4519,12 @@
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>464</v>
+      <c r="A35" s="87" t="s">
+        <v>462</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="70" t="s">
@@ -4104,12 +4540,12 @@
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="K35" s="19" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>466</v>
+      <c r="A36" s="87" t="s">
+        <v>464</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="70" t="s">
@@ -4125,12 +4561,12 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="K36" s="19" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="87" t="s">
         <v>467</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>469</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="70" t="s">
@@ -4146,12 +4582,12 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="K37" s="19" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="87" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="19" t="s">
@@ -4167,12 +4603,12 @@
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
       <c r="K38" s="19" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="87" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="19" t="s">
@@ -4188,7 +4624,7 @@
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
       <c r="K39" s="19" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -4210,12 +4646,316 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="85" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="85" t="s">
+        <v>487</v>
+      </c>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>488</v>
+      </c>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="85"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="68" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="65" t="s">
+        <v>489</v>
+      </c>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="65">
+        <v>50</v>
+      </c>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="65" t="s">
+        <v>490</v>
+      </c>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="65">
+        <v>50</v>
+      </c>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="65" t="s">
+        <v>491</v>
+      </c>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="65">
+        <v>50</v>
+      </c>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="65" t="s">
+        <v>492</v>
+      </c>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="65">
+        <v>50</v>
+      </c>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="65">
+        <v>50</v>
+      </c>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="65" t="s">
+        <v>494</v>
+      </c>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="65">
+        <v>50</v>
+      </c>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="65" t="s">
+        <v>495</v>
+      </c>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="65">
+        <v>50</v>
+      </c>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4263,458 +5003,6 @@
       </c>
       <c r="B4" s="23" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="45"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="23"/>
-    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="45"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="23"/>
-    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -4916,7 +5204,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -4932,7 +5220,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -4940,7 +5228,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5142,7 +5430,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5158,7 +5446,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5166,7 +5454,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5368,7 +5656,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5384,7 +5672,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5392,7 +5680,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5594,7 +5882,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5610,7 +5898,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5618,7 +5906,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5820,7 +6108,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5836,7 +6124,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5844,7 +6132,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5857,7 +6145,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -6046,7 +6334,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6062,7 +6350,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6070,7 +6358,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -6861,6 +7149,458 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="45"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="45"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="45"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="45"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -7004,7 +7744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -7149,7 +7889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -7294,7 +8034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -7439,7 +8179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -8150,7 +8890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -9096,7 +9836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -9283,7 +10023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -9768,1002 +10508,6 @@
       <c r="I29" s="38"/>
       <c r="J29" s="38"/>
       <c r="K29" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:K29"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>212</v>
-      </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="38">
-        <v>50</v>
-      </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="64" t="s">
-        <v>213</v>
-      </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="63">
-        <v>11</v>
-      </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
-        <v>240</v>
-      </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="18">
-        <v>5</v>
-      </c>
-      <c r="E25" s="44"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="18">
-        <v>50</v>
-      </c>
-      <c r="E26" s="44"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="18">
-        <v>1</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:K28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="39.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="23" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="68" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="67" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="67" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>242</v>
-      </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>243</v>
-      </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="38">
-        <v>30</v>
-      </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="38">
-        <v>100</v>
-      </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="38">
-        <v>100</v>
-      </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="38">
-        <v>100</v>
-      </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>247</v>
-      </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="38">
-        <v>100</v>
-      </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="38">
-        <v>100</v>
-      </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="38">
-        <v>100</v>
-      </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="38">
-        <v>100</v>
-      </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
-        <v>251</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="38">
-        <v>100</v>
-      </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="38">
-        <v>100</v>
-      </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
-        <v>253</v>
-      </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="38">
-        <v>100</v>
-      </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="38">
-        <v>100</v>
-      </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
-        <v>255</v>
-      </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="38">
-        <v>100</v>
-      </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="38">
-        <v>100</v>
-      </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
-        <v>257</v>
-      </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="38">
-        <v>100</v>
-      </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="38">
-        <v>100</v>
-      </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
-        <v>259</v>
-      </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="38">
-        <v>20</v>
-      </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
-        <v>260</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="38">
-        <v>50</v>
-      </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11500,6 +11244,1002 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:K29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="38">
+        <v>50</v>
+      </c>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="64" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="63">
+        <v>11</v>
+      </c>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="64" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="18">
+        <v>5</v>
+      </c>
+      <c r="E25" s="44"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="18">
+        <v>50</v>
+      </c>
+      <c r="E26" s="44"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="18">
+        <v>1</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="39.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="23" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="38">
+        <v>30</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="38">
+        <v>100</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="38">
+        <v>100</v>
+      </c>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="38">
+        <v>100</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="38">
+        <v>100</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="38">
+        <v>100</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="38">
+        <v>100</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="38">
+        <v>100</v>
+      </c>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="38">
+        <v>100</v>
+      </c>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="38">
+        <v>100</v>
+      </c>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="38">
+        <v>100</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="38">
+        <v>100</v>
+      </c>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="38">
+        <v>100</v>
+      </c>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="38">
+        <v>100</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="38">
+        <v>100</v>
+      </c>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="38">
+        <v>100</v>
+      </c>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="38">
+        <v>20</v>
+      </c>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="38">
+        <v>50</v>
+      </c>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -12903,7 +13643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -14667,7 +15407,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15030,7 +15770,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update finance_bus_matrix for reconcile_invocie_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7350" windowWidth="24240" windowHeight="5625" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="564">
   <si>
     <t>Category</t>
   </si>
@@ -1786,9 +1786,6 @@
     <t>ComCare_serviced_hours</t>
   </si>
   <si>
-    <t>Comcare_service_charges</t>
-  </si>
-  <si>
     <t>Balance_flag</t>
   </si>
   <si>
@@ -1847,9 +1844,6 @@
   </si>
   <si>
     <t>varchar(32)</t>
-  </si>
-  <si>
-    <t>FK for account_dim</t>
   </si>
   <si>
     <t>join conform_comcare.customer_dim.Client_ID</t>
@@ -1892,21 +1886,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">join conform_finance.program_dim -- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>mabye need to build mapping table</t>
-    </r>
-  </si>
-  <si>
     <t>05/12/2016 to 18/12/2016</t>
   </si>
   <si>
@@ -1919,7 +1898,22 @@
     <t>numeric(14,2)</t>
   </si>
   <si>
-    <t>DSIS DSOATS</t>
+    <t>ComCare_service_charges</t>
+  </si>
+  <si>
+    <t>Accnbri</t>
+  </si>
+  <si>
+    <t>debtor number</t>
+  </si>
+  <si>
+    <t>comcare service type</t>
+  </si>
+  <si>
+    <t>DSIS ,DSOATS,DSDA,DSOR,DSCC</t>
+  </si>
+  <si>
+    <t>ComCare_service_type</t>
   </si>
 </sst>
 </file>
@@ -6787,10 +6781,10 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6910,10 +6904,10 @@
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
-        <v>143</v>
+        <v>559</v>
       </c>
       <c r="B10" s="64" t="s">
-        <v>547</v>
+        <v>560</v>
       </c>
       <c r="C10" s="64" t="s">
         <v>30</v>
@@ -6925,16 +6919,16 @@
         <v>148</v>
       </c>
       <c r="H10" s="64" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I10" s="64" t="s">
         <v>192</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="K10" s="95" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -6942,7 +6936,7 @@
         <v>517</v>
       </c>
       <c r="B11" s="64" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C11" s="64" t="s">
         <v>30</v>
@@ -6954,7 +6948,7 @@
         <v>148</v>
       </c>
       <c r="H11" s="64" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I11" s="64" t="s">
         <v>303</v>
@@ -6963,7 +6957,7 @@
         <v>304</v>
       </c>
       <c r="K11" s="94" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="L11" s="11"/>
     </row>
@@ -6972,7 +6966,7 @@
         <v>518</v>
       </c>
       <c r="B12" s="72" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C12" s="64" t="s">
         <v>30</v>
@@ -6993,7 +6987,7 @@
         <v>519</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C13" s="64" t="s">
         <v>30</v>
@@ -7010,135 +7004,124 @@
       <c r="K13" s="96"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>520</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C14" s="64" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="21"/>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>563</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>561</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H14" s="64" t="s">
-        <v>544</v>
-      </c>
-      <c r="I14" s="64" t="s">
-        <v>545</v>
-      </c>
-      <c r="J14" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="K14" s="96" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="69" t="s">
-        <v>521</v>
-      </c>
-      <c r="B15" s="64" t="s">
-        <v>532</v>
-      </c>
       <c r="C15" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
+        <v>31</v>
+      </c>
+      <c r="D15" s="21">
+        <v>20</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>562</v>
+      </c>
+      <c r="F15" s="21"/>
       <c r="G15" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H15" s="64" t="s">
+        <v>543</v>
+      </c>
+      <c r="I15" s="64" t="s">
         <v>544</v>
       </c>
-      <c r="I15" s="64" t="s">
-        <v>222</v>
-      </c>
-      <c r="J15" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="94" t="s">
-        <v>550</v>
-      </c>
+      <c r="J15" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="K15" s="96"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B16" s="64" t="s">
-        <v>533</v>
-      </c>
-      <c r="C16" s="69" t="s">
-        <v>204</v>
-      </c>
-      <c r="D16" s="64" t="s">
-        <v>177</v>
-      </c>
-      <c r="E16" s="64">
-        <v>175.57</v>
-      </c>
+        <v>531</v>
+      </c>
+      <c r="C16" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
       <c r="F16" s="64"/>
       <c r="G16" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H16" s="64" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I16" s="64" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="J16" s="64" t="s">
-        <v>560</v>
-      </c>
-      <c r="K16" s="97"/>
-    </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="K16" s="94" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B17" s="64" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="64">
-        <v>40</v>
-      </c>
-      <c r="E17" s="64" t="s">
-        <v>557</v>
+        <v>204</v>
+      </c>
+      <c r="D17" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="E17" s="64">
+        <v>175.57</v>
       </c>
       <c r="F17" s="64"/>
       <c r="G17" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H17" s="64" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I17" s="64" t="s">
-        <v>306</v>
+        <v>208</v>
       </c>
       <c r="J17" s="64" t="s">
-        <v>304</v>
-      </c>
-      <c r="K17" s="94" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+      <c r="K17" s="97"/>
+    </row>
+    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
-        <v>524</v>
-      </c>
-      <c r="B18" s="64"/>
+        <v>523</v>
+      </c>
+      <c r="B18" s="64" t="s">
+        <v>533</v>
+      </c>
       <c r="C18" s="69" t="s">
         <v>31</v>
       </c>
@@ -7146,135 +7129,151 @@
         <v>40</v>
       </c>
       <c r="E18" s="64" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="F18" s="64"/>
       <c r="G18" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H18" s="64" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I18" s="64" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J18" s="64" t="s">
         <v>304</v>
       </c>
-      <c r="K18" s="94"/>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K18" s="94" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
+        <v>524</v>
+      </c>
+      <c r="B19" s="64"/>
+      <c r="C19" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="64">
+        <v>40</v>
+      </c>
+      <c r="E19" s="64" t="s">
+        <v>555</v>
+      </c>
+      <c r="F19" s="64"/>
+      <c r="G19" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" s="64" t="s">
+        <v>543</v>
+      </c>
+      <c r="I19" s="64" t="s">
+        <v>305</v>
+      </c>
+      <c r="J19" s="64" t="s">
+        <v>304</v>
+      </c>
+      <c r="K19" s="94"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="69" t="s">
         <v>525</v>
       </c>
-      <c r="B19" s="64" t="s">
-        <v>559</v>
-      </c>
-      <c r="C19" s="69" t="s">
+      <c r="B20" s="64" t="s">
+        <v>556</v>
+      </c>
+      <c r="C20" s="69" t="s">
         <v>228</v>
       </c>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64" t="s">
-        <v>538</v>
-      </c>
-      <c r="H19" s="64" t="s">
-        <v>539</v>
-      </c>
-      <c r="I19" s="64" t="s">
-        <v>540</v>
-      </c>
-      <c r="J19" s="64" t="s">
-        <v>542</v>
-      </c>
-      <c r="K19" s="90" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="69" t="s">
-        <v>526</v>
-      </c>
-      <c r="B20" s="64" t="s">
-        <v>535</v>
-      </c>
-      <c r="C20" s="69" t="s">
-        <v>204</v>
-      </c>
-      <c r="D20" s="64" t="s">
-        <v>536</v>
-      </c>
+      <c r="D20" s="64"/>
       <c r="E20" s="64"/>
       <c r="F20" s="64"/>
       <c r="G20" s="64" t="s">
+        <v>537</v>
+      </c>
+      <c r="H20" s="64" t="s">
         <v>538</v>
       </c>
-      <c r="H20" s="64" t="s">
+      <c r="I20" s="64" t="s">
         <v>539</v>
       </c>
-      <c r="I20" s="64" t="s">
+      <c r="J20" s="64" t="s">
         <v>541</v>
       </c>
-      <c r="J20" s="64" t="s">
-        <v>543</v>
-      </c>
-      <c r="K20" s="98"/>
+      <c r="K20" s="90" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
-        <v>527</v>
-      </c>
-      <c r="B21" s="64"/>
+        <v>558</v>
+      </c>
+      <c r="B21" s="64" t="s">
+        <v>534</v>
+      </c>
       <c r="C21" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="D21" s="64" t="s">
+        <v>535</v>
+      </c>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64" t="s">
+        <v>537</v>
+      </c>
+      <c r="H21" s="64" t="s">
+        <v>538</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>540</v>
+      </c>
+      <c r="J21" s="64" t="s">
+        <v>542</v>
+      </c>
+      <c r="K21" s="98"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="69" t="s">
+        <v>526</v>
+      </c>
+      <c r="B22" s="64"/>
+      <c r="C22" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="64">
+      <c r="D22" s="64">
         <v>1</v>
       </c>
-      <c r="E21" s="64" t="s">
+      <c r="E22" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="97" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="34"/>
-    </row>
-    <row r="23" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
-        <v>552</v>
-      </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="74"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="97" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="s">
-        <v>551</v>
+      <c r="A24" s="63" t="s">
+        <v>550</v>
       </c>
       <c r="B24" s="62"/>
       <c r="C24" s="62"/>
@@ -7285,25 +7284,27 @@
       <c r="H24" s="62"/>
       <c r="I24" s="62"/>
       <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="s">
-        <v>553</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
+      <c r="K24" s="74"/>
+    </row>
+    <row r="25" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="62" t="s">
+        <v>549</v>
+      </c>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="63" t="s">
+        <v>551</v>
+      </c>
       <c r="B26" s="38"/>
       <c r="C26" s="22"/>
       <c r="D26" s="36"/>
@@ -7430,13 +7431,13 @@
       <c r="H35" s="38"/>
       <c r="I35" s="36"/>
       <c r="J35" s="38"/>
-      <c r="K35" s="36"/>
+      <c r="K35" s="38"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="38"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="38"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
@@ -7449,14 +7450,14 @@
       <c r="A37" s="22"/>
       <c r="B37" s="38"/>
       <c r="C37" s="22"/>
-      <c r="D37" s="36"/>
+      <c r="D37" s="38"/>
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
+      <c r="I37" s="36"/>
       <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
+      <c r="K37" s="36"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
@@ -7495,7 +7496,7 @@
       <c r="H40" s="38"/>
       <c r="I40" s="38"/>
       <c r="J40" s="38"/>
-      <c r="K40" s="36"/>
+      <c r="K40" s="38"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
@@ -7505,23 +7506,23 @@
       <c r="E41" s="38"/>
       <c r="F41" s="38"/>
       <c r="G41" s="38"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
       <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
+      <c r="K41" s="36"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="41"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="38"/>
+      <c r="K42" s="38"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="42"/>
@@ -7641,40 +7642,40 @@
       <c r="K51" s="41"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="37"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="40"/>
+      <c r="A52" s="42"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
       <c r="H52" s="41"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="38"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="41"/>
       <c r="K52" s="41"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="38"/>
+      <c r="A53" s="37"/>
       <c r="B53" s="38"/>
       <c r="C53" s="37"/>
       <c r="D53" s="39"/>
-      <c r="E53" s="38"/>
+      <c r="E53" s="40"/>
       <c r="F53" s="38"/>
       <c r="G53" s="40"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="40"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="38"/>
       <c r="J53" s="38"/>
-      <c r="K53" s="38"/>
+      <c r="K53" s="41"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="37"/>
+      <c r="A54" s="38"/>
       <c r="B54" s="38"/>
       <c r="C54" s="37"/>
       <c r="D54" s="39"/>
       <c r="E54" s="38"/>
       <c r="F54" s="38"/>
       <c r="G54" s="40"/>
-      <c r="H54" s="41"/>
+      <c r="H54" s="38"/>
       <c r="I54" s="40"/>
       <c r="J54" s="38"/>
       <c r="K54" s="38"/>
@@ -7691,6 +7692,19 @@
       <c r="I55" s="40"/>
       <c r="J55" s="38"/>
       <c r="K55" s="38"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="37"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="40"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update etl for reconcile_invocie_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2068" uniqueCount="564">
   <si>
     <t>Category</t>
   </si>
@@ -1759,9 +1759,6 @@
     <t>Reconcile Invoice Fact</t>
   </si>
   <si>
-    <t>Client_key</t>
-  </si>
-  <si>
     <t>Portfolio_key</t>
   </si>
   <si>
@@ -1789,9 +1786,6 @@
     <t>Balance_flag</t>
   </si>
   <si>
-    <t>FK for ComCare customer</t>
-  </si>
-  <si>
     <t>FK for Portfolio</t>
   </si>
   <si>
@@ -1813,9 +1807,6 @@
     <t>ComCare actual service charges</t>
   </si>
   <si>
-    <t>9,2</t>
-  </si>
-  <si>
     <t>if Invocie_Amount= Comcare_service_charges, then 'Y' else 'N'</t>
   </si>
   <si>
@@ -1844,9 +1835,6 @@
   </si>
   <si>
     <t>varchar(32)</t>
-  </si>
-  <si>
-    <t>join conform_comcare.customer_dim.Client_ID</t>
   </si>
   <si>
     <t>join conform_finance.account_dim
@@ -1914,6 +1902,18 @@
   </si>
   <si>
     <t>ComCare_service_type</t>
+  </si>
+  <si>
+    <t>Account_key</t>
+  </si>
+  <si>
+    <t>FK for conform_finance.account_dim</t>
+  </si>
+  <si>
+    <t>Client_id</t>
+  </si>
+  <si>
+    <t>28,5</t>
   </si>
 </sst>
 </file>
@@ -2347,7 +2347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2537,6 +2537,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -6781,10 +6784,10 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A13" sqref="A13:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6903,40 +6906,32 @@
       <c r="K9" s="94"/>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="72" t="s">
-        <v>559</v>
-      </c>
-      <c r="B10" s="64" t="s">
+      <c r="A10" s="99" t="s">
         <v>560</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="B10" s="79" t="s">
+        <v>561</v>
+      </c>
+      <c r="C10" s="79" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="64"/>
       <c r="E10" s="64"/>
       <c r="F10" s="64"/>
-      <c r="G10" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H10" s="64" t="s">
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="94" t="s">
         <v>543</v>
       </c>
-      <c r="I10" s="64" t="s">
-        <v>192</v>
-      </c>
-      <c r="J10" s="64" t="s">
-        <v>545</v>
-      </c>
-      <c r="K10" s="95" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>517</v>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
+        <v>555</v>
       </c>
       <c r="B11" s="64" t="s">
-        <v>527</v>
+        <v>556</v>
       </c>
       <c r="C11" s="64" t="s">
         <v>30</v>
@@ -6948,68 +6943,71 @@
         <v>148</v>
       </c>
       <c r="H11" s="64" t="s">
+        <v>540</v>
+      </c>
+      <c r="I11" s="64" t="s">
+        <v>192</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>542</v>
+      </c>
+      <c r="K11" s="95" t="s">
         <v>543</v>
       </c>
-      <c r="I11" s="64" t="s">
-        <v>303</v>
-      </c>
-      <c r="J11" s="64" t="s">
-        <v>304</v>
-      </c>
-      <c r="K11" s="94" t="s">
-        <v>546</v>
-      </c>
-      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
-        <v>518</v>
-      </c>
-      <c r="B12" s="72" t="s">
-        <v>528</v>
-      </c>
+      <c r="A12" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B12" s="64"/>
       <c r="C12" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
       <c r="F12" s="64"/>
       <c r="G12" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
+      <c r="H12" s="64" t="s">
+        <v>540</v>
+      </c>
+      <c r="I12" s="64" t="s">
+        <v>303</v>
+      </c>
+      <c r="J12" s="64" t="s">
+        <v>304</v>
+      </c>
       <c r="K12" s="94"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>519</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>529</v>
+      <c r="A13" s="72" t="s">
+        <v>517</v>
+      </c>
+      <c r="B13" s="72" t="s">
+        <v>526</v>
       </c>
       <c r="C13" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H13" s="64"/>
       <c r="I13" s="64"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="96"/>
-      <c r="L13" s="14"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="94"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C14" s="64" t="s">
         <v>30</v>
@@ -7017,7 +7015,9 @@
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>148</v>
+      </c>
       <c r="H14" s="64"/>
       <c r="I14" s="64"/>
       <c r="J14" s="21"/>
@@ -7026,133 +7026,122 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>563</v>
+        <v>519</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>561</v>
+        <v>528</v>
       </c>
       <c r="C15" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>559</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>557</v>
+      </c>
+      <c r="C16" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D16" s="21">
         <v>20</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>562</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H15" s="64" t="s">
-        <v>543</v>
-      </c>
-      <c r="I15" s="64" t="s">
-        <v>544</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="K15" s="96"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
-        <v>521</v>
-      </c>
-      <c r="B16" s="64" t="s">
-        <v>531</v>
-      </c>
-      <c r="C16" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
+      <c r="E16" s="21" t="s">
+        <v>558</v>
+      </c>
+      <c r="F16" s="21"/>
       <c r="G16" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H16" s="64" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="I16" s="64" t="s">
-        <v>222</v>
-      </c>
-      <c r="J16" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="94" t="s">
-        <v>548</v>
-      </c>
+        <v>541</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="K16" s="96"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B17" s="64" t="s">
-        <v>532</v>
-      </c>
-      <c r="C17" s="69" t="s">
-        <v>204</v>
-      </c>
-      <c r="D17" s="64" t="s">
-        <v>177</v>
-      </c>
-      <c r="E17" s="64">
-        <v>175.57</v>
-      </c>
+        <v>529</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
       <c r="F17" s="64"/>
       <c r="G17" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H17" s="64" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="I17" s="64" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="J17" s="64" t="s">
-        <v>557</v>
-      </c>
-      <c r="K17" s="97"/>
-    </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="K17" s="94" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B18" s="64" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C18" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="64">
-        <v>40</v>
-      </c>
-      <c r="E18" s="64" t="s">
-        <v>554</v>
+        <v>204</v>
+      </c>
+      <c r="D18" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" s="64">
+        <v>175.57</v>
       </c>
       <c r="F18" s="64"/>
       <c r="G18" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H18" s="64" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="I18" s="64" t="s">
-        <v>306</v>
+        <v>208</v>
       </c>
       <c r="J18" s="64" t="s">
-        <v>304</v>
-      </c>
-      <c r="K18" s="94" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="97"/>
+    </row>
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
-        <v>524</v>
-      </c>
-      <c r="B19" s="64"/>
+        <v>522</v>
+      </c>
+      <c r="B19" s="64" t="s">
+        <v>531</v>
+      </c>
       <c r="C19" s="69" t="s">
         <v>31</v>
       </c>
@@ -7160,135 +7149,153 @@
         <v>40</v>
       </c>
       <c r="E19" s="64" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F19" s="64"/>
       <c r="G19" s="21" t="s">
         <v>148</v>
       </c>
       <c r="H19" s="64" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="I19" s="64" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J19" s="64" t="s">
         <v>304</v>
       </c>
-      <c r="K19" s="94"/>
-    </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K19" s="94" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>525</v>
-      </c>
-      <c r="B20" s="64" t="s">
-        <v>556</v>
-      </c>
+        <v>523</v>
+      </c>
+      <c r="B20" s="64"/>
       <c r="C20" s="69" t="s">
-        <v>228</v>
-      </c>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
+        <v>31</v>
+      </c>
+      <c r="D20" s="64">
+        <v>40</v>
+      </c>
+      <c r="E20" s="64" t="s">
+        <v>551</v>
+      </c>
       <c r="F20" s="64"/>
-      <c r="G20" s="64" t="s">
-        <v>537</v>
+      <c r="G20" s="21" t="s">
+        <v>148</v>
       </c>
       <c r="H20" s="64" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="I20" s="64" t="s">
-        <v>539</v>
+        <v>305</v>
       </c>
       <c r="J20" s="64" t="s">
-        <v>541</v>
-      </c>
-      <c r="K20" s="90" t="s">
+        <v>304</v>
+      </c>
+      <c r="K20" s="94"/>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="69" t="s">
+        <v>524</v>
+      </c>
+      <c r="B21" s="64" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="69" t="s">
-        <v>558</v>
-      </c>
-      <c r="B21" s="64" t="s">
-        <v>534</v>
-      </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="D21" s="64" t="s">
-        <v>535</v>
+      <c r="D21" s="79" t="s">
+        <v>563</v>
       </c>
       <c r="E21" s="64"/>
       <c r="F21" s="64"/>
       <c r="G21" s="64" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="H21" s="64" t="s">
+        <v>535</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>536</v>
+      </c>
+      <c r="J21" s="64" t="s">
         <v>538</v>
       </c>
-      <c r="I21" s="64" t="s">
-        <v>540</v>
-      </c>
-      <c r="J21" s="64" t="s">
-        <v>542</v>
-      </c>
-      <c r="K21" s="98"/>
+      <c r="K21" s="90" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
-        <v>526</v>
-      </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="69" t="s">
+        <v>554</v>
+      </c>
+      <c r="B22" s="64" t="s">
+        <v>532</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" s="79" t="s">
+        <v>563</v>
+      </c>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64" t="s">
+        <v>534</v>
+      </c>
+      <c r="H22" s="64" t="s">
+        <v>535</v>
+      </c>
+      <c r="I22" s="64" t="s">
+        <v>537</v>
+      </c>
+      <c r="J22" s="64" t="s">
+        <v>539</v>
+      </c>
+      <c r="K22" s="98"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="69" t="s">
+        <v>525</v>
+      </c>
+      <c r="B23" s="64"/>
+      <c r="C23" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="64">
+      <c r="D23" s="64">
         <v>1</v>
       </c>
-      <c r="E22" s="64" t="s">
+      <c r="E23" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="97" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="34"/>
-    </row>
-    <row r="24" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="63" t="s">
-        <v>550</v>
-      </c>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="74"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="97" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="34"/>
     </row>
     <row r="25" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="62" t="s">
-        <v>549</v>
+      <c r="A25" s="63" t="s">
+        <v>546</v>
       </c>
       <c r="B25" s="62"/>
       <c r="C25" s="62"/>
@@ -7299,25 +7306,27 @@
       <c r="H25" s="62"/>
       <c r="I25" s="62"/>
       <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="63" t="s">
-        <v>551</v>
-      </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
+      <c r="K25" s="74"/>
+    </row>
+    <row r="26" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="62" t="s">
+        <v>545</v>
+      </c>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="62"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="63" t="s">
+        <v>547</v>
+      </c>
       <c r="B27" s="38"/>
       <c r="C27" s="22"/>
       <c r="D27" s="36"/>
@@ -7444,13 +7453,13 @@
       <c r="H36" s="38"/>
       <c r="I36" s="36"/>
       <c r="J36" s="38"/>
-      <c r="K36" s="36"/>
+      <c r="K36" s="38"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="38"/>
       <c r="C37" s="22"/>
-      <c r="D37" s="38"/>
+      <c r="D37" s="36"/>
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
@@ -7463,14 +7472,14 @@
       <c r="A38" s="22"/>
       <c r="B38" s="38"/>
       <c r="C38" s="22"/>
-      <c r="D38" s="36"/>
+      <c r="D38" s="38"/>
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
       <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
+      <c r="I38" s="36"/>
       <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
+      <c r="K38" s="36"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -7509,7 +7518,7 @@
       <c r="H41" s="38"/>
       <c r="I41" s="38"/>
       <c r="J41" s="38"/>
-      <c r="K41" s="36"/>
+      <c r="K41" s="38"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
@@ -7519,23 +7528,23 @@
       <c r="E42" s="38"/>
       <c r="F42" s="38"/>
       <c r="G42" s="38"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
       <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
+      <c r="K42" s="36"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="41"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="42"/>
@@ -7655,40 +7664,40 @@
       <c r="K52" s="41"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="37"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="40"/>
+      <c r="A53" s="42"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="41"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="38"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="41"/>
       <c r="K53" s="41"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="38"/>
+      <c r="A54" s="37"/>
       <c r="B54" s="38"/>
       <c r="C54" s="37"/>
       <c r="D54" s="39"/>
-      <c r="E54" s="38"/>
+      <c r="E54" s="40"/>
       <c r="F54" s="38"/>
       <c r="G54" s="40"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="40"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="38"/>
       <c r="J54" s="38"/>
-      <c r="K54" s="38"/>
+      <c r="K54" s="41"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="37"/>
+      <c r="A55" s="38"/>
       <c r="B55" s="38"/>
       <c r="C55" s="37"/>
       <c r="D55" s="39"/>
       <c r="E55" s="38"/>
       <c r="F55" s="38"/>
       <c r="G55" s="40"/>
-      <c r="H55" s="41"/>
+      <c r="H55" s="38"/>
       <c r="I55" s="40"/>
       <c r="J55" s="38"/>
       <c r="K55" s="38"/>
@@ -7705,6 +7714,19 @@
       <c r="I56" s="40"/>
       <c r="J56" s="38"/>
       <c r="K56" s="38"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="40"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Database updated to the Bus Matrix.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -6786,8 +6786,8 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7204,10 +7204,10 @@
       <c r="B21" s="64" t="s">
         <v>552</v>
       </c>
-      <c r="C21" s="68" t="s">
+      <c r="C21" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="D21" s="79" t="s">
+      <c r="D21" s="38" t="s">
         <v>563</v>
       </c>
       <c r="E21" s="64"/>
@@ -7235,10 +7235,10 @@
       <c r="B22" s="64" t="s">
         <v>532</v>
       </c>
-      <c r="C22" s="68" t="s">
+      <c r="C22" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="D22" s="79" t="s">
+      <c r="D22" s="38" t="s">
         <v>563</v>
       </c>
       <c r="E22" s="64"/>

</xml_diff>

<commit_message>
add Invoice_Period_Start_Date_Key Invoice_Period_End_Date_Key to the Reconcile Invoice Fact table.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="568">
   <si>
     <t>Category</t>
   </si>
@@ -1914,6 +1914,18 @@
   </si>
   <si>
     <t>28,5</t>
+  </si>
+  <si>
+    <t>Invoice_Period_Start_Date_Key</t>
+  </si>
+  <si>
+    <t>Invoice_Period_End_Date_Key</t>
+  </si>
+  <si>
+    <t>Start date key of Invoice period</t>
+  </si>
+  <si>
+    <t>End date key of Invoice period</t>
   </si>
 </sst>
 </file>
@@ -6810,15 +6822,15 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" style="83" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="83" customWidth="1"/>
     <col min="2" max="2" width="39.140625" style="83" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="83" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="83" customWidth="1"/>
@@ -7196,189 +7208,201 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="68" t="s">
-        <v>523</v>
-      </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="63">
-        <v>40</v>
-      </c>
-      <c r="E20" s="63" t="s">
-        <v>551</v>
-      </c>
+        <v>564</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>566</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
       <c r="F20" s="63"/>
-      <c r="G20" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H20" s="63" t="s">
-        <v>540</v>
-      </c>
-      <c r="I20" s="63" t="s">
-        <v>305</v>
-      </c>
-      <c r="J20" s="63" t="s">
-        <v>304</v>
-      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
       <c r="K20" s="93"/>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="68" t="s">
-        <v>524</v>
+        <v>565</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>552</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>563</v>
-      </c>
+        <v>567</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="63"/>
       <c r="E21" s="63"/>
       <c r="F21" s="63"/>
-      <c r="G21" s="63" t="s">
-        <v>534</v>
-      </c>
-      <c r="H21" s="63" t="s">
-        <v>535</v>
-      </c>
-      <c r="I21" s="63" t="s">
-        <v>536</v>
-      </c>
-      <c r="J21" s="63" t="s">
-        <v>538</v>
-      </c>
-      <c r="K21" s="89" t="s">
-        <v>548</v>
-      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="93"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="68" t="s">
+        <v>523</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="63">
+        <v>40</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>551</v>
+      </c>
+      <c r="F22" s="63"/>
+      <c r="G22" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H22" s="63" t="s">
+        <v>540</v>
+      </c>
+      <c r="I22" s="63" t="s">
+        <v>305</v>
+      </c>
+      <c r="J22" s="63" t="s">
+        <v>304</v>
+      </c>
+      <c r="K22" s="93"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="68" t="s">
+        <v>524</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>552</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>563</v>
+      </c>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63" t="s">
+        <v>534</v>
+      </c>
+      <c r="H23" s="63" t="s">
+        <v>535</v>
+      </c>
+      <c r="I23" s="63" t="s">
+        <v>536</v>
+      </c>
+      <c r="J23" s="63" t="s">
+        <v>538</v>
+      </c>
+      <c r="K23" s="89" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="68" t="s">
         <v>554</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B24" s="63" t="s">
         <v>532</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C24" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D24" s="38" t="s">
         <v>563</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63" t="s">
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63" t="s">
         <v>534</v>
       </c>
-      <c r="H22" s="63" t="s">
+      <c r="H24" s="63" t="s">
         <v>535</v>
       </c>
-      <c r="I22" s="63" t="s">
+      <c r="I24" s="63" t="s">
         <v>537</v>
       </c>
-      <c r="J22" s="63" t="s">
+      <c r="J24" s="63" t="s">
         <v>539</v>
       </c>
-      <c r="K22" s="97"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="68" t="s">
+      <c r="K24" s="97"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="68" t="s">
         <v>525</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="68" t="s">
+      <c r="B25" s="63"/>
+      <c r="C25" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="63">
+      <c r="D25" s="63">
         <v>1</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="E25" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="96" t="s">
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="96" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="34"/>
-    </row>
-    <row r="25" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="62" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="34"/>
+    </row>
+    <row r="27" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="62" t="s">
         <v>546</v>
       </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="73"/>
-    </row>
-    <row r="26" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="73"/>
+    </row>
+    <row r="28" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="61" t="s">
         <v>545</v>
       </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="62" t="s">
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="62" t="s">
         <v>547</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
       <c r="B29" s="38"/>
       <c r="C29" s="22"/>
       <c r="D29" s="36"/>
@@ -7492,20 +7516,20 @@
       <c r="H37" s="38"/>
       <c r="I37" s="36"/>
       <c r="J37" s="38"/>
-      <c r="K37" s="36"/>
+      <c r="K37" s="38"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
       <c r="B38" s="38"/>
       <c r="C38" s="22"/>
-      <c r="D38" s="38"/>
+      <c r="D38" s="36"/>
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
       <c r="H38" s="38"/>
       <c r="I38" s="36"/>
       <c r="J38" s="38"/>
-      <c r="K38" s="36"/>
+      <c r="K38" s="38"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -7516,22 +7540,22 @@
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
+      <c r="I39" s="36"/>
       <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
+      <c r="K39" s="36"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="38"/>
       <c r="C40" s="22"/>
-      <c r="D40" s="36"/>
+      <c r="D40" s="38"/>
       <c r="E40" s="38"/>
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
       <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
+      <c r="I40" s="36"/>
       <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
+      <c r="K40" s="36"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
@@ -7557,7 +7581,7 @@
       <c r="H42" s="38"/>
       <c r="I42" s="38"/>
       <c r="J42" s="38"/>
-      <c r="K42" s="36"/>
+      <c r="K42" s="38"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
@@ -7567,36 +7591,36 @@
       <c r="E43" s="38"/>
       <c r="F43" s="38"/>
       <c r="G43" s="38"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
       <c r="J43" s="38"/>
       <c r="K43" s="38"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="41"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="36"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="41"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="42"/>
@@ -7703,56 +7727,82 @@
       <c r="K53" s="41"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="37"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="40"/>
+      <c r="A54" s="42"/>
+      <c r="B54" s="41"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="41"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="38"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="41"/>
       <c r="K54" s="41"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="38"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="38"/>
-      <c r="K55" s="38"/>
+      <c r="A55" s="42"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="41"/>
+      <c r="J55" s="41"/>
+      <c r="K55" s="41"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="37"/>
       <c r="B56" s="38"/>
       <c r="C56" s="37"/>
       <c r="D56" s="39"/>
-      <c r="E56" s="38"/>
+      <c r="E56" s="40"/>
       <c r="F56" s="38"/>
       <c r="G56" s="40"/>
       <c r="H56" s="41"/>
-      <c r="I56" s="40"/>
+      <c r="I56" s="38"/>
       <c r="J56" s="38"/>
-      <c r="K56" s="38"/>
+      <c r="K56" s="41"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="37"/>
+      <c r="A57" s="38"/>
       <c r="B57" s="38"/>
       <c r="C57" s="37"/>
       <c r="D57" s="39"/>
       <c r="E57" s="38"/>
       <c r="F57" s="38"/>
       <c r="G57" s="40"/>
-      <c r="H57" s="41"/>
+      <c r="H57" s="38"/>
       <c r="I57" s="40"/>
       <c r="J57" s="38"/>
       <c r="K57" s="38"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="37"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="38"/>
+      <c r="K58" s="38"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="41"/>
+      <c r="I59" s="40"/>
+      <c r="J59" s="38"/>
+      <c r="K59" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update expense_fact for fiance matrix bus
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565" firstSheet="15" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -23,24 +23,25 @@
     <sheet name="PO_fact" sheetId="24" r:id="rId14"/>
     <sheet name="invoice_fact" sheetId="25" r:id="rId15"/>
     <sheet name="SC_fact" sheetId="26" r:id="rId16"/>
-    <sheet name="expense_fact" sheetId="27" r:id="rId17"/>
-    <sheet name="wage_fact" sheetId="28" r:id="rId18"/>
-    <sheet name="forecasting_fact" sheetId="29" r:id="rId19"/>
-    <sheet name="payments_fact" sheetId="30" r:id="rId20"/>
-    <sheet name="GL_transaction_fact" sheetId="31" r:id="rId21"/>
-    <sheet name="budget_fact" sheetId="32" r:id="rId22"/>
-    <sheet name="Date_DIM" sheetId="7" r:id="rId23"/>
-    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId24"/>
-    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId25"/>
-    <sheet name="Program_DIM" sheetId="11" r:id="rId26"/>
-    <sheet name="cost_centre_DIM" sheetId="15" r:id="rId27"/>
-    <sheet name="Account_DIM" sheetId="13" r:id="rId28"/>
-    <sheet name="Employee_DIM" sheetId="5" r:id="rId29"/>
-    <sheet name="Ledger_DIM" sheetId="33" r:id="rId30"/>
-    <sheet name="accounting_period_dim" sheetId="34" r:id="rId31"/>
-    <sheet name="program_mapping" sheetId="35" r:id="rId32"/>
-    <sheet name="data for program_mapping" sheetId="36" r:id="rId33"/>
-    <sheet name="Fact 2 system mapping" sheetId="38" r:id="rId34"/>
+    <sheet name="extract.expsense" sheetId="42" r:id="rId17"/>
+    <sheet name="expense_fact" sheetId="27" r:id="rId18"/>
+    <sheet name="wage_fact" sheetId="28" r:id="rId19"/>
+    <sheet name="forecasting_fact" sheetId="29" r:id="rId20"/>
+    <sheet name="payments_fact" sheetId="30" r:id="rId21"/>
+    <sheet name="GL_transaction_fact" sheetId="31" r:id="rId22"/>
+    <sheet name="budget_fact" sheetId="32" r:id="rId23"/>
+    <sheet name="Date_DIM" sheetId="7" r:id="rId24"/>
+    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId25"/>
+    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId26"/>
+    <sheet name="Program_DIM" sheetId="11" r:id="rId27"/>
+    <sheet name="cost_centre_DIM" sheetId="15" r:id="rId28"/>
+    <sheet name="Account_DIM" sheetId="13" r:id="rId29"/>
+    <sheet name="Employee_DIM" sheetId="5" r:id="rId30"/>
+    <sheet name="Ledger_DIM" sheetId="33" r:id="rId31"/>
+    <sheet name="accounting_period_dim" sheetId="34" r:id="rId32"/>
+    <sheet name="program_mapping" sheetId="35" r:id="rId33"/>
+    <sheet name="data for program_mapping" sheetId="36" r:id="rId34"/>
+    <sheet name="Fact 2 system mapping" sheetId="38" r:id="rId35"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -132,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2284" uniqueCount="616">
   <si>
     <t>Category</t>
   </si>
@@ -1926,6 +1927,150 @@
   </si>
   <si>
     <t>End date key of Invoice period</t>
+  </si>
+  <si>
+    <t>expense_transaction</t>
+  </si>
+  <si>
+    <t>Records for all expensen transaction which are downloaded from Expensen Manager system</t>
+  </si>
+  <si>
+    <t>Org_ID</t>
+  </si>
+  <si>
+    <t>Transaction_no</t>
+  </si>
+  <si>
+    <t>Transaction_Date</t>
+  </si>
+  <si>
+    <t>Merchant_Name</t>
+  </si>
+  <si>
+    <t>Net_Amount</t>
+  </si>
+  <si>
+    <t>Tax_Amount</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>Activity code</t>
+  </si>
+  <si>
+    <t>Expense_Type</t>
+  </si>
+  <si>
+    <t>Line_desription</t>
+  </si>
+  <si>
+    <t>Costing</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Natural</t>
+  </si>
+  <si>
+    <t>supplier</t>
+  </si>
+  <si>
+    <t>Employee_No</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Employee_Email</t>
+  </si>
+  <si>
+    <t>10,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCESS HARDWARE PTY LTD   </t>
+  </si>
+  <si>
+    <t>TSMITH@ANGLICARESA.COM.AU</t>
+  </si>
+  <si>
+    <t>Visa0000000000117068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cut keys not working </t>
+  </si>
+  <si>
+    <t>MAINTENANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keys cutting </t>
+  </si>
+  <si>
+    <t>Card_Infomation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: </t>
+  </si>
+  <si>
+    <t>1. finance will download files monthly</t>
+  </si>
+  <si>
+    <t>Expense_key</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>txt file</t>
+  </si>
+  <si>
+    <t>Transaction_date_key</t>
+  </si>
+  <si>
+    <t>join with date_dim</t>
+  </si>
+  <si>
+    <t>Service_stream_key</t>
+  </si>
+  <si>
+    <t>HRIS</t>
+  </si>
+  <si>
+    <t>Employee_Key</t>
+  </si>
+  <si>
+    <t>join with employee_dim (some employee maybe have left anlicare)</t>
+  </si>
+  <si>
+    <t>employee_No</t>
+  </si>
+  <si>
+    <t>join with portfolio_dim</t>
+  </si>
+  <si>
+    <t>join with service_stream_dim</t>
+  </si>
+  <si>
+    <t>join with program_dim</t>
+  </si>
+  <si>
+    <t>manager_key</t>
+  </si>
+  <si>
+    <t>report to basing on employee_key</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>Staus</t>
+  </si>
+  <si>
+    <t>Uncoded /Waiting for approval</t>
+  </si>
+  <si>
+    <t>If costing information is NULL then Uncoded else Waiting for approval</t>
   </si>
 </sst>
 </file>
@@ -2368,7 +2513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2567,6 +2712,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2872,7 +3020,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6140,23 +6288,609 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>568</v>
+      </c>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>568</v>
+      </c>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>569</v>
+      </c>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="83"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="s">
+        <v>570</v>
+      </c>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="63">
+        <v>10</v>
+      </c>
+      <c r="E9" s="63">
+        <v>5746</v>
+      </c>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="63" t="s">
+        <v>571</v>
+      </c>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="63">
+        <v>10</v>
+      </c>
+      <c r="E10" s="63">
+        <v>2</v>
+      </c>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="96"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="63" t="s">
+        <v>572</v>
+      </c>
+      <c r="B11" s="63"/>
+      <c r="C11" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="63">
+        <v>10</v>
+      </c>
+      <c r="E11" s="63">
+        <v>20160127</v>
+      </c>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="96"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="63" t="s">
+        <v>573</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="19">
+        <v>50</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>588</v>
+      </c>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="63" t="s">
+        <v>586</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="19">
+        <v>50</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>589</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="63" t="s">
+        <v>584</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="63">
+        <v>10</v>
+      </c>
+      <c r="E14" s="63">
+        <v>3202</v>
+      </c>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="63" t="s">
+        <v>594</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="19">
+        <v>50</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>590</v>
+      </c>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="E16" s="63">
+        <v>48.4</v>
+      </c>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="63" t="s">
+        <v>574</v>
+      </c>
+      <c r="B17" s="63"/>
+      <c r="C17" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="E17" s="63">
+        <v>44</v>
+      </c>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
+        <v>575</v>
+      </c>
+      <c r="B18" s="63"/>
+      <c r="C18" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="E18" s="63">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="63" t="s">
+        <v>576</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="63">
+        <v>10</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>576</v>
+      </c>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="63"/>
+      <c r="C20" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="19">
+        <v>100</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>591</v>
+      </c>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="63" t="s">
+        <v>577</v>
+      </c>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="63">
+        <v>50</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>585</v>
+      </c>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="63" t="s">
+        <v>578</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="63">
+        <v>50</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>592</v>
+      </c>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="63" t="s">
+        <v>579</v>
+      </c>
+      <c r="B23" s="63"/>
+      <c r="C23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="19">
+        <v>100</v>
+      </c>
+      <c r="E23" s="63" t="s">
+        <v>593</v>
+      </c>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="63" t="s">
+        <v>390</v>
+      </c>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="63">
+        <v>10</v>
+      </c>
+      <c r="E24" s="63">
+        <v>10</v>
+      </c>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="63"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="63" t="s">
+        <v>580</v>
+      </c>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="63">
+        <v>10</v>
+      </c>
+      <c r="E25" s="63">
+        <v>6925</v>
+      </c>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="63"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="63" t="s">
+        <v>581</v>
+      </c>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="63">
+        <v>10</v>
+      </c>
+      <c r="E26" s="63">
+        <v>1000</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="63" t="s">
+        <v>582</v>
+      </c>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="63">
+        <v>10</v>
+      </c>
+      <c r="E27" s="63">
+        <v>61020</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="104" t="s">
+        <v>595</v>
+      </c>
+      <c r="B29" t="s">
+        <v>596</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" style="23" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="23"/>
+    <col min="4" max="4" width="8.140625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="23" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="23"/>
     <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="8" max="8" width="22" style="23" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="23" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="23" customWidth="1"/>
     <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="23"/>
   </cols>
@@ -6203,7 +6937,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -6242,347 +6976,632 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
+      <c r="A9" s="63" t="s">
+        <v>597</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>598</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
+      <c r="G9" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>568</v>
+      </c>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
+      <c r="A10" s="63" t="s">
+        <v>571</v>
+      </c>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="63">
+        <v>10</v>
+      </c>
+      <c r="E10" s="63">
+        <v>2</v>
+      </c>
       <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="G10" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>568</v>
+      </c>
+      <c r="I10" s="63" t="s">
+        <v>571</v>
+      </c>
+      <c r="J10" s="63" t="s">
+        <v>31</v>
+      </c>
       <c r="K10" s="45"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
+      <c r="A11" s="63" t="s">
+        <v>600</v>
+      </c>
+      <c r="B11" s="63"/>
+      <c r="C11" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
       <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="45"/>
+      <c r="G11" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>568</v>
+      </c>
+      <c r="I11" s="63" t="s">
+        <v>572</v>
+      </c>
+      <c r="J11" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="45" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="44"/>
+      <c r="A12" s="63" t="s">
+        <v>573</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="19">
+        <v>50</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>588</v>
+      </c>
       <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="G12" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>568</v>
+      </c>
+      <c r="I12" s="63" t="s">
+        <v>573</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="44"/>
+      <c r="A13" s="63" t="s">
+        <v>586</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="19">
+        <v>50</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>589</v>
+      </c>
       <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="G13" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>568</v>
+      </c>
+      <c r="I13" s="63" t="s">
+        <v>586</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="K13" s="38"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="44"/>
+      <c r="A14" s="63" t="s">
+        <v>604</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63">
+        <v>3202</v>
+      </c>
       <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="G14" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>568</v>
+      </c>
+      <c r="I14" s="63" t="s">
+        <v>606</v>
+      </c>
+      <c r="J14" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="38" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="63" t="s">
+        <v>517</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
       <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
+      <c r="G15" s="38" t="s">
+        <v>603</v>
+      </c>
       <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="38" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="63" t="s">
+        <v>602</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
       <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
+      <c r="G16" s="38" t="s">
+        <v>603</v>
+      </c>
       <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="38" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="63" t="s">
+        <v>519</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
       <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
+      <c r="G17" s="38" t="s">
+        <v>603</v>
+      </c>
       <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="23"/>
-    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="38" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
+        <v>610</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38" t="s">
+        <v>603</v>
+      </c>
+      <c r="H18" s="38"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="38" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="63" t="s">
+        <v>594</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="19">
+        <v>50</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>590</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H19" s="38"/>
+      <c r="I19" s="63" t="s">
+        <v>594</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="38"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="E20" s="63">
+        <v>48.4</v>
+      </c>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H20" s="38"/>
+      <c r="I20" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="K20" s="38"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="63" t="s">
+        <v>574</v>
+      </c>
+      <c r="B21" s="63"/>
+      <c r="C21" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="E21" s="63">
+        <v>44</v>
+      </c>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H21" s="38"/>
+      <c r="I21" s="63" t="s">
+        <v>574</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="K21" s="38"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="63" t="s">
+        <v>575</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="E22" s="63">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H22" s="38"/>
+      <c r="I22" s="63" t="s">
+        <v>575</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="K22" s="38"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="63" t="s">
+        <v>576</v>
+      </c>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="63">
         <v>10</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="E23" s="63" t="s">
+        <v>576</v>
+      </c>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H23" s="38"/>
+      <c r="I23" s="63" t="s">
+        <v>576</v>
+      </c>
+      <c r="J23" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" s="38"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="B24" s="63"/>
+      <c r="C24" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="19">
+        <v>100</v>
+      </c>
+      <c r="E24" s="63" t="s">
+        <v>591</v>
+      </c>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H24" s="38"/>
+      <c r="I24" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
+      <c r="J24" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K24" s="38"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="63" t="s">
+        <v>577</v>
+      </c>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="63">
+        <v>50</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>585</v>
+      </c>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H25" s="38"/>
+      <c r="I25" s="63" t="s">
+        <v>577</v>
+      </c>
+      <c r="J25" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="38"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="63" t="s">
+        <v>578</v>
+      </c>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="63">
+        <v>50</v>
+      </c>
+      <c r="E26" s="63" t="s">
+        <v>592</v>
+      </c>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H26" s="38"/>
+      <c r="I26" s="63" t="s">
+        <v>578</v>
+      </c>
+      <c r="J26" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="38"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="63" t="s">
+        <v>579</v>
+      </c>
+      <c r="B27" s="63"/>
+      <c r="C27" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="19">
+        <v>100</v>
+      </c>
+      <c r="E27" s="63" t="s">
+        <v>593</v>
+      </c>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H27" s="38"/>
+      <c r="I27" s="63" t="s">
+        <v>579</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K27" s="38"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="63" t="s">
+        <v>390</v>
+      </c>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="63">
+        <v>10</v>
+      </c>
+      <c r="E28" s="63">
+        <v>10</v>
+      </c>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H28" s="38"/>
+      <c r="I28" s="63" t="s">
+        <v>390</v>
+      </c>
+      <c r="J28" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K28" s="38"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="63" t="s">
+        <v>580</v>
+      </c>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="63">
+        <v>10</v>
+      </c>
+      <c r="E29" s="63">
+        <v>6925</v>
+      </c>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H29" s="38"/>
+      <c r="I29" s="63" t="s">
+        <v>580</v>
+      </c>
+      <c r="J29" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K29" s="38"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="63" t="s">
+        <v>581</v>
+      </c>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="63">
+        <v>10</v>
+      </c>
+      <c r="E30" s="63">
+        <v>1000</v>
+      </c>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H30" s="38"/>
+      <c r="I30" s="63" t="s">
+        <v>581</v>
+      </c>
+      <c r="J30" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K30" s="38"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="63" t="s">
+        <v>582</v>
+      </c>
+      <c r="B31" s="63"/>
+      <c r="C31" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="63">
+        <v>10</v>
+      </c>
+      <c r="E31" s="63">
+        <v>61020</v>
+      </c>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="H31" s="38"/>
+      <c r="I31" s="63" t="s">
+        <v>582</v>
+      </c>
+      <c r="J31" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K31" s="38"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="97" t="s">
+        <v>613</v>
+      </c>
+      <c r="B32" s="38"/>
+      <c r="C32" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="97">
         <v>20</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="45"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="E32" s="38" t="s">
+        <v>614</v>
+      </c>
+      <c r="F32" s="38"/>
+      <c r="G32" s="36" t="s">
+        <v>612</v>
+      </c>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38" t="s">
+        <v>615</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6618,7 +7637,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6634,7 +7653,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6642,7 +7661,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -6824,7 +7843,7 @@
   </sheetPr>
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -7838,7 +8857,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7854,7 +8873,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -7862,7 +8881,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -8064,7 +9083,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -8080,7 +9099,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -8088,7 +9107,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -8101,7 +9120,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -8290,7 +9309,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -8306,7 +9325,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -8314,7 +9333,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -8327,7 +9346,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -8489,6 +9508,232 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="45"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="45"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -8631,7 +9876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -8776,7 +10021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -8921,7 +10166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -9066,7 +10311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -9777,7 +11022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -10720,193 +11965,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -11530,6 +12588,193 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12016,7 +13261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -12525,7 +13770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -13012,7 +14257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -14416,7 +15661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -17272,7 +18517,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Expense ETL for finance added.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565"/>
+    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565" firstSheet="10" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -2080,7 +2080,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2172,8 +2172,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2208,6 +2215,11 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -2559,11 +2571,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2769,8 +2782,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3073,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6374,7 +6391,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6955,8 +6972,8 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7092,8 +7109,8 @@
       <c r="E10" s="61">
         <v>2</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38" t="s">
+      <c r="F10" s="61"/>
+      <c r="G10" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H10" s="38" t="s">
@@ -7112,13 +7129,13 @@
         <v>600</v>
       </c>
       <c r="B11" s="61"/>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="61"/>
       <c r="E11" s="61"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38" t="s">
+      <c r="F11" s="61"/>
+      <c r="G11" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H11" s="38" t="s">
@@ -7138,20 +7155,20 @@
       <c r="A12" s="61" t="s">
         <v>573</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="61" t="s">
         <v>583</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="61">
         <v>50</v>
       </c>
       <c r="E12" s="61" t="s">
         <v>588</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38" t="s">
+      <c r="F12" s="61"/>
+      <c r="G12" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H12" s="38" t="s">
@@ -7169,18 +7186,18 @@
       <c r="A13" s="61" t="s">
         <v>586</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="61"/>
+      <c r="C13" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="61">
         <v>50</v>
       </c>
       <c r="E13" s="61" t="s">
         <v>589</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38" t="s">
+      <c r="F13" s="61"/>
+      <c r="G13" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H13" s="38" t="s">
@@ -7198,7 +7215,7 @@
       <c r="A14" s="61" t="s">
         <v>604</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="61" t="s">
         <v>30</v>
       </c>
@@ -7206,8 +7223,8 @@
       <c r="E14" s="61">
         <v>3202</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38" t="s">
+      <c r="F14" s="61"/>
+      <c r="G14" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H14" s="38" t="s">
@@ -7227,14 +7244,14 @@
       <c r="A15" s="61" t="s">
         <v>517</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="61"/>
       <c r="E15" s="61"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38" t="s">
+      <c r="F15" s="61"/>
+      <c r="G15" s="61" t="s">
         <v>603</v>
       </c>
       <c r="H15" s="38"/>
@@ -7248,14 +7265,14 @@
       <c r="A16" s="61" t="s">
         <v>602</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="61"/>
       <c r="E16" s="61"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38" t="s">
+      <c r="F16" s="61"/>
+      <c r="G16" s="61" t="s">
         <v>603</v>
       </c>
       <c r="H16" s="38"/>
@@ -7269,14 +7286,14 @@
       <c r="A17" s="61" t="s">
         <v>519</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="61"/>
       <c r="E17" s="61"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38" t="s">
+      <c r="F17" s="61"/>
+      <c r="G17" s="61" t="s">
         <v>603</v>
       </c>
       <c r="H17" s="38"/>
@@ -7290,14 +7307,14 @@
       <c r="A18" s="61" t="s">
         <v>610</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="61"/>
       <c r="E18" s="61"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38" t="s">
+      <c r="F18" s="61"/>
+      <c r="G18" s="61" t="s">
         <v>603</v>
       </c>
       <c r="H18" s="38"/>
@@ -7311,18 +7328,18 @@
       <c r="A19" s="61" t="s">
         <v>594</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19" t="s">
+      <c r="B19" s="61"/>
+      <c r="C19" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="61">
         <v>50</v>
       </c>
       <c r="E19" s="61" t="s">
         <v>590</v>
       </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38" t="s">
+      <c r="F19" s="61"/>
+      <c r="G19" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H19" s="38"/>
@@ -7338,18 +7355,18 @@
       <c r="A20" s="61" t="s">
         <v>393</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="61"/>
+      <c r="C20" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="61" t="s">
         <v>587</v>
       </c>
       <c r="E20" s="61">
         <v>48.4</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38" t="s">
+      <c r="F20" s="61"/>
+      <c r="G20" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H20" s="38"/>
@@ -7366,17 +7383,17 @@
         <v>574</v>
       </c>
       <c r="B21" s="61"/>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="61" t="s">
         <v>587</v>
       </c>
       <c r="E21" s="61">
         <v>44</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38" t="s">
+      <c r="F21" s="61"/>
+      <c r="G21" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H21" s="38"/>
@@ -7393,17 +7410,17 @@
         <v>575</v>
       </c>
       <c r="B22" s="61"/>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="61" t="s">
         <v>587</v>
       </c>
       <c r="E22" s="61">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38" t="s">
+      <c r="F22" s="61"/>
+      <c r="G22" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H22" s="38"/>
@@ -7429,8 +7446,8 @@
       <c r="E23" s="61" t="s">
         <v>576</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38" t="s">
+      <c r="F23" s="61"/>
+      <c r="G23" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H23" s="38"/>
@@ -7447,17 +7464,17 @@
         <v>12</v>
       </c>
       <c r="B24" s="61"/>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="19">
-        <v>100</v>
+      <c r="D24" s="107">
+        <v>200</v>
       </c>
       <c r="E24" s="61" t="s">
         <v>591</v>
       </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38" t="s">
+      <c r="F24" s="61"/>
+      <c r="G24" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H24" s="38"/>
@@ -7483,8 +7500,8 @@
       <c r="E25" s="61" t="s">
         <v>585</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38" t="s">
+      <c r="F25" s="61"/>
+      <c r="G25" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H25" s="38"/>
@@ -7510,8 +7527,8 @@
       <c r="E26" s="61" t="s">
         <v>592</v>
       </c>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38" t="s">
+      <c r="F26" s="61"/>
+      <c r="G26" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H26" s="38"/>
@@ -7528,17 +7545,17 @@
         <v>579</v>
       </c>
       <c r="B27" s="61"/>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="61">
         <v>100</v>
       </c>
       <c r="E27" s="61" t="s">
         <v>593</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38" t="s">
+      <c r="F27" s="61"/>
+      <c r="G27" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H27" s="38"/>
@@ -7564,8 +7581,8 @@
       <c r="E28" s="61">
         <v>10</v>
       </c>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38" t="s">
+      <c r="F28" s="61"/>
+      <c r="G28" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H28" s="38"/>
@@ -7591,8 +7608,8 @@
       <c r="E29" s="61">
         <v>6925</v>
       </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38" t="s">
+      <c r="F29" s="61"/>
+      <c r="G29" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H29" s="38"/>
@@ -7618,8 +7635,8 @@
       <c r="E30" s="61">
         <v>1000</v>
       </c>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38" t="s">
+      <c r="F30" s="61"/>
+      <c r="G30" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H30" s="38"/>
@@ -7645,8 +7662,8 @@
       <c r="E31" s="61">
         <v>61020</v>
       </c>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38" t="s">
+      <c r="F31" s="61"/>
+      <c r="G31" s="61" t="s">
         <v>599</v>
       </c>
       <c r="H31" s="38"/>

</xml_diff>

<commit_message>
update finance_bus_matrxi for reconcile_invocie_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565" firstSheet="10" activeTab="17"/>
+    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="620">
   <si>
     <t>Category</t>
   </si>
@@ -1846,15 +1846,6 @@
     <t>join conform_finance.date_dim</t>
   </si>
   <si>
-    <t>1. some clients have different invocies for same period. basedon different servides (user_fld1) and comcare.task_type_code. How to process?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes and questions: </t>
-  </si>
-  <si>
-    <t>2.split invocie: Invoice_Period 05/06/2017 to 18/06/2017 to get start_day and end_day for that peirod    then match visit_date between start_day and end_day</t>
-  </si>
-  <si>
     <t>when do sum and group, need to map T1.invoice.user_fld1 and Comcare.actual_service.Task_type_code.</t>
   </si>
   <si>
@@ -2074,6 +2065,33 @@
   </si>
   <si>
     <t>expense_fact</t>
+  </si>
+  <si>
+    <t>cost_centre</t>
+  </si>
+  <si>
+    <t>Glcode</t>
+  </si>
+  <si>
+    <t>glcode</t>
+  </si>
+  <si>
+    <t>substring(glcode,2,4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  case costing
+   when '3225' then 'Children''s Accomodation Support'
+   when '3235' then 'Children''s Community Day Activities'
+   when '3609' then 'Children''s in home care'
+   when '3607' then  'OATS'
+   when '3608' then   'MT Gambier NDIS Case Co-ord'
+   when '3611' then   'Metro NDIS Case Co-ord'
+   else 'No Costing'</t>
+  </si>
+  <si>
+    <t>notes: 
+ Children's disability: 3225 / 3235 / 3609
+ Autism ELC: 3607 / 3608 / 3611</t>
   </si>
 </sst>
 </file>
@@ -4036,7 +4054,7 @@
         <v>57</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C22" s="49" t="s">
         <v>28</v>
@@ -6408,7 +6426,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C1" s="81"/>
       <c r="D1" s="81"/>
@@ -6442,7 +6460,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C3" s="81"/>
       <c r="D3" s="81"/>
@@ -6459,7 +6477,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C4" s="81"/>
       <c r="D4" s="81"/>
@@ -6553,7 +6571,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B9" s="61"/>
       <c r="C9" s="61" t="s">
@@ -6574,7 +6592,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="61" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B10" s="61"/>
       <c r="C10" s="61" t="s">
@@ -6595,7 +6613,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="61" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B11" s="61"/>
       <c r="C11" s="66" t="s">
@@ -6616,10 +6634,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>31</v>
@@ -6628,7 +6646,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F12" s="61"/>
       <c r="G12" s="61"/>
@@ -6639,7 +6657,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="61" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="19" t="s">
@@ -6649,7 +6667,7 @@
         <v>50</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F13" s="61"/>
       <c r="G13" s="61"/>
@@ -6660,7 +6678,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="61" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="61" t="s">
@@ -6681,7 +6699,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="61" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="19" t="s">
@@ -6691,7 +6709,7 @@
         <v>50</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F15" s="61"/>
       <c r="G15" s="61"/>
@@ -6709,7 +6727,7 @@
         <v>204</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E16" s="61">
         <v>48.4</v>
@@ -6723,14 +6741,14 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="61" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B17" s="61"/>
       <c r="C17" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E17" s="61">
         <v>44</v>
@@ -6744,14 +6762,14 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="61" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B18" s="61"/>
       <c r="C18" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E18" s="61">
         <v>4.4000000000000004</v>
@@ -6765,7 +6783,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="61" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B19" s="61"/>
       <c r="C19" s="61" t="s">
@@ -6775,7 +6793,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F19" s="61"/>
       <c r="G19" s="61"/>
@@ -6796,7 +6814,7 @@
         <v>100</v>
       </c>
       <c r="E20" s="61" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F20" s="61"/>
       <c r="G20" s="61"/>
@@ -6807,7 +6825,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="61" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B21" s="61"/>
       <c r="C21" s="61" t="s">
@@ -6817,7 +6835,7 @@
         <v>50</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F21" s="61"/>
       <c r="G21" s="61"/>
@@ -6828,7 +6846,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="61" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B22" s="61"/>
       <c r="C22" s="61" t="s">
@@ -6838,7 +6856,7 @@
         <v>50</v>
       </c>
       <c r="E22" s="61" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F22" s="61"/>
       <c r="G22" s="61"/>
@@ -6849,7 +6867,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="61" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B23" s="61"/>
       <c r="C23" s="19" t="s">
@@ -6859,7 +6877,7 @@
         <v>100</v>
       </c>
       <c r="E23" s="61" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
@@ -6891,7 +6909,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="61" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B25" s="61"/>
       <c r="C25" s="61" t="s">
@@ -6912,7 +6930,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="61" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B26" s="61"/>
       <c r="C26" s="61" t="s">
@@ -6933,7 +6951,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="61" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B27" s="61"/>
       <c r="C27" s="61" t="s">
@@ -6954,10 +6972,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="101" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B29" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -6972,7 +6990,7 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -7074,10 +7092,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C9" s="61" t="s">
         <v>30</v>
@@ -7086,10 +7104,10 @@
       <c r="E9" s="61"/>
       <c r="F9" s="38"/>
       <c r="G9" s="38" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
@@ -7097,7 +7115,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="61" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B10" s="61"/>
       <c r="C10" s="61" t="s">
@@ -7111,13 +7129,13 @@
       </c>
       <c r="F10" s="61"/>
       <c r="G10" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H10" s="38" t="s">
+        <v>565</v>
+      </c>
+      <c r="I10" s="61" t="s">
         <v>568</v>
-      </c>
-      <c r="I10" s="61" t="s">
-        <v>571</v>
       </c>
       <c r="J10" s="61" t="s">
         <v>31</v>
@@ -7126,7 +7144,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="61" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B11" s="61"/>
       <c r="C11" s="61" t="s">
@@ -7136,27 +7154,27 @@
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
       <c r="G11" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H11" s="38" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="I11" s="61" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="J11" s="66" t="s">
         <v>31</v>
       </c>
       <c r="K11" s="45" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C12" s="61" t="s">
         <v>31</v>
@@ -7165,17 +7183,17 @@
         <v>50</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F12" s="61"/>
       <c r="G12" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="I12" s="61" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>31</v>
@@ -7184,7 +7202,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="61" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B13" s="61"/>
       <c r="C13" s="61" t="s">
@@ -7194,17 +7212,17 @@
         <v>50</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F13" s="61"/>
       <c r="G13" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H13" s="38" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="I13" s="61" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>31</v>
@@ -7213,7 +7231,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="61" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B14" s="61"/>
       <c r="C14" s="61" t="s">
@@ -7225,19 +7243,19 @@
       </c>
       <c r="F14" s="61"/>
       <c r="G14" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="I14" s="61" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="J14" s="61" t="s">
         <v>31</v>
       </c>
       <c r="K14" s="38" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -7252,18 +7270,18 @@
       <c r="E15" s="61"/>
       <c r="F15" s="61"/>
       <c r="G15" s="61" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H15" s="38"/>
       <c r="I15" s="61"/>
       <c r="J15" s="61"/>
       <c r="K15" s="38" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="61" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B16" s="61"/>
       <c r="C16" s="61" t="s">
@@ -7273,13 +7291,13 @@
       <c r="E16" s="61"/>
       <c r="F16" s="61"/>
       <c r="G16" s="61" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H16" s="38"/>
       <c r="I16" s="61"/>
       <c r="J16" s="61"/>
       <c r="K16" s="38" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -7294,18 +7312,18 @@
       <c r="E17" s="61"/>
       <c r="F17" s="61"/>
       <c r="G17" s="61" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H17" s="38"/>
       <c r="I17" s="61"/>
       <c r="J17" s="61"/>
       <c r="K17" s="38" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="61" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B18" s="61"/>
       <c r="C18" s="61" t="s">
@@ -7315,18 +7333,18 @@
       <c r="E18" s="61"/>
       <c r="F18" s="61"/>
       <c r="G18" s="61" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H18" s="38"/>
       <c r="I18" s="61"/>
       <c r="J18" s="61"/>
       <c r="K18" s="38" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="61" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B19" s="61"/>
       <c r="C19" s="61" t="s">
@@ -7336,15 +7354,15 @@
         <v>50</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F19" s="61"/>
       <c r="G19" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H19" s="38"/>
       <c r="I19" s="61" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>31</v>
@@ -7360,14 +7378,14 @@
         <v>204</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E20" s="61">
         <v>48.4</v>
       </c>
       <c r="F20" s="61"/>
       <c r="G20" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H20" s="38"/>
       <c r="I20" s="61" t="s">
@@ -7380,25 +7398,25 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="61" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B21" s="61"/>
       <c r="C21" s="61" t="s">
         <v>204</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E21" s="61">
         <v>44</v>
       </c>
       <c r="F21" s="61"/>
       <c r="G21" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H21" s="38"/>
       <c r="I21" s="61" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>204</v>
@@ -7407,25 +7425,25 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="61" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B22" s="61"/>
       <c r="C22" s="61" t="s">
         <v>204</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E22" s="61">
         <v>4.4000000000000004</v>
       </c>
       <c r="F22" s="61"/>
       <c r="G22" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H22" s="38"/>
       <c r="I22" s="61" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="J22" s="19" t="s">
         <v>204</v>
@@ -7434,7 +7452,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="61" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B23" s="61"/>
       <c r="C23" s="61" t="s">
@@ -7444,15 +7462,15 @@
         <v>10</v>
       </c>
       <c r="E23" s="61" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F23" s="61"/>
       <c r="G23" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H23" s="38"/>
       <c r="I23" s="61" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="J23" s="61" t="s">
         <v>31</v>
@@ -7471,11 +7489,11 @@
         <v>200</v>
       </c>
       <c r="E24" s="61" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F24" s="61"/>
       <c r="G24" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H24" s="38"/>
       <c r="I24" s="61" t="s">
@@ -7488,7 +7506,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="61" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B25" s="61"/>
       <c r="C25" s="61" t="s">
@@ -7498,15 +7516,15 @@
         <v>50</v>
       </c>
       <c r="E25" s="61" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F25" s="61"/>
       <c r="G25" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H25" s="38"/>
       <c r="I25" s="61" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="J25" s="61" t="s">
         <v>31</v>
@@ -7515,7 +7533,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="61" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B26" s="61"/>
       <c r="C26" s="61" t="s">
@@ -7525,15 +7543,15 @@
         <v>50</v>
       </c>
       <c r="E26" s="61" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F26" s="61"/>
       <c r="G26" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H26" s="38"/>
       <c r="I26" s="61" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="J26" s="61" t="s">
         <v>31</v>
@@ -7542,7 +7560,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="61" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B27" s="61"/>
       <c r="C27" s="61" t="s">
@@ -7552,15 +7570,15 @@
         <v>100</v>
       </c>
       <c r="E27" s="61" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F27" s="61"/>
       <c r="G27" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H27" s="38"/>
       <c r="I27" s="61" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>31</v>
@@ -7583,7 +7601,7 @@
       </c>
       <c r="F28" s="61"/>
       <c r="G28" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H28" s="38"/>
       <c r="I28" s="61" t="s">
@@ -7596,7 +7614,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="61" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B29" s="61"/>
       <c r="C29" s="61" t="s">
@@ -7610,11 +7628,11 @@
       </c>
       <c r="F29" s="61"/>
       <c r="G29" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H29" s="38"/>
       <c r="I29" s="61" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="J29" s="61" t="s">
         <v>31</v>
@@ -7623,7 +7641,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="61" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B30" s="61"/>
       <c r="C30" s="61" t="s">
@@ -7637,11 +7655,11 @@
       </c>
       <c r="F30" s="61"/>
       <c r="G30" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H30" s="38"/>
       <c r="I30" s="61" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J30" s="61" t="s">
         <v>31</v>
@@ -7650,7 +7668,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="61" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B31" s="61"/>
       <c r="C31" s="61" t="s">
@@ -7664,11 +7682,11 @@
       </c>
       <c r="F31" s="61"/>
       <c r="G31" s="61" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H31" s="38"/>
       <c r="I31" s="61" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="J31" s="61" t="s">
         <v>31</v>
@@ -7677,7 +7695,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="94" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B32" s="38"/>
       <c r="C32" s="94" t="s">
@@ -7687,17 +7705,17 @@
         <v>20</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F32" s="38"/>
       <c r="G32" s="36" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="H32" s="38"/>
       <c r="I32" s="38"/>
       <c r="J32" s="38"/>
       <c r="K32" s="38" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -7938,10 +7956,10 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8061,10 +8079,10 @@
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="61" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C10" s="61" t="s">
         <v>30</v>
@@ -8082,10 +8100,10 @@
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="69" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B11" s="61" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C11" s="61" t="s">
         <v>30</v>
@@ -8111,7 +8129,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="61" t="s">
@@ -8200,10 +8218,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C16" s="61" t="s">
         <v>31</v>
@@ -8212,7 +8230,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21" t="s">
@@ -8285,7 +8303,7 @@
         <v>208</v>
       </c>
       <c r="J18" s="61" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="K18" s="93"/>
     </row>
@@ -8303,7 +8321,7 @@
         <v>40</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="F19" s="61"/>
       <c r="G19" s="21" t="s">
@@ -8319,15 +8337,15 @@
         <v>304</v>
       </c>
       <c r="K19" s="90" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="66" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C20" s="61" t="s">
         <v>30</v>
@@ -8343,10 +8361,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="66" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C21" s="61" t="s">
         <v>30</v>
@@ -8372,7 +8390,7 @@
         <v>40</v>
       </c>
       <c r="E22" s="61" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F22" s="61"/>
       <c r="G22" s="21" t="s">
@@ -8394,13 +8412,13 @@
         <v>524</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>204</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
@@ -8417,12 +8435,12 @@
         <v>538</v>
       </c>
       <c r="K23" s="87" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="66" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B24" s="61" t="s">
         <v>532</v>
@@ -8431,7 +8449,7 @@
         <v>204</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
@@ -8458,7 +8476,7 @@
         <v>31</v>
       </c>
       <c r="D25" s="61">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E25" s="61" t="s">
         <v>53</v>
@@ -8473,52 +8491,80 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="34"/>
-    </row>
-    <row r="27" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
-        <v>546</v>
-      </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="71"/>
-    </row>
-    <row r="28" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="s">
-        <v>545</v>
-      </c>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
+      <c r="A26" s="66" t="s">
+        <v>615</v>
+      </c>
+      <c r="B26" s="61"/>
+      <c r="C26" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="61">
+        <v>4</v>
+      </c>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>540</v>
+      </c>
+      <c r="I26" s="61" t="s">
+        <v>616</v>
+      </c>
+      <c r="J26" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="93"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="38">
+        <v>50</v>
+      </c>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H27" s="61" t="s">
+        <v>540</v>
+      </c>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="34" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>614</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" s="61" t="s">
+        <v>540</v>
+      </c>
+      <c r="I28" s="36"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="34" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
-        <v>547</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="38"/>
       <c r="C29" s="22"/>
       <c r="D29" s="36"/>
@@ -8530,7 +8576,7 @@
       <c r="J29" s="38"/>
       <c r="K29" s="38"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
       <c r="B30" s="38"/>
       <c r="C30" s="22"/>
@@ -8541,7 +8587,9 @@
       <c r="H30" s="38"/>
       <c r="I30" s="36"/>
       <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
+      <c r="K30" s="34" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
@@ -8606,20 +8654,20 @@
       <c r="H35" s="38"/>
       <c r="I35" s="36"/>
       <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
+      <c r="K35" s="36"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="38"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="36"/>
+      <c r="D36" s="38"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
       <c r="H36" s="38"/>
       <c r="I36" s="36"/>
       <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
+      <c r="K36" s="36"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
@@ -8630,7 +8678,7 @@
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="38"/>
-      <c r="I37" s="36"/>
+      <c r="I37" s="38"/>
       <c r="J37" s="38"/>
       <c r="K37" s="38"/>
     </row>
@@ -8643,7 +8691,7 @@
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
       <c r="H38" s="38"/>
-      <c r="I38" s="36"/>
+      <c r="I38" s="38"/>
       <c r="J38" s="38"/>
       <c r="K38" s="38"/>
     </row>
@@ -8656,20 +8704,20 @@
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="38"/>
-      <c r="I39" s="36"/>
+      <c r="I39" s="38"/>
       <c r="J39" s="38"/>
-      <c r="K39" s="36"/>
+      <c r="K39" s="38"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="38"/>
       <c r="C40" s="22"/>
-      <c r="D40" s="38"/>
+      <c r="D40" s="36"/>
       <c r="E40" s="38"/>
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
       <c r="H40" s="38"/>
-      <c r="I40" s="36"/>
+      <c r="I40" s="38"/>
       <c r="J40" s="38"/>
       <c r="K40" s="36"/>
     </row>
@@ -8681,62 +8729,62 @@
       <c r="E41" s="38"/>
       <c r="F41" s="38"/>
       <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="36"/>
       <c r="J41" s="38"/>
       <c r="K41" s="38"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
+      <c r="A42" s="42"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="41"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="41"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="38"/>
-      <c r="K44" s="36"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="38"/>
-      <c r="K45" s="38"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="41"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="42"/>
@@ -8817,108 +8865,56 @@
       <c r="K51" s="41"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="42"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="41"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="40"/>
       <c r="H52" s="41"/>
-      <c r="I52" s="41"/>
-      <c r="J52" s="41"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
       <c r="K52" s="41"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="42"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="41"/>
-      <c r="K53" s="41"/>
+      <c r="A53" s="38"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="40"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="42"/>
-      <c r="B54" s="41"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="40"/>
       <c r="H54" s="41"/>
-      <c r="I54" s="41"/>
-      <c r="J54" s="41"/>
-      <c r="K54" s="41"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="38"/>
+      <c r="K54" s="38"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="42"/>
-      <c r="B55" s="41"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="41"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="40"/>
       <c r="H55" s="41"/>
-      <c r="I55" s="41"/>
-      <c r="J55" s="41"/>
-      <c r="K55" s="41"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="37"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="38"/>
-      <c r="J56" s="38"/>
-      <c r="K56" s="41"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="38"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="38"/>
-      <c r="I57" s="40"/>
-      <c r="J57" s="38"/>
-      <c r="K57" s="38"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="37"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="41"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="37"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="41"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="38"/>
-      <c r="K59" s="38"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update etl for reconcile_invoice_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="624">
   <si>
     <t>Category</t>
   </si>
@@ -2092,6 +2092,18 @@
   </si>
   <si>
     <t>substring(glcode,3,4)</t>
+  </si>
+  <si>
+    <t>comcare service visit_date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Visit_Date</t>
+  </si>
+  <si>
+    <t>Comcare_visit_date</t>
   </si>
 </sst>
 </file>
@@ -7956,10 +7968,10 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8592,15 +8604,27 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="22"/>
+      <c r="A31" s="60" t="s">
+        <v>623</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>620</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>621</v>
+      </c>
       <c r="D31" s="36"/>
       <c r="E31" s="38"/>
       <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="36"/>
+      <c r="G31" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H31" s="61" t="s">
+        <v>535</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>622</v>
+      </c>
       <c r="J31" s="38"/>
       <c r="K31" s="38"/>
     </row>
@@ -8641,13 +8665,13 @@
       <c r="H34" s="38"/>
       <c r="I34" s="36"/>
       <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
+      <c r="K34" s="36"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="38"/>
       <c r="C35" s="22"/>
-      <c r="D35" s="36"/>
+      <c r="D35" s="38"/>
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
       <c r="G35" s="38"/>
@@ -8660,14 +8684,14 @@
       <c r="A36" s="22"/>
       <c r="B36" s="38"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="38"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
       <c r="H36" s="38"/>
-      <c r="I36" s="36"/>
+      <c r="I36" s="38"/>
       <c r="J36" s="38"/>
-      <c r="K36" s="36"/>
+      <c r="K36" s="38"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
@@ -8706,7 +8730,7 @@
       <c r="H39" s="38"/>
       <c r="I39" s="38"/>
       <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
+      <c r="K39" s="36"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
@@ -8716,23 +8740,23 @@
       <c r="E40" s="38"/>
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
       <c r="J40" s="38"/>
-      <c r="K40" s="36"/>
+      <c r="K40" s="38"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="41"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="42"/>
@@ -8852,40 +8876,40 @@
       <c r="K50" s="41"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="42"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="40"/>
       <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="41"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
       <c r="K51" s="41"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="37"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="38"/>
       <c r="C52" s="37"/>
       <c r="D52" s="39"/>
-      <c r="E52" s="40"/>
+      <c r="E52" s="38"/>
       <c r="F52" s="38"/>
       <c r="G52" s="40"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="40"/>
       <c r="J52" s="38"/>
-      <c r="K52" s="41"/>
+      <c r="K52" s="38"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="38"/>
+      <c r="A53" s="37"/>
       <c r="B53" s="38"/>
       <c r="C53" s="37"/>
       <c r="D53" s="39"/>
       <c r="E53" s="38"/>
       <c r="F53" s="38"/>
       <c r="G53" s="40"/>
-      <c r="H53" s="38"/>
+      <c r="H53" s="41"/>
       <c r="I53" s="40"/>
       <c r="J53" s="38"/>
       <c r="K53" s="38"/>
@@ -8902,19 +8926,6 @@
       <c r="I54" s="40"/>
       <c r="J54" s="38"/>
       <c r="K54" s="38"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="37"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="41"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="38"/>
-      <c r="K55" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update finance_bus_matrix and etl for reconcile_unbilledservice_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,44 +4,45 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="7410" windowWidth="24240" windowHeight="5565" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="reconcile_invoice_fact" sheetId="41" r:id="rId2"/>
-    <sheet name="debtor_fact" sheetId="22" r:id="rId3"/>
-    <sheet name="year_end_fact" sheetId="2" r:id="rId4"/>
-    <sheet name="salary_fact" sheetId="18" r:id="rId5"/>
-    <sheet name="actual_budget_fact" sheetId="19" r:id="rId6"/>
-    <sheet name="extract.GLF_Period_Balance_forK" sheetId="37" r:id="rId7"/>
-    <sheet name="KPI_fact" sheetId="17" r:id="rId8"/>
-    <sheet name="bad_debt_fact" sheetId="20" r:id="rId9"/>
-    <sheet name="Long_Service_Leave_fact" sheetId="23" r:id="rId10"/>
-    <sheet name="creditor_fact" sheetId="21" r:id="rId11"/>
-    <sheet name="Finance_Variable_Dim" sheetId="40" r:id="rId12"/>
-    <sheet name="extract.employee_workcover_rate" sheetId="39" r:id="rId13"/>
-    <sheet name="PO_fact" sheetId="24" r:id="rId14"/>
-    <sheet name="invoice_fact" sheetId="25" r:id="rId15"/>
-    <sheet name="SC_fact" sheetId="26" r:id="rId16"/>
-    <sheet name="extract.expsense" sheetId="42" r:id="rId17"/>
-    <sheet name="expense_fact" sheetId="27" r:id="rId18"/>
-    <sheet name="wage_fact" sheetId="28" r:id="rId19"/>
-    <sheet name="forecasting_fact" sheetId="29" r:id="rId20"/>
-    <sheet name="payments_fact" sheetId="30" r:id="rId21"/>
-    <sheet name="GL_transaction_fact" sheetId="31" r:id="rId22"/>
-    <sheet name="budget_fact" sheetId="32" r:id="rId23"/>
-    <sheet name="Date_DIM" sheetId="7" r:id="rId24"/>
-    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId25"/>
-    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId26"/>
-    <sheet name="Program_DIM" sheetId="11" r:id="rId27"/>
-    <sheet name="cost_centre_DIM" sheetId="15" r:id="rId28"/>
-    <sheet name="Account_DIM" sheetId="13" r:id="rId29"/>
-    <sheet name="Employee_DIM" sheetId="5" r:id="rId30"/>
-    <sheet name="Ledger_DIM" sheetId="33" r:id="rId31"/>
-    <sheet name="accounting_period_dim" sheetId="34" r:id="rId32"/>
-    <sheet name="program_mapping" sheetId="35" r:id="rId33"/>
-    <sheet name="data for program_mapping" sheetId="36" r:id="rId34"/>
-    <sheet name="Fact 2 system mapping" sheetId="38" r:id="rId35"/>
+    <sheet name="reconcile_unbilledservice_fact" sheetId="43" r:id="rId3"/>
+    <sheet name="debtor_fact" sheetId="22" r:id="rId4"/>
+    <sheet name="year_end_fact" sheetId="2" r:id="rId5"/>
+    <sheet name="salary_fact" sheetId="18" r:id="rId6"/>
+    <sheet name="actual_budget_fact" sheetId="19" r:id="rId7"/>
+    <sheet name="extract.GLF_Period_Balance_forK" sheetId="37" r:id="rId8"/>
+    <sheet name="KPI_fact" sheetId="17" r:id="rId9"/>
+    <sheet name="bad_debt_fact" sheetId="20" r:id="rId10"/>
+    <sheet name="Long_Service_Leave_fact" sheetId="23" r:id="rId11"/>
+    <sheet name="creditor_fact" sheetId="21" r:id="rId12"/>
+    <sheet name="Finance_Variable_Dim" sheetId="40" r:id="rId13"/>
+    <sheet name="extract.employee_workcover_rate" sheetId="39" r:id="rId14"/>
+    <sheet name="PO_fact" sheetId="24" r:id="rId15"/>
+    <sheet name="invoice_fact" sheetId="25" r:id="rId16"/>
+    <sheet name="SC_fact" sheetId="26" r:id="rId17"/>
+    <sheet name="extract.expsense" sheetId="42" r:id="rId18"/>
+    <sheet name="expense_fact" sheetId="27" r:id="rId19"/>
+    <sheet name="wage_fact" sheetId="28" r:id="rId20"/>
+    <sheet name="forecasting_fact" sheetId="29" r:id="rId21"/>
+    <sheet name="payments_fact" sheetId="30" r:id="rId22"/>
+    <sheet name="GL_transaction_fact" sheetId="31" r:id="rId23"/>
+    <sheet name="budget_fact" sheetId="32" r:id="rId24"/>
+    <sheet name="Date_DIM" sheetId="7" r:id="rId25"/>
+    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId26"/>
+    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId27"/>
+    <sheet name="Program_DIM" sheetId="11" r:id="rId28"/>
+    <sheet name="cost_centre_DIM" sheetId="15" r:id="rId29"/>
+    <sheet name="Account_DIM" sheetId="13" r:id="rId30"/>
+    <sheet name="Employee_DIM" sheetId="5" r:id="rId31"/>
+    <sheet name="Ledger_DIM" sheetId="33" r:id="rId32"/>
+    <sheet name="accounting_period_dim" sheetId="34" r:id="rId33"/>
+    <sheet name="program_mapping" sheetId="35" r:id="rId34"/>
+    <sheet name="data for program_mapping" sheetId="36" r:id="rId35"/>
+    <sheet name="Fact 2 system mapping" sheetId="38" r:id="rId36"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -133,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="676">
   <si>
     <t>Category</t>
   </si>
@@ -2094,16 +2095,173 @@
     <t>substring(glcode,3,4)</t>
   </si>
   <si>
-    <t>comcare service visit_date</t>
-  </si>
-  <si>
-    <t>date</t>
+    <t>reconcile_notbilledservice_fact</t>
+  </si>
+  <si>
+    <t>Used to store information regarding comcare provider has provided services but not billed client</t>
+  </si>
+  <si>
+    <t>notbilled_key</t>
+  </si>
+  <si>
+    <t>provider_id</t>
+  </si>
+  <si>
+    <t>provider_name</t>
+  </si>
+  <si>
+    <t>client_id</t>
+  </si>
+  <si>
+    <t>client_name</t>
+  </si>
+  <si>
+    <t>service_date_key</t>
+  </si>
+  <si>
+    <t>service_type_code</t>
+  </si>
+  <si>
+    <t>service_name</t>
+  </si>
+  <si>
+    <t>service_start_time</t>
+  </si>
+  <si>
+    <t>service_end_time</t>
+  </si>
+  <si>
+    <t>service_duration</t>
+  </si>
+  <si>
+    <t>travel_duration</t>
+  </si>
+  <si>
+    <t>schedule_duration</t>
+  </si>
+  <si>
+    <t>provider_contract_type</t>
+  </si>
+  <si>
+    <t>billing_funding_prog</t>
+  </si>
+  <si>
+    <t>billing_rate</t>
+  </si>
+  <si>
+    <t>billing_unit</t>
+  </si>
+  <si>
+    <t>billing_amount</t>
+  </si>
+  <si>
+    <t>billing_comments</t>
+  </si>
+  <si>
+    <t>unbilled_flag</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>6,2</t>
+  </si>
+  <si>
+    <t>10,5</t>
+  </si>
+  <si>
+    <t>employee name</t>
+  </si>
+  <si>
+    <t>payroll / autopay / contract</t>
+  </si>
+  <si>
+    <t>client name</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>billing funding program</t>
+  </si>
+  <si>
+    <t>billing hours</t>
+  </si>
+  <si>
+    <t>billing rate</t>
+  </si>
+  <si>
+    <t>If Yes, means  provider has provided services but not billed client</t>
+  </si>
+  <si>
+    <t>FK for Date_DIM</t>
+  </si>
+  <si>
+    <t>FB_Client_CB_Transaction</t>
+  </si>
+  <si>
+    <t>FC_Funder_Contract</t>
+  </si>
+  <si>
+    <t>Rate_Used</t>
   </si>
   <si>
     <t>Visit_Date</t>
   </si>
   <si>
-    <t>Comcare_visit_date</t>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>billing_period</t>
+  </si>
+  <si>
+    <t>Billing_Period_From / Billing_Period_To</t>
+  </si>
+  <si>
+    <t>activity_work_table</t>
+  </si>
+  <si>
+    <t>provider / person</t>
+  </si>
+  <si>
+    <t>provider_contract</t>
+  </si>
+  <si>
+    <t>provider_contract_type_code</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>activity_date</t>
+  </si>
+  <si>
+    <t>task_type_code</t>
+  </si>
+  <si>
+    <t>activity_start_time</t>
+  </si>
+  <si>
+    <t>activity_end_time</t>
+  </si>
+  <si>
+    <t>activity_duration</t>
+  </si>
+  <si>
+    <t>[schedule_duration]</t>
+  </si>
+  <si>
+    <t>organisation_id =7 for children disability providers</t>
+  </si>
+  <si>
+    <t>Funder_Contract_ID in (25,26,27,28,29,31)
+ and Funding_Care_Model_ID=6    for children disability</t>
+  </si>
+  <si>
+    <t>RECONCILE_UNBILLEDSERVICE_FACT</t>
+  </si>
+  <si>
+    <t>billing_visit_date</t>
   </si>
 </sst>
 </file>
@@ -2606,7 +2764,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2814,6 +2972,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4108,6 +4275,232 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="45"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="45"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -4881,7 +5274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -5105,7 +5498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -5431,7 +5824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -5735,7 +6128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -5788,232 +6181,6 @@
       </c>
       <c r="B4" s="23" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="45"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="23"/>
-    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -6215,7 +6382,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6231,7 +6398,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6239,7 +6406,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -6414,6 +6581,232 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="45"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="45"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -6995,7 +7388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -7736,242 +8129,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="23"/>
-    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="45"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8026,6 +8193,9 @@
       <c r="A5" s="26" t="s">
         <v>13</v>
       </c>
+      <c r="B5" s="81" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
@@ -8604,27 +8774,15 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
-        <v>623</v>
-      </c>
-      <c r="B31" s="38" t="s">
-        <v>620</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>621</v>
-      </c>
+      <c r="A31" s="22"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="36"/>
       <c r="E31" s="38"/>
       <c r="F31" s="38"/>
-      <c r="G31" s="61" t="s">
-        <v>534</v>
-      </c>
-      <c r="H31" s="61" t="s">
-        <v>535</v>
-      </c>
-      <c r="I31" s="36" t="s">
-        <v>622</v>
-      </c>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="36"/>
       <c r="J31" s="38"/>
       <c r="K31" s="38"/>
     </row>
@@ -8652,13 +8810,13 @@
       <c r="H33" s="38"/>
       <c r="I33" s="36"/>
       <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
+      <c r="K33" s="36"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="38"/>
       <c r="C34" s="22"/>
-      <c r="D34" s="36"/>
+      <c r="D34" s="38"/>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
       <c r="G34" s="38"/>
@@ -8671,14 +8829,14 @@
       <c r="A35" s="22"/>
       <c r="B35" s="38"/>
       <c r="C35" s="22"/>
-      <c r="D35" s="38"/>
+      <c r="D35" s="36"/>
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
       <c r="G35" s="38"/>
       <c r="H35" s="38"/>
-      <c r="I35" s="36"/>
+      <c r="I35" s="38"/>
       <c r="J35" s="38"/>
-      <c r="K35" s="36"/>
+      <c r="K35" s="38"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
@@ -8717,7 +8875,7 @@
       <c r="H38" s="38"/>
       <c r="I38" s="38"/>
       <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
+      <c r="K38" s="36"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -8727,23 +8885,23 @@
       <c r="E39" s="38"/>
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
       <c r="J39" s="38"/>
-      <c r="K39" s="36"/>
+      <c r="K39" s="38"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="41"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="42"/>
@@ -8863,40 +9021,40 @@
       <c r="K49" s="41"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="42"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="40"/>
       <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="41"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="38"/>
       <c r="K50" s="41"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="37"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="38"/>
       <c r="C51" s="37"/>
       <c r="D51" s="39"/>
-      <c r="E51" s="40"/>
+      <c r="E51" s="38"/>
       <c r="F51" s="38"/>
       <c r="G51" s="40"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="40"/>
       <c r="J51" s="38"/>
-      <c r="K51" s="41"/>
+      <c r="K51" s="38"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="38"/>
+      <c r="A52" s="37"/>
       <c r="B52" s="38"/>
       <c r="C52" s="37"/>
       <c r="D52" s="39"/>
       <c r="E52" s="38"/>
       <c r="F52" s="38"/>
       <c r="G52" s="40"/>
-      <c r="H52" s="38"/>
+      <c r="H52" s="41"/>
       <c r="I52" s="40"/>
       <c r="J52" s="38"/>
       <c r="K52" s="38"/>
@@ -8913,19 +9071,6 @@
       <c r="I53" s="40"/>
       <c r="J53" s="38"/>
       <c r="K53" s="38"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="37"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="38"/>
-      <c r="K54" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8961,7 +9106,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -8977,7 +9122,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -8985,7 +9130,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -9187,7 +9332,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -9203,7 +9348,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -9211,7 +9356,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -9413,7 +9558,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -9429,7 +9574,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -9437,7 +9582,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -9450,7 +9595,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -9639,7 +9784,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -9655,7 +9800,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -9663,7 +9808,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -9676,7 +9821,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -9838,6 +9983,232 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="45"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="45"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -9980,7 +10351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -10125,7 +10496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -10270,7 +10641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -10415,7 +10786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -11126,7 +11497,668 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" style="81" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" style="81" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="81" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="81" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="81" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="81" customWidth="1"/>
+    <col min="7" max="7" width="14" style="81" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="81" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="81" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="81" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="67.140625" style="81" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="81"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="81" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="81" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="81" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="69" t="s">
+        <v>622</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="90"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="61" t="s">
+        <v>623</v>
+      </c>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H10" s="61" t="s">
+        <v>661</v>
+      </c>
+      <c r="I10" s="61" t="s">
+        <v>623</v>
+      </c>
+      <c r="J10" s="61"/>
+      <c r="K10" s="90" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="109" t="s">
+        <v>624</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>645</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="108">
+        <v>50</v>
+      </c>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H11" s="110" t="s">
+        <v>662</v>
+      </c>
+      <c r="I11" s="108"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="109" t="s">
+        <v>635</v>
+      </c>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="108">
+        <v>10</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>646</v>
+      </c>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H12" s="108" t="s">
+        <v>663</v>
+      </c>
+      <c r="I12" s="108" t="s">
+        <v>664</v>
+      </c>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="61" t="s">
+        <v>625</v>
+      </c>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H13" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I13" s="61" t="s">
+        <v>625</v>
+      </c>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
+        <v>626</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>647</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="108">
+        <v>50</v>
+      </c>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H14" s="110" t="s">
+        <v>665</v>
+      </c>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="61" t="s">
+        <v>627</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>653</v>
+      </c>
+      <c r="C15" s="94" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I15" s="61" t="s">
+        <v>666</v>
+      </c>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="94" t="s">
+        <v>628</v>
+      </c>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="108">
+        <v>50</v>
+      </c>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H16" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I16" s="61" t="s">
+        <v>667</v>
+      </c>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="108">
+        <v>50</v>
+      </c>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H17" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="94" t="s">
+        <v>630</v>
+      </c>
+      <c r="B18" s="61"/>
+      <c r="C18" s="94" t="s">
+        <v>642</v>
+      </c>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H18" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I18" s="61" t="s">
+        <v>668</v>
+      </c>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="94" t="s">
+        <v>631</v>
+      </c>
+      <c r="B19" s="61"/>
+      <c r="C19" s="94" t="s">
+        <v>642</v>
+      </c>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H19" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I19" s="61" t="s">
+        <v>669</v>
+      </c>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="94" t="s">
+        <v>632</v>
+      </c>
+      <c r="B20" s="61" t="s">
+        <v>648</v>
+      </c>
+      <c r="C20" s="94" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="61" t="s">
+        <v>643</v>
+      </c>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H20" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I20" s="61" t="s">
+        <v>670</v>
+      </c>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="94" t="s">
+        <v>633</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>648</v>
+      </c>
+      <c r="C21" s="94" t="s">
+        <v>204</v>
+      </c>
+      <c r="D21" s="61" t="s">
+        <v>643</v>
+      </c>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H21" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I21" s="61" t="s">
+        <v>633</v>
+      </c>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="94" t="s">
+        <v>634</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>648</v>
+      </c>
+      <c r="C22" s="94" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" s="61" t="s">
+        <v>643</v>
+      </c>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H22" s="110" t="s">
+        <v>661</v>
+      </c>
+      <c r="I22" s="61" t="s">
+        <v>671</v>
+      </c>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="94" t="s">
+        <v>636</v>
+      </c>
+      <c r="B23" s="61" t="s">
+        <v>649</v>
+      </c>
+      <c r="C23" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="61">
+        <v>50</v>
+      </c>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H23" s="61" t="s">
+        <v>655</v>
+      </c>
+      <c r="I23" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="61"/>
+      <c r="K23" s="90" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="94" t="s">
+        <v>637</v>
+      </c>
+      <c r="B24" s="61" t="s">
+        <v>651</v>
+      </c>
+      <c r="C24" s="94" t="s">
+        <v>204</v>
+      </c>
+      <c r="D24" s="61" t="s">
+        <v>644</v>
+      </c>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H24" s="61" t="s">
+        <v>654</v>
+      </c>
+      <c r="I24" s="61" t="s">
+        <v>656</v>
+      </c>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="94" t="s">
+        <v>638</v>
+      </c>
+      <c r="B25" s="61" t="s">
+        <v>650</v>
+      </c>
+      <c r="C25" s="94" t="s">
+        <v>204</v>
+      </c>
+      <c r="D25" s="61" t="s">
+        <v>644</v>
+      </c>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H25" s="61" t="s">
+        <v>654</v>
+      </c>
+      <c r="I25" s="61" t="s">
+        <v>495</v>
+      </c>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="94" t="s">
+        <v>639</v>
+      </c>
+      <c r="B26" s="61"/>
+      <c r="C26" s="94" t="s">
+        <v>204</v>
+      </c>
+      <c r="D26" s="61" t="s">
+        <v>644</v>
+      </c>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>654</v>
+      </c>
+      <c r="I26" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="94" t="s">
+        <v>675</v>
+      </c>
+      <c r="B27" s="61"/>
+      <c r="C27" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="61">
+        <v>10</v>
+      </c>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61" t="s">
+        <v>654</v>
+      </c>
+      <c r="I27" s="61" t="s">
+        <v>657</v>
+      </c>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="94" t="s">
+        <v>640</v>
+      </c>
+      <c r="B28" s="61"/>
+      <c r="C28" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="61">
+        <v>500</v>
+      </c>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H28" s="61" t="s">
+        <v>654</v>
+      </c>
+      <c r="I28" s="61" t="s">
+        <v>658</v>
+      </c>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="94" t="s">
+        <v>659</v>
+      </c>
+      <c r="B29" s="61"/>
+      <c r="C29" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="61">
+        <v>50</v>
+      </c>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H29" s="61" t="s">
+        <v>654</v>
+      </c>
+      <c r="I29" s="61" t="s">
+        <v>660</v>
+      </c>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="94" t="s">
+        <v>641</v>
+      </c>
+      <c r="B30" s="61" t="s">
+        <v>652</v>
+      </c>
+      <c r="C30" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="61">
+        <v>2</v>
+      </c>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -12072,622 +13104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="23" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="10.28515625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.85546875" style="23" customWidth="1"/>
-    <col min="12" max="12" width="50.5703125" style="23" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="57" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-    </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="70" t="s">
-        <v>307</v>
-      </c>
-      <c r="L10" s="21"/>
-    </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="B11" s="61" t="s">
-        <v>207</v>
-      </c>
-      <c r="C11" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="72" t="s">
-        <v>329</v>
-      </c>
-      <c r="L11" s="21"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="C12" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="L14" s="21"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="69" t="s">
-        <v>216</v>
-      </c>
-      <c r="B15" s="69" t="s">
-        <v>217</v>
-      </c>
-      <c r="C15" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="L15" s="21"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
-        <v>219</v>
-      </c>
-      <c r="B16" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="61"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
-        <v>221</v>
-      </c>
-      <c r="B17" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="61"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="65" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="69" t="s">
-        <v>191</v>
-      </c>
-      <c r="B18" s="61" t="s">
-        <v>232</v>
-      </c>
-      <c r="C18" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="61"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="J20" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="21">
-        <v>40</v>
-      </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="21">
-        <v>40</v>
-      </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="K23" s="19"/>
-      <c r="L23" s="73"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>306</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="21">
-        <v>40</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="K24" s="19"/>
-      <c r="L24" s="73"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
-        <v>330</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="66">
-        <v>10</v>
-      </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I25" s="66" t="s">
-        <v>330</v>
-      </c>
-      <c r="J25" s="21">
-        <v>10</v>
-      </c>
-      <c r="K25" s="61"/>
-      <c r="L25" s="73"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="66" t="s">
-        <v>331</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="73" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="66" t="s">
-        <v>333</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="66" t="s">
-        <v>204</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I27" s="66" t="s">
-        <v>333</v>
-      </c>
-      <c r="J27" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="K27" s="38"/>
-      <c r="L27" s="73" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="66" t="s">
-        <v>334</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="66" t="s">
-        <v>204</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -12874,7 +13291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -13365,7 +13782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -13874,7 +14291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -14361,7 +14778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -15765,7 +16182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -16070,6 +16487,621 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="23" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="10.28515625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.85546875" style="23" customWidth="1"/>
+    <col min="12" max="12" width="50.5703125" style="23" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="57" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="69" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="61"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="61" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="61"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="K10" s="70" t="s">
+        <v>307</v>
+      </c>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="66" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="61"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="72" t="s">
+        <v>329</v>
+      </c>
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="69" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="61"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="L15" s="21"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="61"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="61" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="61"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="J17" s="21"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="65" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="61" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="61"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="61"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="21">
+        <v>40</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="21">
+        <v>40</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="K23" s="19"/>
+      <c r="L23" s="73"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="21">
+        <v>40</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="K24" s="19"/>
+      <c r="L24" s="73"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="66" t="s">
+        <v>330</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="66">
+        <v>10</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I25" s="66" t="s">
+        <v>330</v>
+      </c>
+      <c r="J25" s="21">
+        <v>10</v>
+      </c>
+      <c r="K25" s="61"/>
+      <c r="L25" s="73"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="66" t="s">
+        <v>331</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="73" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="66" t="s">
+        <v>333</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="66" t="s">
+        <v>204</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I27" s="66" t="s">
+        <v>333</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="K27" s="38"/>
+      <c r="L27" s="73" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="66" t="s">
+        <v>334</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="66" t="s">
+        <v>204</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -16798,7 +17830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -17524,7 +18556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -18250,7 +19282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -18613,7 +19645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -19188,230 +20220,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="15.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="23"/>
-    <col min="11" max="11" width="77.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="45"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added ETL for kypera_tenancy_balance_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7470" windowWidth="24240" windowHeight="5505" activeTab="4"/>
+    <workbookView xWindow="-90" yWindow="7530" windowWidth="24240" windowHeight="5445" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2585" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="760">
   <si>
     <t>Category</t>
   </si>
@@ -2356,9 +2356,6 @@
     <t>Kypera_Tenancy_Balance_Fact</t>
   </si>
   <si>
-    <t>Monthly snapshot for kypera tenancy balance</t>
-  </si>
-  <si>
     <t>balance_key</t>
   </si>
   <si>
@@ -2380,18 +2377,6 @@
     <t>scheme</t>
   </si>
   <si>
-    <t>credit</t>
-  </si>
-  <si>
-    <t>arrears</t>
-  </si>
-  <si>
-    <t>start_date_key</t>
-  </si>
-  <si>
-    <t>end_date_key</t>
-  </si>
-  <si>
     <t>indicates data belongs to which month</t>
   </si>
   <si>
@@ -2401,26 +2386,190 @@
     <t>program</t>
   </si>
   <si>
-    <t>data_day_key</t>
-  </si>
-  <si>
     <t>every first of month morning, take snapshot for last month's balance</t>
   </si>
   <si>
-    <t>ASA owns money to tenancy</t>
-  </si>
-  <si>
-    <t>tenancy owns money to ASA</t>
-  </si>
-  <si>
-    <t>balance</t>
+    <t>Monthly snapshot for kypera tenancy balance including currrent/former tenancy</t>
+  </si>
+  <si>
+    <t>Mr C Herft</t>
+  </si>
+  <si>
+    <t>28 Sampson Road</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Chris Maudsley</t>
+  </si>
+  <si>
+    <t>RentBalance</t>
+  </si>
+  <si>
+    <t>OtherChargesBalance</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>BK_day_key</t>
+  </si>
+  <si>
+    <t>Entity: LAW  / Scheme: Laura and Alfred West Community Housing
+Entity: ASA / Scheme:  not in ('Regional Housing')</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>propertyID</t>
+  </si>
+  <si>
+    <t>Effective_Days</t>
+  </si>
+  <si>
+    <t>Occupancies_Occupancy</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>1: current / 0: former</t>
+  </si>
+  <si>
+    <t>Salutation</t>
+  </si>
+  <si>
+    <t>Address1Line</t>
+  </si>
+  <si>
+    <t>PropertyStructure_Unit</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Startdate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <r>
+      <t>For arrears current arrears - we need to filter on property tree for ASAH and LAWCH only (not including AC Care as they are not on board yet), then use the advance filter for effective days greater than or equal to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>days (for arrears) and less than or equal to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">days for credit.
+For former – same property tree filter, but advance filter on greater than 0 for arrears and less than zero for credit.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Security_User</t>
+  </si>
+  <si>
+    <t>[User]</t>
+  </si>
+  <si>
+    <t>//Property Unit Level
+INNER JOIN anglicare.dbo.PropertyStructure_Unit AS f
+  ON a.Unit = f.ID
+//For Housing Officer
+LEFT JOIN anglicare.dbo.Security_User AS su ON su.[User] = f.HousingOfficer</t>
+  </si>
+  <si>
+    <t>PropertyStructure_District</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>PropertyStructure_scheme</t>
+  </si>
+  <si>
+    <t>ActualRentBalance</t>
+  </si>
+  <si>
+    <t>ActualNonRentBalance</t>
+  </si>
+  <si>
+    <t>ActualTotalBalance</t>
+  </si>
+  <si>
+    <t>Occupancies_RentCalculation_Arrears_EffectiveBalances</t>
+  </si>
+  <si>
+    <t>this table need to backup monthly</t>
+  </si>
+  <si>
+    <t>EffectiveRentDaysInArrears</t>
+  </si>
+  <si>
+    <t>CreditORArrears</t>
+  </si>
+  <si>
+    <t>Credit / Arrears</t>
+  </si>
+  <si>
+    <t>basing on Effective_Days and use above rules.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> convert(varchar,a.StartDate,103)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> convert(varchar,a.EndDate,103)</t>
+  </si>
+  <si>
+    <t>dwhb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2519,8 +2668,106 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2562,8 +2809,176 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -2910,13 +3325,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="35" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3151,11 +3724,57 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="8" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="5" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="6" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="7" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -17987,24 +18606,24 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" style="81" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="81" customWidth="1"/>
+    <col min="2" max="2" width="24" style="81" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="81"/>
-    <col min="5" max="5" width="10.28515625" style="81" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="81" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="81"/>
     <col min="7" max="7" width="14" style="81" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="81" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="81" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" style="81" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" style="81" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.85546875" style="81" customWidth="1"/>
+    <col min="11" max="11" width="68.7109375" style="81" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="81"/>
   </cols>
   <sheetData>
@@ -18037,13 +18656,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>706</v>
+        <v>717</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>13</v>
       </c>
+      <c r="B5" s="81" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
@@ -18090,7 +18712,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B9" s="61" t="s">
         <v>29</v>
@@ -18109,27 +18731,35 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="61" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B10" s="61"/>
       <c r="C10" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="61"/>
-      <c r="E10" s="21"/>
+      <c r="E10" s="118">
+        <v>10808</v>
+      </c>
       <c r="F10" s="21"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
+      <c r="G10" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H10" s="84" t="s">
+        <v>731</v>
+      </c>
+      <c r="I10" s="84" t="s">
+        <v>732</v>
+      </c>
       <c r="J10" s="84"/>
       <c r="K10" s="112"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="61" t="s">
+        <v>709</v>
+      </c>
+      <c r="B11" s="61" t="s">
         <v>710</v>
-      </c>
-      <c r="B11" s="61" t="s">
-        <v>711</v>
       </c>
       <c r="C11" s="61" t="s">
         <v>31</v>
@@ -18137,13 +18767,21 @@
       <c r="D11" s="61">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="118" t="s">
+        <v>720</v>
+      </c>
       <c r="F11" s="21"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
+      <c r="G11" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H11" s="84" t="s">
+        <v>731</v>
+      </c>
       <c r="I11" s="84"/>
       <c r="J11" s="84"/>
-      <c r="K11" s="112"/>
+      <c r="K11" s="112" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
@@ -18156,17 +18794,25 @@
       <c r="D12" s="61">
         <v>50</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="21" t="s">
+        <v>718</v>
+      </c>
       <c r="F12" s="21"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
+      <c r="G12" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H12" s="84" t="s">
+        <v>731</v>
+      </c>
+      <c r="I12" s="84" t="s">
+        <v>734</v>
+      </c>
       <c r="J12" s="84"/>
       <c r="K12" s="113"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="66" t="s">
@@ -18175,77 +18821,107 @@
       <c r="D13" s="61">
         <v>100</v>
       </c>
-      <c r="E13" s="68"/>
+      <c r="E13" s="21" t="s">
+        <v>719</v>
+      </c>
       <c r="F13" s="21"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="84"/>
+      <c r="G13" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H13" s="84" t="s">
+        <v>736</v>
+      </c>
+      <c r="I13" s="84" t="s">
+        <v>735</v>
+      </c>
       <c r="J13" s="84"/>
       <c r="K13" s="84"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>716</v>
-      </c>
-      <c r="C14" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="68"/>
+        <v>729</v>
+      </c>
+      <c r="B14" s="119"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
+      <c r="G14" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H14" s="84" t="s">
+        <v>731</v>
+      </c>
       <c r="I14" s="84"/>
       <c r="J14" s="84"/>
-      <c r="K14" s="69" t="s">
-        <v>653</v>
+      <c r="K14" s="84" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>717</v>
-      </c>
-      <c r="B15" s="69"/>
+        <v>727</v>
+      </c>
       <c r="C15" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="68"/>
+        <v>31</v>
+      </c>
+      <c r="D15" s="19">
+        <v>10</v>
+      </c>
+      <c r="E15" s="68">
+        <v>42301</v>
+      </c>
       <c r="F15" s="21"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
+      <c r="G15" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H15" s="84" t="s">
+        <v>731</v>
+      </c>
+      <c r="I15" s="84" t="s">
+        <v>738</v>
+      </c>
+      <c r="J15" s="84" t="s">
+        <v>32</v>
+      </c>
       <c r="K15" s="69" t="s">
-        <v>653</v>
+        <v>757</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
-        <v>712</v>
+      <c r="A16" s="19" t="s">
+        <v>728</v>
       </c>
       <c r="B16" s="69"/>
       <c r="C16" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="61">
-        <v>50</v>
-      </c>
-      <c r="E16" s="21"/>
+      <c r="D16" s="19">
+        <v>10</v>
+      </c>
+      <c r="E16" s="68"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G16" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H16" s="84" t="s">
+        <v>731</v>
+      </c>
+      <c r="I16" s="84" t="s">
+        <v>739</v>
+      </c>
+      <c r="J16" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="69" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
-        <v>713</v>
-      </c>
-      <c r="B17" s="69" t="s">
-        <v>720</v>
-      </c>
+        <v>711</v>
+      </c>
+      <c r="B17" s="69"/>
       <c r="C17" s="66" t="s">
         <v>31</v>
       </c>
@@ -18253,211 +18929,341 @@
         <v>50</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="84"/>
+      <c r="G17" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H17" s="84" t="s">
+        <v>741</v>
+      </c>
+      <c r="I17" s="84" t="s">
+        <v>742</v>
+      </c>
       <c r="J17" s="84"/>
-      <c r="K17" s="84"/>
+      <c r="K17" s="112" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
-        <v>714</v>
-      </c>
-      <c r="B18" s="69" t="s">
-        <v>723</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>205</v>
-      </c>
+      <c r="A18" s="69" t="s">
+        <v>193</v>
+      </c>
+      <c r="B18" s="69"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="84"/>
+      <c r="G18" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H18" s="84" t="s">
+        <v>744</v>
+      </c>
+      <c r="I18" s="84" t="s">
+        <v>745</v>
+      </c>
       <c r="J18" s="84"/>
       <c r="K18" s="84"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
+        <v>712</v>
+      </c>
+      <c r="B19" s="69" t="s">
         <v>715</v>
       </c>
-      <c r="B19" s="61" t="s">
-        <v>724</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="E19" s="21"/>
+      <c r="C19" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="61">
+        <v>50</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>714</v>
+      </c>
       <c r="F19" s="21"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
+      <c r="G19" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H19" s="84" t="s">
+        <v>747</v>
+      </c>
+      <c r="I19" s="84" t="s">
+        <v>746</v>
+      </c>
       <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
+      <c r="K19" s="112" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="69" t="s">
-        <v>725</v>
-      </c>
-      <c r="B20" s="61"/>
+      <c r="A20" s="61" t="s">
+        <v>722</v>
+      </c>
+      <c r="B20" s="69"/>
       <c r="C20" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="E20" s="21"/>
+      <c r="E20" s="21">
+        <v>202.48</v>
+      </c>
       <c r="F20" s="21"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="84"/>
+      <c r="G20" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H20" s="84" t="s">
+        <v>751</v>
+      </c>
+      <c r="I20" s="84" t="s">
+        <v>748</v>
+      </c>
       <c r="J20" s="84"/>
-      <c r="K20" s="84"/>
+      <c r="K20" s="65" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="61" t="s">
-        <v>721</v>
-      </c>
-      <c r="B21" s="61" t="s">
-        <v>718</v>
-      </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="69" t="s">
+        <v>723</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="E21" s="21">
+        <v>0</v>
+      </c>
       <c r="F21" s="21"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
+      <c r="G21" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H21" s="84" t="s">
+        <v>751</v>
+      </c>
+      <c r="I21" s="84" t="s">
+        <v>749</v>
+      </c>
       <c r="J21" s="84"/>
-      <c r="K21" s="84" t="s">
-        <v>722</v>
-      </c>
+      <c r="K21" s="84"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="21"/>
+      <c r="A22" s="69" t="s">
+        <v>724</v>
+      </c>
+      <c r="B22" s="61"/>
+      <c r="C22" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="E22" s="21">
+        <v>202.48</v>
+      </c>
       <c r="F22" s="21"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
+      <c r="G22" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H22" s="84" t="s">
+        <v>751</v>
+      </c>
+      <c r="I22" s="84" t="s">
+        <v>750</v>
+      </c>
       <c r="J22" s="84"/>
       <c r="K22" s="84"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+    <row r="23" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="69" t="s">
+        <v>730</v>
+      </c>
+      <c r="B23" s="61"/>
+      <c r="C23" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="19"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
+      <c r="G23" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="H23" s="84" t="s">
+        <v>751</v>
+      </c>
+      <c r="I23" s="84" t="s">
+        <v>753</v>
+      </c>
       <c r="J23" s="84"/>
-      <c r="K23" s="114"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+      <c r="K23" s="112" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="69" t="s">
+        <v>754</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>755</v>
+      </c>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
       <c r="G24" s="84"/>
       <c r="H24" s="84"/>
       <c r="I24" s="84"/>
       <c r="J24" s="84"/>
-      <c r="K24" s="114"/>
+      <c r="K24" s="112" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="A25" s="61" t="s">
+        <v>725</v>
+      </c>
+      <c r="B25" s="61" t="s">
+        <v>713</v>
+      </c>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="68">
+        <v>43008</v>
+      </c>
       <c r="F25" s="21"/>
       <c r="G25" s="84"/>
       <c r="H25" s="84"/>
       <c r="I25" s="84"/>
       <c r="J25" s="84"/>
-      <c r="K25" s="114"/>
+      <c r="K25" s="84" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="84"/>
       <c r="H26" s="84"/>
       <c r="I26" s="84"/>
       <c r="J26" s="84"/>
-      <c r="K26" s="114"/>
+      <c r="K26" s="84"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
-      <c r="D27" s="66"/>
+      <c r="D27" s="21"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="84"/>
       <c r="H27" s="84"/>
       <c r="I27" s="84"/>
       <c r="J27" s="84"/>
-      <c r="K27" s="115"/>
+      <c r="K27" s="114"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="116"/>
-      <c r="H28" s="116"/>
-      <c r="I28" s="116"/>
-      <c r="J28" s="116"/>
-      <c r="K28" s="117"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="114"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
       <c r="G29" s="84"/>
       <c r="H29" s="84"/>
       <c r="I29" s="84"/>
       <c r="J29" s="84"/>
-      <c r="K29" s="117"/>
+      <c r="K29" s="114"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="117"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="84"/>
+      <c r="K30" s="114"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="66"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="84"/>
+      <c r="I31" s="84"/>
+      <c r="J31" s="84"/>
+      <c r="K31" s="115"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="66"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="116"/>
+      <c r="I32" s="116"/>
+      <c r="J32" s="116"/>
+      <c r="K32" s="117"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="66"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="84"/>
+      <c r="K33" s="117"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="66"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="116"/>
+      <c r="J34" s="116"/>
+      <c r="K34" s="117"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update finance matrix bus for RECONCILE_UNBILLEDSERVICE_FACT
</commit_message>
<xml_diff>
--- a/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
+++ b/Matrix_Bus/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7530" windowWidth="24240" windowHeight="5445" activeTab="4"/>
+    <workbookView xWindow="-90" yWindow="7530" windowWidth="24240" windowHeight="5445" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="762">
   <si>
     <t>Category</t>
   </si>
@@ -2563,6 +2563,12 @@
   </si>
   <si>
     <t>dwhb</t>
+  </si>
+  <si>
+    <t>est_visit_charge</t>
+  </si>
+  <si>
+    <t>numeric</t>
   </si>
 </sst>
 </file>
@@ -12374,10 +12380,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13024,6 +13030,31 @@
       <c r="I30" s="61"/>
       <c r="J30" s="61"/>
       <c r="K30" s="61"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="38" t="s">
+        <v>760</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38" t="s">
+        <v>761</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>584</v>
+      </c>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="61" t="s">
+        <v>534</v>
+      </c>
+      <c r="H31" s="61" t="s">
+        <v>661</v>
+      </c>
+      <c r="I31" s="38" t="s">
+        <v>760</v>
+      </c>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18608,7 +18639,7 @@
   </sheetPr>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>